<commit_message>
KL final calculations and visual package being developed
</commit_message>
<xml_diff>
--- a/src/results/kl_content_vs_domain.xlsx
+++ b/src/results/kl_content_vs_domain.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6006562394409126</v>
+        <v>0.9251511857443364</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.5140648490122401</v>
+        <v>0.7620693316763634</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.477452083984183</v>
+        <v>0.7842021244848932</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.6184173132138232</v>
+        <v>0.9805763031769701</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5752841456888848</v>
+        <v>0.9228475915176979</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4921853728232786</v>
+        <v>0.7936678103050605</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -633,7 +633,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6561552049546702</v>
+        <v>1.021656157081017</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.7758346995788798</v>
+        <v>1.202232665100662</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.730249848402359</v>
+        <v>1.195083493543541</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5507626904539298</v>
+        <v>0.9048165736872354</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.5097738401156459</v>
+        <v>0.879107954112294</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -763,7 +763,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.5150868719357055</v>
+        <v>1.003431014672907</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -789,7 +789,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.7659960643140019</v>
+        <v>1.10254227034616</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.6023854028278619</v>
+        <v>0.9454770549090322</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -841,7 +841,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.8004096180779974</v>
+        <v>1.655622795138359</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -867,7 +867,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.7540390046171732</v>
+        <v>1.309345107064612</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -893,7 +893,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.6666773043684373</v>
+        <v>1.051825159337061</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -919,7 +919,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.6394202446583863</v>
+        <v>1.078862827749338</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.5100126993679333</v>
+        <v>0.81612081962609</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.4749251603978977</v>
+        <v>0.7725947570821188</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.7614346865363162</v>
+        <v>1.32078453497408</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1023,7 +1023,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.6737031090198544</v>
+        <v>1.061984453095498</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.4679390418083255</v>
+        <v>0.7658686418432765</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.594513629007586</v>
+        <v>1.158926839087477</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.5601797556342527</v>
+        <v>0.8923965870319139</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.5147494042551717</v>
+        <v>0.8828807322248121</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.4868816874787782</v>
+        <v>0.7961545396071323</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1179,7 +1179,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.4943455194547152</v>
+        <v>0.7940398241272142</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1205,7 +1205,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.5750587353501438</v>
+        <v>0.9763419090948953</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.6125203047482622</v>
+        <v>1.088159863689639</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.5040249341049442</v>
+        <v>0.8093659912769549</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1283,7 +1283,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.5055023842669155</v>
+        <v>0.8097386869533613</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1309,7 +1309,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.5172126319318253</v>
+        <v>0.8002194508143495</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1335,7 +1335,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.5279306480604539</v>
+        <v>0.8045413470862837</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.5191906165139111</v>
+        <v>0.8839604572400914</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.2709963365231917</v>
+        <v>0.5163440213014413</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1413,7 +1413,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.6045025645922981</v>
+        <v>0.958535990820544</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1439,7 +1439,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.4648523827376018</v>
+        <v>1.162657416639946</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.4736446987681839</v>
+        <v>0.780416014936605</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1491,7 +1491,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.007889811593841639</v>
+        <v>-0.009328921433373671</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.6938395517167446</v>
+        <v>1.152525195679933</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1543,7 +1543,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.5874869679720381</v>
+        <v>0.9736341010902606</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.5643375863482801</v>
+        <v>1.297472128273978</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1595,7 +1595,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.5990457476873547</v>
+        <v>0.9230993929333375</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1621,7 +1621,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.8020655970352654</v>
+        <v>0.9770271529592774</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1647,7 +1647,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.8113889532045915</v>
+        <v>1.300188020951307</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1673,7 +1673,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.7191213807384406</v>
+        <v>1.546153676316226</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1699,7 +1699,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.6739155603159158</v>
+        <v>1.20609419516364</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.6266197251338157</v>
+        <v>1.019139453594172</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1751,7 +1751,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.7719897319739162</v>
+        <v>1.196628386353387</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.480051396378577</v>
+        <v>0.8406185143355298</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.5962915605494619</v>
+        <v>1.161778438445792</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1829,7 +1829,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.4990453834932723</v>
+        <v>0.8019126382143702</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1855,7 +1855,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.7218771222449408</v>
+        <v>1.19045678195221</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1881,7 +1881,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.7425208189330139</v>
+        <v>1.64406325608195</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.6968586840790576</v>
+        <v>1.299300129651006</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.4871512350478486</v>
+        <v>0.8060291675244182</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1959,7 +1959,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.4416544864600802</v>
+        <v>0.9968093941272378</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1985,7 +1985,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.510232011685544</v>
+        <v>0.8160782051549252</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -2011,7 +2011,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.534487388282239</v>
+        <v>0.808228217767328</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -2037,7 +2037,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.5714169863760175</v>
+        <v>0.8973516234105906</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -2063,7 +2063,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.651930886723056</v>
+        <v>1.149662857102538</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.00456675294311994</v>
+        <v>1.371301553812185</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -2115,7 +2115,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.7067293537613037</v>
+        <v>0.8979241089680022</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -2141,7 +2141,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.5388255860652824</v>
+        <v>0.8117268046484413</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.4939411347201113</v>
+        <v>0.8023308361177167</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -2193,7 +2193,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.6179932578919405</v>
+        <v>1.058689616851366</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -2219,7 +2219,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.5779274288435179</v>
+        <v>0.9597311102219686</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -2245,7 +2245,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.5059489608497444</v>
+        <v>0.793655383802047</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -2271,7 +2271,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.542285671605204</v>
+        <v>0.8820544615209158</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -2297,7 +2297,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.5272915610965684</v>
+        <v>0.9002505895642162</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -2323,7 +2323,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.7582866753154796</v>
+        <v>1.65331287479124</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -2349,7 +2349,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.7675027913289278</v>
+        <v>1.103010743362235</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -2375,7 +2375,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.5320670861471846</v>
+        <v>1.144124984441628</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -2401,7 +2401,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.5176135823767993</v>
+        <v>0.7992675294739581</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.5089195431457716</v>
+        <v>0.87845264203492</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.4950234734336392</v>
+        <v>0.7977031503880849</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2479,7 +2479,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.4818025251932206</v>
+        <v>1.004918637784497</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2505,7 +2505,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.5070137454130099</v>
+        <v>0.8128335718637812</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2531,7 +2531,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0.8006317242857622</v>
+        <v>1.656729989157039</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.7542553607167379</v>
+        <v>1.310307363760873</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2583,7 +2583,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.6668828273305583</v>
+        <v>1.052679628979815</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2609,7 +2609,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.5874869679720381</v>
+        <v>0.9736341010902606</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2635,7 +2635,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.7225687218454563</v>
+        <v>1.191739326397291</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2661,7 +2661,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0.5525898298139794</v>
+        <v>0.9133102250669155</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2687,7 +2687,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.4956519171732275</v>
+        <v>0.7978591721836809</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2713,7 +2713,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.6418891868722517</v>
+        <v>0.8027227852954837</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2739,7 +2739,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.4402000803190848</v>
+        <v>0.9953481725579773</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2765,7 +2765,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.6105706556722432</v>
+        <v>0.9985257383160193</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2791,7 +2791,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.473443950670043</v>
+        <v>1.177096843518948</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2817,7 +2817,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.5959436824192121</v>
+        <v>0.9354285654204095</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2843,7 +2843,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.5357230559198708</v>
+        <v>1.145872458093022</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -2869,7 +2869,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.621854045808126</v>
+        <v>1.102173543057682</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2895,7 +2895,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.003130977900491801</v>
+        <v>0.2885249267089345</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2921,7 +2921,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.4464914290174098</v>
+        <v>1.004635220030704</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -2947,7 +2947,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0.5210543149744989</v>
+        <v>0.8865023898254771</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2974,7 +2974,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.5135765171143716</v>
+        <v>0.821578825130743</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -3000,7 +3000,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0.5284503448853383</v>
+        <v>1.140922812366161</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -3026,7 +3026,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0.4902746345167236</v>
+        <v>0.714503395830094</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0.7574149880649279</v>
+        <v>0.9724883674677001</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0.7114817891938328</v>
+        <v>1.084087129779844</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -3104,7 +3104,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.6250584216751288</v>
+        <v>1.046991585851753</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -3130,7 +3130,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0.5305921923522883</v>
+        <v>0.9005245002959414</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -3156,7 +3156,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>0.4907834134077879</v>
+        <v>0.7994926286410695</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0.5778514065214622</v>
+        <v>0.9598427629497396</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -3208,7 +3208,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>0.002721068270541498</v>
+        <v>0.003015071025280447</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -3234,7 +3234,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0.3937937339814045</v>
+        <v>0.402040483774579</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -3260,7 +3260,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>0.7020440901702445</v>
+        <v>1.164768315389567</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -3286,7 +3286,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>0.3483811968013244</v>
+        <v>0.3949164317674301</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -3312,7 +3312,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>0.654329973515289</v>
+        <v>1.016867235342934</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>0.4802027048352119</v>
+        <v>0.787535684465967</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -3364,7 +3364,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0.5874869679720381</v>
+        <v>0.9736341010902606</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -3390,7 +3390,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>0.4921853728232786</v>
+        <v>0.7936678103050605</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -3416,7 +3416,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0.7303869163960004</v>
+        <v>1.19508138732885</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0.5498442480266633</v>
+        <v>0.8856880781593204</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -3468,7 +3468,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>0.7538388284320459</v>
+        <v>1.309312010068817</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -3494,7 +3494,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>0.8095177988740521</v>
+        <v>1.104809434058442</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -3520,7 +3520,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0.5084011629095626</v>
+        <v>0.8130099040738472</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
@@ -3546,7 +3546,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>0.4440524446674365</v>
+        <v>1.000933600989995</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
@@ -3572,7 +3572,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>0.7580335980053102</v>
+        <v>1.091519160643542</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>0.813846369883884</v>
+        <v>1.303090774223941</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -3624,7 +3624,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>0.7525186475372635</v>
+        <v>0.9708822545719143</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -3650,7 +3650,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>0.7066727957410057</v>
+        <v>1.082389595924046</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -3676,7 +3676,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>0.6204253995894669</v>
+        <v>1.045324440417545</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -3702,7 +3702,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0.771972976582864</v>
+        <v>1.157126597218684</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -3728,7 +3728,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0.4996726726423966</v>
+        <v>0.8021783106325583</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -3754,7 +3754,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>0.5681753610689265</v>
+        <v>0.8402796965008181</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
@@ -3780,7 +3780,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>0.4674567367534873</v>
+        <v>1.003931981225926</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
@@ -3806,7 +3806,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0.5135467390317162</v>
+        <v>0.8216396937944614</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
@@ -3832,7 +3832,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>0.7556598934699111</v>
+        <v>1.312131528785209</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -3858,7 +3858,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0.4421045550580366</v>
+        <v>0.9977525088168081</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
@@ -3884,7 +3884,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.5752841456888848</v>
+        <v>0.9228475915176979</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
@@ -3910,7 +3910,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>0.719544479631357</v>
+        <v>1.150365203900187</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -3936,7 +3936,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0.5303758413222843</v>
+        <v>0.9026686090036761</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
@@ -3962,7 +3962,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>0.5081857076200115</v>
+        <v>1.090453557507115</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
@@ -3988,7 +3988,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>0.5104018992748692</v>
+        <v>0.8159920862280736</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
@@ -4014,7 +4014,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>0.4774003897985523</v>
+        <v>0.7842022986857551</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
@@ -4040,7 +4040,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>0.5315112931955098</v>
+        <v>0.9716699779419523</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
@@ -4066,7 +4066,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0.5683827472412131</v>
+        <v>1.083222161725817</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0.6487795090440738</v>
+        <v>1.046142100548664</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
@@ -4118,7 +4118,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0.543905966186926</v>
+        <v>0.8859548301057605</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
@@ -4144,7 +4144,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>0.541467501093442</v>
+        <v>0.7931090934313132</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
@@ -4170,7 +4170,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>0.476943801712326</v>
+        <v>0.7726264619423427</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
@@ -4196,7 +4196,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>0.7999673908241263</v>
+        <v>1.655891769342095</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
@@ -4222,7 +4222,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>0.7536082273604165</v>
+        <v>1.309578869092147</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
@@ -4248,7 +4248,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>0.6662680987740144</v>
+        <v>1.052032734757469</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
@@ -4274,7 +4274,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>0.7256235832803387</v>
+        <v>1.153413220353133</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
@@ -4300,7 +4300,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>0.4862440082148677</v>
+        <v>1.059995385067475</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
@@ -4326,7 +4326,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>0.480051396378577</v>
+        <v>0.8406185143355298</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
@@ -4352,7 +4352,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>0.4778653039044789</v>
+        <v>0.783992099392521</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0.7760576788558101</v>
+        <v>1.202466806333066</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
@@ -4404,7 +4404,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>0.7070905323552281</v>
+        <v>1.304865447552159</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
@@ -4431,7 +4431,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>0.766266203288982</v>
+        <v>1.102883248215501</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
@@ -4457,7 +4457,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>0.7551619983648222</v>
+        <v>0.9714058884172551</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
@@ -4483,7 +4483,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0.7092687720501192</v>
+        <v>1.082943039489161</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
@@ -4509,7 +4509,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>0.6229259336649657</v>
+        <v>1.045867975200999</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
@@ -4535,7 +4535,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>0.720906769228436</v>
+        <v>1.190825161130525</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
@@ -4561,7 +4561,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>0.003522335031410384</v>
+        <v>0.2888858810129574</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
@@ -4587,7 +4587,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>0.4470566570033783</v>
+        <v>1.005197686377464</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
@@ -4613,7 +4613,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0.5092684532938081</v>
+        <v>0.8159083644324522</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
@@ -4639,7 +4639,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>0.811416481343344</v>
+        <v>1.107894385802455</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
@@ -4665,7 +4665,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>0.5749470521413744</v>
+        <v>0.8110395791943045</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
@@ -4691,7 +4691,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>0.6124059509900321</v>
+        <v>0.9003023474705429</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>
@@ -4717,7 +4717,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>0.693934586815539</v>
+        <v>1.153008121267897</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
@@ -4743,7 +4743,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>0.5379246494456402</v>
+        <v>1.290141852419778</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
@@ -4769,7 +4769,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>0.4930642723757469</v>
+        <v>1.08734780026408</v>
       </c>
       <c r="D167" t="inlineStr">
         <is>
@@ -4795,7 +4795,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>0.6170524688931442</v>
+        <v>1.034777040740063</v>
       </c>
       <c r="D168" t="inlineStr">
         <is>
@@ -4821,7 +4821,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>0.6938050674451746</v>
+        <v>0.9673891174138604</v>
       </c>
       <c r="D169" t="inlineStr">
         <is>
@@ -4847,7 +4847,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>0.7658423414358785</v>
+        <v>1.102577451388186</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
@@ -4873,7 +4873,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>0.6243177140516517</v>
+        <v>1.049620302549755</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
@@ -4900,7 +4900,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>0.6120022751606462</v>
+        <v>0.9620680614896875</v>
       </c>
       <c r="D172" t="inlineStr">
         <is>
@@ -4927,7 +4927,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>0.4859168392105859</v>
+        <v>1.192826672629859</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>0.5147702967578196</v>
+        <v>0.8219952608780432</v>
       </c>
       <c r="D174" t="inlineStr">
         <is>
@@ -4979,7 +4979,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>0.545875720225144</v>
+        <v>0.909890661523359</v>
       </c>
       <c r="D175" t="inlineStr">
         <is>
@@ -5005,7 +5005,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>0.5305921923522883</v>
+        <v>0.9005245002959414</v>
       </c>
       <c r="D176" t="inlineStr">
         <is>
@@ -5031,7 +5031,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>0.480065581215994</v>
+        <v>0.7866742383695804</v>
       </c>
       <c r="D177" t="inlineStr">
         <is>
@@ -5057,7 +5057,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>0.5804577251203613</v>
+        <v>0.8187628032829893</v>
       </c>
       <c r="D178" t="inlineStr">
         <is>
@@ -5083,7 +5083,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>0.5137663643496321</v>
+        <v>1.096984294537662</v>
       </c>
       <c r="D179" t="inlineStr">
         <is>
@@ -5109,7 +5109,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>0.7537111607773304</v>
+        <v>0.9709570719707696</v>
       </c>
       <c r="D180" t="inlineStr">
         <is>
@@ -5135,7 +5135,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>0.7078438723906679</v>
+        <v>1.082468672815592</v>
       </c>
       <c r="D181" t="inlineStr">
         <is>
@@ -5161,7 +5161,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>0.6215532897066977</v>
+        <v>1.045402101449318</v>
       </c>
       <c r="D182" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>0.7721412768866881</v>
+        <v>1.197423670884637</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
@@ -5213,7 +5213,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>0.574119702414803</v>
+        <v>0.9226375361752605</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
@@ -5239,7 +5239,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>0.5330695360947558</v>
+        <v>0.8082442268551389</v>
       </c>
       <c r="D185" t="inlineStr">
         <is>
@@ -5265,7 +5265,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>0.4883403096353498</v>
+        <v>0.7988463550005407</v>
       </c>
       <c r="D186" t="inlineStr">
         <is>
@@ -5291,7 +5291,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>0.6119802474015924</v>
+        <v>1.054868618009125</v>
       </c>
       <c r="D187" t="inlineStr">
         <is>
@@ -5317,7 +5317,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>0.005229053737757906</v>
+        <v>0.2783237528758306</v>
       </c>
       <c r="D188" t="inlineStr">
         <is>
@@ -5343,7 +5343,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>0.6158179008036555</v>
+        <v>0.9047861053116246</v>
       </c>
       <c r="D189" t="inlineStr">
         <is>
@@ -5369,7 +5369,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>0.5801729178723267</v>
+        <v>0.81806566225674</v>
       </c>
       <c r="D190" t="inlineStr">
         <is>
@@ -5395,7 +5395,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>0.001411982538289157</v>
+        <v>0.4023500350798024</v>
       </c>
       <c r="D191" t="inlineStr">
         <is>
@@ -5421,7 +5421,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>0.480051396378577</v>
+        <v>0.8406185143355298</v>
       </c>
       <c r="D192" t="inlineStr">
         <is>
@@ -5447,7 +5447,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>0.6045025645922981</v>
+        <v>0.958535990820544</v>
       </c>
       <c r="D193" t="inlineStr">
         <is>
@@ -5473,7 +5473,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>0.5084504756410342</v>
+        <v>1.285794488867437</v>
       </c>
       <c r="D194" t="inlineStr">
         <is>
@@ -5499,7 +5499,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>0.5726193329461753</v>
+        <v>0.9739088391417525</v>
       </c>
       <c r="D195" t="inlineStr">
         <is>
@@ -5525,7 +5525,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>0.4912158691765995</v>
+        <v>0.7933492809089383</v>
       </c>
       <c r="D196" t="inlineStr">
         <is>
@@ -5551,7 +5551,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>0.3881870590208416</v>
+        <v>0.8437139661855002</v>
       </c>
       <c r="D197" t="inlineStr">
         <is>
@@ -5577,7 +5577,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>0.4660163787522322</v>
+        <v>0.7717237840964803</v>
       </c>
       <c r="D198" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>0.5344240184643225</v>
+        <v>0.904715844874459</v>
       </c>
       <c r="D199" t="inlineStr">
         <is>
@@ -5629,7 +5629,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>0.7242653065127765</v>
+        <v>1.191936519506979</v>
       </c>
       <c r="D200" t="inlineStr">
         <is>
@@ -5655,7 +5655,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>0.6671596847695089</v>
+        <v>0.9469300328248199</v>
       </c>
       <c r="D201" t="inlineStr">
         <is>
@@ -5681,7 +5681,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>0.4819133211437011</v>
+        <v>0.7906259106340428</v>
       </c>
       <c r="D202" t="inlineStr">
         <is>
@@ -5707,7 +5707,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>0.6105664544985002</v>
+        <v>0.9612751316359143</v>
       </c>
       <c r="D203" t="inlineStr">
         <is>
@@ -5733,7 +5733,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>0.7185507494429584</v>
+        <v>1.189805315787567</v>
       </c>
       <c r="D204" t="inlineStr">
         <is>
@@ -5759,7 +5759,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>1.0111328324688</v>
+        <v>1.080289987075832</v>
       </c>
       <c r="D205" t="inlineStr">
         <is>
@@ -5785,7 +5785,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>0.6277723986636564</v>
+        <v>1.039247667390604</v>
       </c>
       <c r="D206" t="inlineStr">
         <is>
@@ -5811,7 +5811,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>0.5331477624034205</v>
+        <v>0.98741648837243</v>
       </c>
       <c r="D207" t="inlineStr">
         <is>
@@ -5837,7 +5837,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>0.4837548925363499</v>
+        <v>0.7838171772697139</v>
       </c>
       <c r="D208" t="inlineStr">
         <is>
@@ -5863,7 +5863,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>0.5984238127285088</v>
+        <v>0.9053906674357205</v>
       </c>
       <c r="D209" t="inlineStr">
         <is>
@@ -5889,7 +5889,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>0.4776838977840286</v>
+        <v>1.010574966033383</v>
       </c>
       <c r="D210" t="inlineStr">
         <is>
@@ -5915,7 +5915,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>0.6149141909129613</v>
+        <v>0.9716635923413418</v>
       </c>
       <c r="D211" t="inlineStr">
         <is>
@@ -5941,7 +5941,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>0.5323365171849384</v>
+        <v>1.183728486429264</v>
       </c>
       <c r="D212" t="inlineStr">
         <is>
@@ -5967,7 +5967,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>0.5013511368540552</v>
+        <v>1.040350276124655</v>
       </c>
       <c r="D213" t="inlineStr">
         <is>
@@ -5993,7 +5993,7 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>0.766646179247911</v>
+        <v>1.294946667666711</v>
       </c>
       <c r="D214" t="inlineStr">
         <is>
@@ -6019,7 +6019,7 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>0.6250757849934008</v>
+        <v>1.047030124807407</v>
       </c>
       <c r="D215" t="inlineStr">
         <is>
@@ -6045,7 +6045,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>0.5637758133162106</v>
+        <v>0.9343678160062792</v>
       </c>
       <c r="D216" t="inlineStr">
         <is>
@@ -6071,7 +6071,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>0.6184173132138232</v>
+        <v>0.9805763031769701</v>
       </c>
       <c r="D217" t="inlineStr">
         <is>
@@ -6097,7 +6097,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>0.5061141976645372</v>
+        <v>0.8096937291822263</v>
       </c>
       <c r="D218" t="inlineStr">
         <is>
@@ -6123,7 +6123,7 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>0.5173496359938339</v>
+        <v>0.8247297348223899</v>
       </c>
       <c r="D219" t="inlineStr">
         <is>
@@ -6149,7 +6149,7 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>0.5982196850958632</v>
+        <v>0.9218615071990631</v>
       </c>
       <c r="D220" t="inlineStr">
         <is>
@@ -6175,7 +6175,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>0.6790550763099459</v>
+        <v>1.045300624997171</v>
       </c>
       <c r="D221" t="inlineStr">
         <is>
@@ -6201,7 +6201,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>0.7730868745805141</v>
+        <v>1.19847753556293</v>
       </c>
       <c r="D222" t="inlineStr">
         <is>
@@ -6227,7 +6227,7 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>0.5124725506101819</v>
+        <v>0.8190686780079089</v>
       </c>
       <c r="D223" t="inlineStr">
         <is>
@@ -6253,7 +6253,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>0.5708032187152575</v>
+        <v>0.9349921379667659</v>
       </c>
       <c r="D224" t="inlineStr">
         <is>
@@ -6279,7 +6279,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>0.4984952140853634</v>
+        <v>0.801818688443401</v>
       </c>
       <c r="D225" t="inlineStr">
         <is>
@@ -6305,7 +6305,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>0.4847762240172538</v>
+        <v>0.7838549960904776</v>
       </c>
       <c r="D226" t="inlineStr">
         <is>
@@ -6331,7 +6331,7 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>0.7068931436419978</v>
+        <v>1.182327166446044</v>
       </c>
       <c r="D227" t="inlineStr">
         <is>
@@ -6357,7 +6357,7 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>0.7751623533392132</v>
+        <v>1.161605015643351</v>
       </c>
       <c r="D228" t="inlineStr">
         <is>
@@ -6383,7 +6383,7 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>0.8049965390109113</v>
+        <v>1.663130660002236</v>
       </c>
       <c r="D229" t="inlineStr">
         <is>
@@ -6409,7 +6409,7 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>0.8143351233536988</v>
+        <v>1.110784904955627</v>
       </c>
       <c r="D230" t="inlineStr">
         <is>
@@ -6435,7 +6435,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>0.5463525660363906</v>
+        <v>0.8852475101494343</v>
       </c>
       <c r="D231" t="inlineStr">
         <is>
@@ -6461,7 +6461,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>0.6178054966395019</v>
+        <v>1.009453232784819</v>
       </c>
       <c r="D232" t="inlineStr">
         <is>
@@ -6487,7 +6487,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>0.7066528959830991</v>
+        <v>1.182299727162589</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -6513,7 +6513,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>0.40182332858359</v>
+        <v>0.7485515355909331</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -6539,7 +6539,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>0.5754402112890188</v>
+        <v>0.9035284669797958</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -6565,7 +6565,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>0.703855751805904</v>
+        <v>1.180540922939193</v>
       </c>
       <c r="D236" t="inlineStr">
         <is>
@@ -6591,7 +6591,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>0.6022461320635195</v>
+        <v>1.17049186955002</v>
       </c>
       <c r="D237" t="inlineStr">
         <is>
@@ -6617,7 +6617,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>0.5354326577457433</v>
+        <v>0.904961133294546</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
@@ -6643,7 +6643,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>0.508203755433044</v>
+        <v>0.8735872506309847</v>
       </c>
       <c r="D239" t="inlineStr">
         <is>
@@ -6669,7 +6669,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>0.5151872058299167</v>
+        <v>0.8220602544230596</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>
@@ -6695,7 +6695,7 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>0.5939614561347774</v>
+        <v>1.157822765181761</v>
       </c>
       <c r="D241" t="inlineStr">
         <is>
@@ -6721,7 +6721,7 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>0.5112431605243881</v>
+        <v>0.8187712083289204</v>
       </c>
       <c r="D242" t="inlineStr">
         <is>
@@ -6747,7 +6747,7 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>0.5941396217080936</v>
+        <v>0.9166075345436369</v>
       </c>
       <c r="D243" t="inlineStr">
         <is>
@@ -6773,7 +6773,7 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>0.5296794476667871</v>
+        <v>0.901234518440594</v>
       </c>
       <c r="D244" t="inlineStr">
         <is>
@@ -6799,7 +6799,7 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>0.5059891216711152</v>
+        <v>0.8097351777541896</v>
       </c>
       <c r="D245" t="inlineStr">
         <is>
@@ -6825,7 +6825,7 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>0.7080784481856572</v>
+        <v>1.183779967035533</v>
       </c>
       <c r="D246" t="inlineStr">
         <is>
@@ -6851,7 +6851,7 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>0.5874869679720381</v>
+        <v>0.9736341010902606</v>
       </c>
       <c r="D247" t="inlineStr">
         <is>
@@ -6877,7 +6877,7 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>0.6103135410736518</v>
+        <v>0.9992578928547016</v>
       </c>
       <c r="D248" t="inlineStr">
         <is>
@@ -6903,7 +6903,7 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>0.564592005240703</v>
+        <v>1.296976663779622</v>
       </c>
       <c r="D249" t="inlineStr">
         <is>
@@ -6929,7 +6929,7 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>0.5178359708966128</v>
+        <v>0.8248289664701212</v>
       </c>
       <c r="D250" t="inlineStr">
         <is>
@@ -6955,7 +6955,7 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>0.515040632306609</v>
+        <v>0.822007614376669</v>
       </c>
       <c r="D251" t="inlineStr">
         <is>
@@ -6981,7 +6981,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>0.543905966186926</v>
+        <v>0.8859548301057605</v>
       </c>
       <c r="D252" t="inlineStr">
         <is>
@@ -7007,7 +7007,7 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>0.3961721222324364</v>
+        <v>0.6836071386768621</v>
       </c>
       <c r="D253" t="inlineStr">
         <is>
@@ -7033,7 +7033,7 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>0.6249774080026272</v>
+        <v>0.9171012635629811</v>
       </c>
       <c r="D254" t="inlineStr">
         <is>
@@ -7059,7 +7059,7 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>0.005722584807563865</v>
+        <v>0.006383140819778305</v>
       </c>
       <c r="D255" t="inlineStr">
         <is>
@@ -7085,7 +7085,7 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>0.6102361142854303</v>
+        <v>1.084647289073029</v>
       </c>
       <c r="D256" t="inlineStr">
         <is>
@@ -7111,7 +7111,7 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>0.759760702896024</v>
+        <v>1.317788614706045</v>
       </c>
       <c r="D257" t="inlineStr">
         <is>
@@ -7137,7 +7137,7 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>0.8156285117387028</v>
+        <v>1.112532527464772</v>
       </c>
       <c r="D258" t="inlineStr">
         <is>
@@ -7163,7 +7163,7 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>0.2971001991276088</v>
+        <v>0.7664692548041706</v>
       </c>
       <c r="D259" t="inlineStr">
         <is>
@@ -7189,7 +7189,7 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>1.016127186660797</v>
+        <v>1.080308649558468</v>
       </c>
       <c r="D260" t="inlineStr">
         <is>
@@ -7215,7 +7215,7 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>0.7742725885733329</v>
+        <v>1.202170835770731</v>
       </c>
       <c r="D261" t="inlineStr">
         <is>
@@ -7241,7 +7241,7 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>0.5287563153563123</v>
+        <v>1.140067129806242</v>
       </c>
       <c r="D262" t="inlineStr">
         <is>
@@ -7267,7 +7267,7 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>0.63092262088579</v>
+        <v>1.138659808989161</v>
       </c>
       <c r="D263" t="inlineStr">
         <is>
@@ -7293,7 +7293,7 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>0.4876287902480587</v>
+        <v>0.7888125846860762</v>
       </c>
       <c r="D264" t="inlineStr">
         <is>
@@ -7319,7 +7319,7 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>0.7737451956589788</v>
+        <v>1.159653805646729</v>
       </c>
       <c r="D265" t="inlineStr">
         <is>
@@ -7345,7 +7345,7 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>0.505523230624264</v>
+        <v>0.8095296850537064</v>
       </c>
       <c r="D266" t="inlineStr">
         <is>
@@ -7371,7 +7371,7 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>0.7582372004669664</v>
+        <v>1.091620561568922</v>
       </c>
       <c r="D267" t="inlineStr">
         <is>
@@ -7397,7 +7397,7 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>0.7298596302391213</v>
+        <v>1.194325578929917</v>
       </c>
       <c r="D268" t="inlineStr">
         <is>
@@ -7423,7 +7423,7 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>0.6906615681288837</v>
+        <v>1.100191201786831</v>
       </c>
       <c r="D269" t="inlineStr">
         <is>
@@ -7449,7 +7449,7 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>0.5930476607874037</v>
+        <v>1.156267262962512</v>
       </c>
       <c r="D270" t="inlineStr">
         <is>
@@ -7475,7 +7475,7 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>0.5100121141842502</v>
+        <v>0.8161271876364102</v>
       </c>
       <c r="D271" t="inlineStr">
         <is>
@@ -7501,7 +7501,7 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>0.5033254768752925</v>
+        <v>1.041139135198765</v>
       </c>
       <c r="D272" t="inlineStr">
         <is>
@@ -7527,7 +7527,7 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>0.8095413035598503</v>
+        <v>0.8893724982224133</v>
       </c>
       <c r="D273" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>0.5030457814761768</v>
+        <v>0.8056253464069706</v>
       </c>
       <c r="D274" t="inlineStr">
         <is>
@@ -7579,7 +7579,7 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>0.511949306442247</v>
+        <v>0.8164495691285552</v>
       </c>
       <c r="D275" t="inlineStr">
         <is>
@@ -7605,7 +7605,7 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>0.4961743804129929</v>
+        <v>0.7981955945459819</v>
       </c>
       <c r="D276" t="inlineStr">
         <is>
@@ -7631,7 +7631,7 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>0.5060899815282843</v>
+        <v>0.8098260913854762</v>
       </c>
       <c r="D277" t="inlineStr">
         <is>
@@ -7657,7 +7657,7 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>0.564647121911473</v>
+        <v>1.297422262911572</v>
       </c>
       <c r="D278" t="inlineStr">
         <is>
@@ -7683,7 +7683,7 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>0.2852564012916069</v>
+        <v>0.6905856838873534</v>
       </c>
       <c r="D279" t="inlineStr">
         <is>
@@ -7709,7 +7709,7 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>0.6923943533240565</v>
+        <v>1.049237009245282</v>
       </c>
       <c r="D280" t="inlineStr">
         <is>
@@ -7735,7 +7735,7 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>0.4674567367534873</v>
+        <v>1.003931981225926</v>
       </c>
       <c r="D281" t="inlineStr">
         <is>
@@ -7761,7 +7761,7 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>0.6199741487064104</v>
+        <v>0.9107387317951309</v>
       </c>
       <c r="D282" t="inlineStr">
         <is>
@@ -7787,7 +7787,7 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>0.002782312435445793</v>
+        <v>0.4045992360076677</v>
       </c>
       <c r="D283" t="inlineStr">
         <is>
@@ -7813,7 +7813,7 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>0.6263404363753264</v>
+        <v>0.9494829025377663</v>
       </c>
       <c r="D284" t="inlineStr">
         <is>
@@ -7839,7 +7839,7 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>0.5752841456888848</v>
+        <v>0.9228475915176979</v>
       </c>
       <c r="D285" t="inlineStr">
         <is>
@@ -7865,7 +7865,7 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>0.586878052129718</v>
+        <v>0.8846132081003446</v>
       </c>
       <c r="D286" t="inlineStr">
         <is>
@@ -7891,7 +7891,7 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>0.40182332858359</v>
+        <v>0.7485515355909331</v>
       </c>
       <c r="D287" t="inlineStr">
         <is>
@@ -7917,7 +7917,7 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>0.6238309803816657</v>
+        <v>0.9812396747978469</v>
       </c>
       <c r="D288" t="inlineStr">
         <is>
@@ -7943,7 +7943,7 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>0.6330642191776333</v>
+        <v>0.989738072531985</v>
       </c>
       <c r="D289" t="inlineStr">
         <is>
@@ -7969,7 +7969,7 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>0.5964592983517919</v>
+        <v>1.161805099536567</v>
       </c>
       <c r="D290" t="inlineStr">
         <is>
@@ -7995,7 +7995,7 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>0.4493825448300773</v>
+        <v>0.799965221053682</v>
       </c>
       <c r="D291" t="inlineStr">
         <is>
@@ -8021,7 +8021,7 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>0.7750219144814838</v>
+        <v>1.161492035442104</v>
       </c>
       <c r="D292" t="inlineStr">
         <is>
@@ -8047,7 +8047,7 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>0.6042900605328243</v>
+        <v>1.213746462992864</v>
       </c>
       <c r="D293" t="inlineStr">
         <is>
@@ -8073,7 +8073,7 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>0.4957306442269463</v>
+        <v>0.7979124913723817</v>
       </c>
       <c r="D294" t="inlineStr">
         <is>
@@ -8099,7 +8099,7 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>0.4769876951159101</v>
+        <v>0.77768632045761</v>
       </c>
       <c r="D295" t="inlineStr">
         <is>
@@ -8125,7 +8125,7 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>0.6536168951899896</v>
+        <v>0.9647000843027527</v>
       </c>
       <c r="D296" t="inlineStr">
         <is>
@@ -8151,7 +8151,7 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>0.4912158691765995</v>
+        <v>0.7933492809089383</v>
       </c>
       <c r="D297" t="inlineStr">
         <is>
@@ -8177,7 +8177,7 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>0.5058317851691435</v>
+        <v>0.8097189976521512</v>
       </c>
       <c r="D298" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>0.6000492240341959</v>
+        <v>0.9243621920393591</v>
       </c>
       <c r="D299" t="inlineStr">
         <is>
@@ -8229,7 +8229,7 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>0.5362706932000687</v>
+        <v>0.904974404969567</v>
       </c>
       <c r="D300" t="inlineStr">
         <is>
@@ -8255,7 +8255,7 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>0.6100716725113579</v>
+        <v>0.897140503265181</v>
       </c>
       <c r="D301" t="inlineStr">
         <is>
@@ -8281,7 +8281,7 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>0.5638036642775844</v>
+        <v>0.8876006355793847</v>
       </c>
       <c r="D302" t="inlineStr">
         <is>
@@ -8307,7 +8307,7 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>0.7592382746268913</v>
+        <v>1.092744516514538</v>
       </c>
       <c r="D303" t="inlineStr">
         <is>
@@ -8333,7 +8333,7 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>0.8150894386995162</v>
+        <v>1.304440538171306</v>
       </c>
       <c r="D304" t="inlineStr">
         <is>
@@ -8359,7 +8359,7 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>0.4932423776558644</v>
+        <v>1.070435198633322</v>
       </c>
       <c r="D305" t="inlineStr">
         <is>
@@ -8385,7 +8385,7 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>0.4987518039950561</v>
+        <v>1.078851910309706</v>
       </c>
       <c r="D306" t="inlineStr">
         <is>
@@ -8411,7 +8411,7 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>0.9133873120813211</v>
+        <v>1.188235858747638</v>
       </c>
       <c r="D307" t="inlineStr">
         <is>
@@ -8437,7 +8437,7 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>0.5120424878806242</v>
+        <v>0.8165698000770351</v>
       </c>
       <c r="D308" t="inlineStr">
         <is>
@@ -8463,7 +8463,7 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>0.5942203675323584</v>
+        <v>0.9164297500094949</v>
       </c>
       <c r="D309" t="inlineStr">
         <is>
@@ -8489,7 +8489,7 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>0.7007853487918478</v>
+        <v>1.179304675031934</v>
       </c>
       <c r="D310" t="inlineStr">
         <is>
@@ -8515,7 +8515,7 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>0.7722196504311367</v>
+        <v>1.19722019516806</v>
       </c>
       <c r="D311" t="inlineStr">
         <is>
@@ -8541,7 +8541,7 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>0.5518038386716035</v>
+        <v>0.8876790204652035</v>
       </c>
       <c r="D312" t="inlineStr">
         <is>
@@ -8567,7 +8567,7 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>0.5065818633872063</v>
+        <v>0.8781870767483215</v>
       </c>
       <c r="D313" t="inlineStr">
         <is>
@@ -8593,7 +8593,7 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>0.5504156222658719</v>
+        <v>0.8863505060913084</v>
       </c>
       <c r="D314" t="inlineStr">
         <is>
@@ -8619,7 +8619,7 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>0.5052289100747341</v>
+        <v>0.8768653016915404</v>
       </c>
       <c r="D315" t="inlineStr">
         <is>
@@ -8645,7 +8645,7 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>0.7763163545822119</v>
+        <v>1.163253050824435</v>
       </c>
       <c r="D316" t="inlineStr">
         <is>
@@ -8671,7 +8671,7 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>0.7773830320284503</v>
+        <v>1.164508235182245</v>
       </c>
       <c r="D317" t="inlineStr">
         <is>
@@ -8697,7 +8697,7 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>0.5498247931403408</v>
+        <v>0.9114518428328982</v>
       </c>
       <c r="D318" t="inlineStr">
         <is>
@@ -8723,7 +8723,7 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>0.6113325635159776</v>
+        <v>0.8989539024575023</v>
       </c>
       <c r="D319" t="inlineStr">
         <is>
@@ -8749,7 +8749,7 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>0.7145955753441948</v>
+        <v>1.147991179603878</v>
       </c>
       <c r="D320" t="inlineStr">
         <is>
@@ -8775,7 +8775,7 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>0.4335328512216905</v>
+        <v>0.9616363119716375</v>
       </c>
       <c r="D321" t="inlineStr">
         <is>
@@ -8801,7 +8801,7 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>0.5357401162328252</v>
+        <v>1.145944945302291</v>
       </c>
       <c r="D322" t="inlineStr">
         <is>
@@ -8827,7 +8827,7 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>0.7140984755589062</v>
+        <v>1.148526077313738</v>
       </c>
       <c r="D323" t="inlineStr">
         <is>
@@ -8853,7 +8853,7 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>0.5364322532267052</v>
+        <v>1.145289764256723</v>
       </c>
       <c r="D324" t="inlineStr">
         <is>
@@ -8879,7 +8879,7 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>0.7714281570247011</v>
+        <v>1.196160152881235</v>
       </c>
       <c r="D325" t="inlineStr">
         <is>
@@ -8905,7 +8905,7 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>0.5175443333503588</v>
+        <v>0.8245390871344461</v>
       </c>
       <c r="D326" t="inlineStr">
         <is>
@@ -8931,7 +8931,7 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>0.4561164357391147</v>
+        <v>0.9815764878376714</v>
       </c>
       <c r="D327" t="inlineStr">
         <is>
@@ -8957,7 +8957,7 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>0.5507626904539298</v>
+        <v>0.9048165736872354</v>
       </c>
       <c r="D328" t="inlineStr">
         <is>
@@ -8983,7 +8983,7 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>0.7266256628485734</v>
+        <v>1.192999712469995</v>
       </c>
       <c r="D329" t="inlineStr">
         <is>
@@ -9009,7 +9009,7 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>0.6507639487571596</v>
+        <v>1.011069752334873</v>
       </c>
       <c r="D330" t="inlineStr">
         <is>
@@ -9035,7 +9035,7 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>0.7546598751505789</v>
+        <v>1.086979311609661</v>
       </c>
       <c r="D331" t="inlineStr">
         <is>
@@ -9061,7 +9061,7 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>0.441284026626288</v>
+        <v>0.9965912285912136</v>
       </c>
       <c r="D332" t="inlineStr">
         <is>
@@ -9087,7 +9087,7 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>0.8103650490439921</v>
+        <v>1.298089698803732</v>
       </c>
       <c r="D333" t="inlineStr">
         <is>
@@ -9113,7 +9113,7 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>0.5874869679720381</v>
+        <v>0.9736341010902606</v>
       </c>
       <c r="D334" t="inlineStr">
         <is>
@@ -9139,7 +9139,7 @@
         </is>
       </c>
       <c r="C335" t="n">
-        <v>0.7663033244902087</v>
+        <v>1.295417156244694</v>
       </c>
       <c r="D335" t="inlineStr">
         <is>
@@ -9165,7 +9165,7 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>0.4493825448300773</v>
+        <v>0.799965221053682</v>
       </c>
       <c r="D336" t="inlineStr">
         <is>
@@ -9191,7 +9191,7 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>0.7821428025893818</v>
+        <v>1.210980135096017</v>
       </c>
       <c r="D337" t="inlineStr">
         <is>
@@ -9217,7 +9217,7 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>0.5233505392577787</v>
+        <v>0.8982734872145269</v>
       </c>
       <c r="D338" t="inlineStr">
         <is>
@@ -9243,7 +9243,7 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>0.5343112851967439</v>
+        <v>0.808663669989255</v>
       </c>
       <c r="D339" t="inlineStr">
         <is>
@@ -9269,7 +9269,7 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>0.5290551116765003</v>
+        <v>0.9011652575302479</v>
       </c>
       <c r="D340" t="inlineStr">
         <is>
@@ -9295,7 +9295,7 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>0.5347970006146151</v>
+        <v>0.9896205918281874</v>
       </c>
       <c r="D341" t="inlineStr">
         <is>
@@ -9321,7 +9321,7 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>0.5931164603496929</v>
+        <v>0.9163335731980065</v>
       </c>
       <c r="D342" t="inlineStr">
         <is>
@@ -9347,7 +9347,7 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>0.6187416390751018</v>
+        <v>0.9089015200882787</v>
       </c>
       <c r="D343" t="inlineStr">
         <is>
@@ -9373,7 +9373,7 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>0.4493825448300773</v>
+        <v>0.799965221053682</v>
       </c>
       <c r="D344" t="inlineStr">
         <is>
@@ -9399,7 +9399,7 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>0.5194282263536564</v>
+        <v>1.136549070821849</v>
       </c>
       <c r="D345" t="inlineStr">
         <is>
@@ -9425,7 +9425,7 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>0.6440797448109135</v>
+        <v>1.004349073791385</v>
       </c>
       <c r="D346" t="inlineStr">
         <is>
@@ -9451,7 +9451,7 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>0.4962380407298554</v>
+        <v>1.175297994823818</v>
       </c>
       <c r="D347" t="inlineStr">
         <is>
@@ -9477,7 +9477,7 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>0.5394662901371123</v>
+        <v>0.9063522918568704</v>
       </c>
       <c r="D348" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>0.5624221260132576</v>
+        <v>0.9426836346928026</v>
       </c>
       <c r="D349" t="inlineStr">
         <is>
@@ -9529,7 +9529,7 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>0.6238309803816657</v>
+        <v>0.9812396747978469</v>
       </c>
       <c r="D350" t="inlineStr">
         <is>
@@ -9555,7 +9555,7 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>0.524463812185918</v>
+        <v>0.8984831630703159</v>
       </c>
       <c r="D351" t="inlineStr">
         <is>
@@ -9581,7 +9581,7 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>0.5487229409660401</v>
+        <v>1.152511172722902</v>
       </c>
       <c r="D352" t="inlineStr">
         <is>
@@ -9607,7 +9607,7 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>0.5684949149071238</v>
+        <v>0.6986696015812173</v>
       </c>
       <c r="D353" t="inlineStr">
         <is>
@@ -9633,7 +9633,7 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>0.5969777524877322</v>
+        <v>0.9202397095788424</v>
       </c>
       <c r="D354" t="inlineStr">
         <is>
@@ -9659,7 +9659,7 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>0.7231408702352859</v>
+        <v>1.15150030765314</v>
       </c>
       <c r="D355" t="inlineStr">
         <is>
@@ -9685,7 +9685,7 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>0.5592316590640217</v>
+        <v>0.8912788934279851</v>
       </c>
       <c r="D356" t="inlineStr">
         <is>
@@ -9711,7 +9711,7 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>0.5846523385396194</v>
+        <v>0.823669758195022</v>
       </c>
       <c r="D357" t="inlineStr">
         <is>
@@ -9737,7 +9737,7 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>0.6223428613935859</v>
+        <v>0.913557152338528</v>
       </c>
       <c r="D358" t="inlineStr">
         <is>
@@ -9763,7 +9763,7 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>0.5066533151288171</v>
+        <v>0.8738729052802318</v>
       </c>
       <c r="D359" t="inlineStr">
         <is>
@@ -9789,7 +9789,7 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>0.5290590394960357</v>
+        <v>0.9011286846481411</v>
       </c>
       <c r="D360" t="inlineStr">
         <is>
@@ -9815,7 +9815,7 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>0.5026960450108879</v>
+        <v>0.8060002607660285</v>
       </c>
       <c r="D361" t="inlineStr">
         <is>
@@ -9841,7 +9841,7 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>0.7758409640193364</v>
+        <v>1.162257196413647</v>
       </c>
       <c r="D362" t="inlineStr">
         <is>
@@ -9867,7 +9867,7 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>0.5367395747530843</v>
+        <v>0.9055445607947552</v>
       </c>
       <c r="D363" t="inlineStr">
         <is>
@@ -9893,7 +9893,7 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>0.511273877446607</v>
+        <v>0.816177947254238</v>
       </c>
       <c r="D364" t="inlineStr">
         <is>
@@ -9919,7 +9919,7 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>0.5368295343919249</v>
+        <v>1.18536195278948</v>
       </c>
       <c r="D365" t="inlineStr">
         <is>
@@ -9945,7 +9945,7 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>0.5857667549009983</v>
+        <v>0.9917385700172701</v>
       </c>
       <c r="D366" t="inlineStr">
         <is>
@@ -9971,7 +9971,7 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>0.5768290059470809</v>
+        <v>1.317310852555214</v>
       </c>
       <c r="D367" t="inlineStr">
         <is>
@@ -9997,7 +9997,7 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>0.5217365606481907</v>
+        <v>0.7935096669221362</v>
       </c>
       <c r="D368" t="inlineStr">
         <is>
@@ -10023,7 +10023,7 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>0.5058150452632076</v>
+        <v>0.7936083685744214</v>
       </c>
       <c r="D369" t="inlineStr">
         <is>
@@ -10049,7 +10049,7 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>0.6998902756073623</v>
+        <v>1.05942309850988</v>
       </c>
       <c r="D370" t="inlineStr">
         <is>
@@ -10075,7 +10075,7 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>0.52421591155307</v>
+        <v>0.8990509251553289</v>
       </c>
       <c r="D371" t="inlineStr">
         <is>
@@ -10101,7 +10101,7 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>0.6102920866003034</v>
+        <v>0.8977808369094461</v>
       </c>
       <c r="D372" t="inlineStr">
         <is>
@@ -10127,7 +10127,7 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>0.5297813462956368</v>
+        <v>0.8031534166987926</v>
       </c>
       <c r="D373" t="inlineStr">
         <is>
@@ -10153,7 +10153,7 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>0.4577276884287985</v>
+        <v>0.7914904501816945</v>
       </c>
       <c r="D374" t="inlineStr">
         <is>
@@ -10179,7 +10179,7 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>0.589386505000849</v>
+        <v>0.9377001146258521</v>
       </c>
       <c r="D375" t="inlineStr">
         <is>
@@ -10205,7 +10205,7 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>0.6078763270877966</v>
+        <v>1.046435937996625</v>
       </c>
       <c r="D376" t="inlineStr">
         <is>
@@ -10231,7 +10231,7 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>0.7521097918236626</v>
+        <v>1.099147923823703</v>
       </c>
       <c r="D377" t="inlineStr">
         <is>
@@ -10257,7 +10257,7 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>0.6113902211621074</v>
+        <v>1.046277668348691</v>
       </c>
       <c r="D378" t="inlineStr">
         <is>
@@ -10283,7 +10283,7 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>0.4413359316007087</v>
+        <v>0.6532295078409319</v>
       </c>
       <c r="D379" t="inlineStr">
         <is>
@@ -10309,7 +10309,7 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>1.016307893474708</v>
+        <v>1.010432249814712</v>
       </c>
       <c r="D380" t="inlineStr">
         <is>
@@ -10335,7 +10335,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>0.7033688025466308</v>
+        <v>1.064043360835601</v>
       </c>
       <c r="D381" t="inlineStr">
         <is>
@@ -10361,7 +10361,7 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>0.7575213402076694</v>
+        <v>1.314739329745646</v>
       </c>
       <c r="D382" t="inlineStr">
         <is>
@@ -10387,7 +10387,7 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>0.8133177822534652</v>
+        <v>1.109754165537558</v>
       </c>
       <c r="D383" t="inlineStr">
         <is>
@@ -10413,7 +10413,7 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>0.6699853688905447</v>
+        <v>1.056615399094345</v>
       </c>
       <c r="D384" t="inlineStr">
         <is>
@@ -10439,7 +10439,7 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>0.5310341616655254</v>
+        <v>0.9027166314437385</v>
       </c>
       <c r="D385" t="inlineStr">
         <is>
@@ -10465,7 +10465,7 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>0.522486348512599</v>
+        <v>0.8974467798892408</v>
       </c>
       <c r="D386" t="inlineStr">
         <is>
@@ -10491,7 +10491,7 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>0.4383163213972944</v>
+        <v>0.7696044049798559</v>
       </c>
       <c r="D387" t="inlineStr">
         <is>
@@ -10517,7 +10517,7 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>1.017959773290549</v>
+        <v>1.308371901557461</v>
       </c>
       <c r="D388" t="inlineStr">
         <is>
@@ -10543,7 +10543,7 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>0.6227125092586951</v>
+        <v>0.9139881720070478</v>
       </c>
       <c r="D389" t="inlineStr">
         <is>
@@ -10569,7 +10569,7 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>0.5760798891987891</v>
+        <v>0.9043632787410276</v>
       </c>
       <c r="D390" t="inlineStr">
         <is>
@@ -10595,7 +10595,7 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>0.5410240692164086</v>
+        <v>1.06699335378894</v>
       </c>
       <c r="D391" t="inlineStr">
         <is>
@@ -10621,7 +10621,7 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>0.2283975634450452</v>
+        <v>0.6749086909127469</v>
       </c>
       <c r="D392" t="inlineStr">
         <is>
@@ -10647,7 +10647,7 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>0.6149141909129613</v>
+        <v>0.9716635923413418</v>
       </c>
       <c r="D393" t="inlineStr">
         <is>
@@ -10673,7 +10673,7 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>0.1373908425006979</v>
+        <v>0.3786150638679462</v>
       </c>
       <c r="D394" t="inlineStr">
         <is>
@@ -10699,7 +10699,7 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>0.7589423972795546</v>
+        <v>1.316844151076587</v>
       </c>
       <c r="D395" t="inlineStr">
         <is>
@@ -10725,7 +10725,7 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>0.8147841333362914</v>
+        <v>1.111671961150397</v>
       </c>
       <c r="D396" t="inlineStr">
         <is>
@@ -10751,7 +10751,7 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>0.7192066470298464</v>
+        <v>1.191423360700792</v>
       </c>
       <c r="D397" t="inlineStr">
         <is>
@@ -10777,7 +10777,7 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>0.4992493520346758</v>
+        <v>1.078876114551234</v>
       </c>
       <c r="D398" t="inlineStr">
         <is>
@@ -10803,7 +10803,7 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>0.5130328831896311</v>
+        <v>0.7822924343198053</v>
       </c>
       <c r="D399" t="inlineStr">
         <is>
@@ -10829,7 +10829,7 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>0.5009602595390691</v>
+        <v>0.8023666826813944</v>
       </c>
       <c r="D400" t="inlineStr">
         <is>
@@ -10855,7 +10855,7 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>0.5682892572801094</v>
+        <v>1.306622699698165</v>
       </c>
       <c r="D401" t="inlineStr">
         <is>
@@ -10881,7 +10881,7 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>0.007613741441063618</v>
+        <v>1.085710095892315</v>
       </c>
       <c r="D402" t="inlineStr">
         <is>
@@ -10907,7 +10907,7 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>0.6486823819379056</v>
+        <v>1.049407807327577</v>
       </c>
       <c r="D403" t="inlineStr">
         <is>
@@ -10933,7 +10933,7 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>0.5101616541174289</v>
+        <v>0.8155656963122825</v>
       </c>
       <c r="D404" t="inlineStr">
         <is>
@@ -10959,7 +10959,7 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>0.8174811079357933</v>
+        <v>1.115281131367188</v>
       </c>
       <c r="D405" t="inlineStr">
         <is>
@@ -10985,7 +10985,7 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>0.4734936876686381</v>
+        <v>0.6938410490489123</v>
       </c>
       <c r="D406" t="inlineStr">
         <is>
@@ -11011,7 +11011,7 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>0.5828442855524216</v>
+        <v>0.8214071023393741</v>
       </c>
       <c r="D407" t="inlineStr">
         <is>
@@ -11037,7 +11037,7 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>0.7024307196037441</v>
+        <v>1.165340586769594</v>
       </c>
       <c r="D408" t="inlineStr">
         <is>
@@ -11063,7 +11063,7 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>0.7672000148430473</v>
+        <v>1.328896734761429</v>
       </c>
       <c r="D409" t="inlineStr">
         <is>
@@ -11089,7 +11089,7 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>0.823304539253079</v>
+        <v>1.12265500806447</v>
       </c>
       <c r="D410" t="inlineStr">
         <is>
@@ -11115,7 +11115,7 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>1.366474630683818</v>
+        <v>1.383283339117241</v>
       </c>
       <c r="D411" t="inlineStr">
         <is>
@@ -11141,7 +11141,7 @@
         </is>
       </c>
       <c r="C412" t="n">
-        <v>0.6791807100370785</v>
+        <v>1.069190500093204</v>
       </c>
       <c r="D412" t="inlineStr">
         <is>
@@ -11167,7 +11167,7 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>0.6127904367062095</v>
+        <v>0.9707834229449559</v>
       </c>
       <c r="D413" t="inlineStr">
         <is>
@@ -11193,7 +11193,7 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>0.5592346891373322</v>
+        <v>0.8581254374774394</v>
       </c>
       <c r="D414" t="inlineStr">
         <is>
@@ -11219,7 +11219,7 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>0.5847091536767084</v>
+        <v>0.8238060149574141</v>
       </c>
       <c r="D415" t="inlineStr">
         <is>
@@ -11245,7 +11245,7 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>0.6224010298192296</v>
+        <v>0.9137001346922736</v>
       </c>
       <c r="D416" t="inlineStr">
         <is>
@@ -11271,7 +11271,7 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>0.5757773729070758</v>
+        <v>0.9040766917682419</v>
       </c>
       <c r="D417" t="inlineStr">
         <is>
@@ -11297,7 +11297,7 @@
         </is>
       </c>
       <c r="C418" t="n">
-        <v>0.4920669035195493</v>
+        <v>1.069671142063382</v>
       </c>
       <c r="D418" t="inlineStr">
         <is>
@@ -11323,7 +11323,7 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>0.5664207190010178</v>
+        <v>0.9005175094443117</v>
       </c>
       <c r="D419" t="inlineStr">
         <is>
@@ -11349,7 +11349,7 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>0.400997819075796</v>
+        <v>0.4093440614403802</v>
       </c>
       <c r="D420" t="inlineStr">
         <is>
@@ -11375,7 +11375,7 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>0.6772781497403375</v>
+        <v>1.064232031979684</v>
       </c>
       <c r="D421" t="inlineStr">
         <is>
@@ -11401,7 +11401,7 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>0.7666973094203159</v>
+        <v>1.103047782530701</v>
       </c>
       <c r="D422" t="inlineStr">
         <is>
@@ -11427,7 +11427,7 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>0.7039202076343845</v>
+        <v>1.167365241737782</v>
       </c>
       <c r="D423" t="inlineStr">
         <is>
@@ -11453,7 +11453,7 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>0.8059081156734713</v>
+        <v>0.9814441665795927</v>
       </c>
       <c r="D424" t="inlineStr">
         <is>
@@ -11479,7 +11479,7 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>0.6717655979628574</v>
+        <v>1.056287246266585</v>
       </c>
       <c r="D425" t="inlineStr">
         <is>
@@ -11505,7 +11505,7 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>0.552166259362216</v>
+        <v>0.8871422948940501</v>
       </c>
       <c r="D426" t="inlineStr">
         <is>
@@ -11531,7 +11531,7 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>0.5069351115536067</v>
+        <v>0.877653073587546</v>
       </c>
       <c r="D427" t="inlineStr">
         <is>
@@ -11557,7 +11557,7 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>0.6468054111593382</v>
+        <v>1.095362611778106</v>
       </c>
       <c r="D428" t="inlineStr">
         <is>
@@ -11583,7 +11583,7 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>0.513511403912852</v>
+        <v>0.8604093657647406</v>
       </c>
       <c r="D429" t="inlineStr">
         <is>
@@ -11609,7 +11609,7 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>0.508203755433044</v>
+        <v>0.8735872506309847</v>
       </c>
       <c r="D430" t="inlineStr">
         <is>
@@ -11635,7 +11635,7 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>0.508203755433044</v>
+        <v>0.8735872506309847</v>
       </c>
       <c r="D431" t="inlineStr">
         <is>
@@ -11661,7 +11661,7 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>0.6149141909129613</v>
+        <v>0.9716635923413418</v>
       </c>
       <c r="D432" t="inlineStr">
         <is>
@@ -11687,7 +11687,7 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>0.2945878436566248</v>
+        <v>1.382873000608318</v>
       </c>
       <c r="D433" t="inlineStr">
         <is>
@@ -11713,7 +11713,7 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>0.5794555705164132</v>
+        <v>0.9830701586770633</v>
       </c>
       <c r="D434" t="inlineStr">
         <is>
@@ -11739,7 +11739,7 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>0.8135428052650958</v>
+        <v>0.8241594161382686</v>
       </c>
       <c r="D435" t="inlineStr">
         <is>
@@ -11765,7 +11765,7 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>0.7668328600915374</v>
+        <v>0.9140709783612474</v>
       </c>
       <c r="D436" t="inlineStr">
         <is>
@@ -11791,7 +11791,7 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>0.5576546773787037</v>
+        <v>1.078308539597659</v>
       </c>
       <c r="D437" t="inlineStr">
         <is>
@@ -11817,7 +11817,7 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>0.8130998760689292</v>
+        <v>0.9900565051540713</v>
       </c>
       <c r="D438" t="inlineStr">
         <is>
@@ -11843,7 +11843,7 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>0.7664013529928823</v>
+        <v>1.102652809700569</v>
       </c>
       <c r="D439" t="inlineStr">
         <is>
@@ -11869,7 +11869,7 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>0.8224804914482647</v>
+        <v>1.315353527948743</v>
       </c>
       <c r="D440" t="inlineStr">
         <is>
@@ -11895,7 +11895,7 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>0.6784218748159341</v>
+        <v>1.065225681702834</v>
       </c>
       <c r="D441" t="inlineStr">
         <is>
@@ -11921,7 +11921,7 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>0.7359084355037959</v>
+        <v>0.9635767327337086</v>
       </c>
       <c r="D442" t="inlineStr">
         <is>
@@ -11947,7 +11947,7 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>0.6047467664172371</v>
+        <v>1.037740988277038</v>
       </c>
       <c r="D443" t="inlineStr">
         <is>
@@ -11973,7 +11973,7 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>0.7673235690171576</v>
+        <v>1.103874616125087</v>
       </c>
       <c r="D444" t="inlineStr">
         <is>
@@ -11999,7 +11999,7 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>0.8234320200919443</v>
+        <v>1.316699068736741</v>
       </c>
       <c r="D445" t="inlineStr">
         <is>
@@ -12025,7 +12025,7 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>0.6045025645922981</v>
+        <v>0.958535990820544</v>
       </c>
       <c r="D446" t="inlineStr">
         <is>
@@ -12051,7 +12051,7 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>0.566416338244202</v>
+        <v>1.308823887823753</v>
       </c>
       <c r="D447" t="inlineStr">
         <is>
@@ -12077,7 +12077,7 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>0.5208358443496358</v>
+        <v>1.104364738837706</v>
       </c>
       <c r="D448" t="inlineStr">
         <is>
@@ -12103,7 +12103,7 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>0.5748949320304265</v>
+        <v>0.9430872121692568</v>
       </c>
       <c r="D449" t="inlineStr">
         <is>
@@ -12129,7 +12129,7 @@
         </is>
       </c>
       <c r="C450" t="n">
-        <v>0.518390054440141</v>
+        <v>1.004112965841077</v>
       </c>
       <c r="D450" t="inlineStr">
         <is>
@@ -12155,7 +12155,7 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>0.5852161982716318</v>
+        <v>0.9909718761806159</v>
       </c>
       <c r="D451" t="inlineStr">
         <is>
@@ -12181,7 +12181,7 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>0.5839323819542704</v>
+        <v>0.822781614158685</v>
       </c>
       <c r="D452" t="inlineStr">
         <is>
@@ -12207,7 +12207,7 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>0.5750049862126619</v>
+        <v>0.9030071338759323</v>
       </c>
       <c r="D453" t="inlineStr">
         <is>
@@ -12233,7 +12233,7 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>0.7036011850547897</v>
+        <v>1.166975145422432</v>
       </c>
       <c r="D454" t="inlineStr">
         <is>
@@ -12259,7 +12259,7 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>0.5072053030554533</v>
+        <v>0.8566166842415504</v>
       </c>
       <c r="D455" t="inlineStr">
         <is>
@@ -12311,7 +12311,7 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>0.6245365357525244</v>
+        <v>0.9165131788909052</v>
       </c>
       <c r="D457" t="inlineStr">
         <is>
@@ -12337,7 +12337,7 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>0.7066803307396361</v>
+        <v>1.171380779405432</v>
       </c>
       <c r="D458" t="inlineStr">
         <is>
@@ -12363,7 +12363,7 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>0.6486162440032331</v>
+        <v>1.148045959020233</v>
       </c>
       <c r="D459" t="inlineStr">
         <is>
@@ -12389,7 +12389,7 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>0.5026768416881935</v>
+        <v>0.806067910936006</v>
       </c>
       <c r="D460" t="inlineStr">
         <is>
@@ -12415,7 +12415,7 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>0.6238273339291602</v>
+        <v>1.135141591450392</v>
       </c>
       <c r="D461" t="inlineStr">
         <is>
@@ -12441,7 +12441,7 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>0.5268423814820127</v>
+        <v>0.9002197389891996</v>
       </c>
       <c r="D462" t="inlineStr">
         <is>
@@ -12467,7 +12467,7 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>0.7839753467342502</v>
+        <v>1.173413819128643</v>
       </c>
       <c r="D463" t="inlineStr">
         <is>
@@ -12493,7 +12493,7 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>0.6733197574268317</v>
+        <v>1.061115285974553</v>
       </c>
       <c r="D464" t="inlineStr">
         <is>
@@ -12519,7 +12519,7 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>0.5507626904539298</v>
+        <v>0.9048165736872354</v>
       </c>
       <c r="D465" t="inlineStr">
         <is>
@@ -12545,7 +12545,7 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>0.5690403043224164</v>
+        <v>0.9340233692950888</v>
       </c>
       <c r="D466" t="inlineStr">
         <is>
@@ -12571,7 +12571,7 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>0.582159848769169</v>
+        <v>1.016268812725203</v>
       </c>
       <c r="D467" t="inlineStr">
         <is>
@@ -12597,7 +12597,7 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>0.7996331743497831</v>
+        <v>0.9744670698342591</v>
       </c>
       <c r="D468" t="inlineStr">
         <is>
@@ -12623,7 +12623,7 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>0.5350055538724104</v>
+        <v>0.8407016319724134</v>
       </c>
       <c r="D469" t="inlineStr">
         <is>
@@ -12649,7 +12649,7 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>0.5044246683515217</v>
+        <v>0.8093089943517654</v>
       </c>
       <c r="D470" t="inlineStr">
         <is>
@@ -12675,7 +12675,7 @@
         </is>
       </c>
       <c r="C471" t="n">
-        <v>0.4764899298871533</v>
+        <v>0.6978525031006638</v>
       </c>
       <c r="D471" t="inlineStr">
         <is>
@@ -12701,7 +12701,7 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>0.5900674537071842</v>
+        <v>1.026309217954979</v>
       </c>
       <c r="D472" t="inlineStr">
         <is>
@@ -12727,7 +12727,7 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>0.3981447055847172</v>
+        <v>0.406950876107914</v>
       </c>
       <c r="D473" t="inlineStr">
         <is>
@@ -12753,7 +12753,7 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>0.5416699351132422</v>
+        <v>0.8811088670264807</v>
       </c>
       <c r="D474" t="inlineStr">
         <is>
@@ -12779,7 +12779,7 @@
         </is>
       </c>
       <c r="C475" t="n">
-        <v>0.9254943261036076</v>
+        <v>1.26867825078507</v>
       </c>
       <c r="D475" t="inlineStr">
         <is>
@@ -12805,7 +12805,7 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>0.534692114471275</v>
+        <v>0.8937474754957208</v>
       </c>
       <c r="D476" t="inlineStr">
         <is>
@@ -12831,7 +12831,7 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>0.5809953425792205</v>
+        <v>0.8189774297528674</v>
       </c>
       <c r="D477" t="inlineStr">
         <is>
@@ -12857,7 +12857,7 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>0.7004417292196995</v>
+        <v>1.162450975382636</v>
       </c>
       <c r="D478" t="inlineStr">
         <is>
@@ -12883,7 +12883,7 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>0.6762254408844949</v>
+        <v>1.065034597790177</v>
       </c>
       <c r="D479" t="inlineStr">
         <is>
@@ -12909,7 +12909,7 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>0.8001272925368239</v>
+        <v>1.655545036729936</v>
       </c>
       <c r="D480" t="inlineStr">
         <is>
@@ -12935,7 +12935,7 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>0.7251307506894639</v>
+        <v>1.192174635370317</v>
       </c>
       <c r="D481" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Preprocessing text as Class
</commit_message>
<xml_diff>
--- a/src/results/kl_content_vs_domain.xlsx
+++ b/src/results/kl_content_vs_domain.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -863,11 +863,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1.309345107064612</v>
+        <v>1.051825159337061</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -889,11 +889,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.051825159337061</v>
+        <v>1.309345107064612</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -993,11 +993,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.32078453497408</v>
+        <v>1.061984453095498</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1019,11 +1019,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.061984453095498</v>
+        <v>1.32078453497408</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -2033,11 +2033,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.8973516234105906</v>
+        <v>1.149662857102538</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -2059,11 +2059,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1.149662857102538</v>
+        <v>0.8973516234105906</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -2137,11 +2137,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.8117268046484413</v>
+        <v>1.058689616851366</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -2163,11 +2163,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.8023308361177167</v>
+        <v>0.8117268046484413</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -2189,11 +2189,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1.058689616851366</v>
+        <v>0.8023308361177167</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -2553,11 +2553,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1.310307363760873</v>
+        <v>1.052679628979815</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2579,11 +2579,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1.052679628979815</v>
+        <v>1.310307363760873</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2787,11 +2787,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1.177096843518948</v>
+        <v>0.9354285654204095</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2813,11 +2813,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.9354285654204095</v>
+        <v>1.177096843518948</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2891,11 +2891,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Electricity</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.2885249267089345</v>
+        <v>1.004635220030704</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2917,11 +2917,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Electricity</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1.004635220030704</v>
+        <v>0.2885249267089345</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -3074,11 +3074,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1.084087129779844</v>
+        <v>1.046991585851753</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -3100,11 +3100,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1.046991585851753</v>
+        <v>1.084087129779844</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -3204,11 +3204,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Cloud Computing</t>
+          <t>Banking</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>0.003015071025280447</v>
+        <v>0.402040483774579</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -3230,11 +3230,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Banking</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0.402040483774579</v>
+        <v>1.164768315389567</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -3256,11 +3256,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Cloud Computing</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1.164768315389567</v>
+        <v>0.003015071025280447</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -3646,11 +3646,11 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1.082389595924046</v>
+        <v>1.045324440417545</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -3672,11 +3672,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1.045324440417545</v>
+        <v>1.082389595924046</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -3828,11 +3828,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1.312131528785209</v>
+        <v>0.9977525088168081</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -3854,11 +3854,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0.9977525088168081</v>
+        <v>1.312131528785209</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
@@ -4062,11 +4062,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>1.083222161725817</v>
+        <v>1.046142100548664</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
@@ -4088,11 +4088,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>1.046142100548664</v>
+        <v>1.083222161725817</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
@@ -4218,11 +4218,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1.309578869092147</v>
+        <v>1.052032734757469</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
@@ -4244,11 +4244,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>1.052032734757469</v>
+        <v>1.309578869092147</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
@@ -4479,11 +4479,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>1.082943039489161</v>
+        <v>1.045867975200999</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
@@ -4505,11 +4505,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>1.045867975200999</v>
+        <v>1.082943039489161</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
@@ -4557,11 +4557,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Electricity</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>0.2888858810129574</v>
+        <v>1.005197686377464</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
@@ -4583,11 +4583,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Electricity</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>1.005197686377464</v>
+        <v>0.2888858810129574</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
@@ -4687,11 +4687,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>0.9003023474705429</v>
+        <v>1.153008121267897</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>
@@ -4713,11 +4713,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>1.153008121267897</v>
+        <v>0.9003023474705429</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
@@ -4739,11 +4739,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1.290141852419778</v>
+        <v>1.034777040740063</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
@@ -4765,11 +4765,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1.08734780026408</v>
+        <v>1.290141852419778</v>
       </c>
       <c r="D167" t="inlineStr">
         <is>
@@ -4791,11 +4791,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>1.034777040740063</v>
+        <v>1.08734780026408</v>
       </c>
       <c r="D168" t="inlineStr">
         <is>
@@ -4843,11 +4843,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>1.102577451388186</v>
+        <v>1.049620302549755</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
@@ -4869,11 +4869,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>1.049620302549755</v>
+        <v>1.102577451388186</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
@@ -5131,11 +5131,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>1.082468672815592</v>
+        <v>1.045402101449318</v>
       </c>
       <c r="D181" t="inlineStr">
         <is>
@@ -5157,11 +5157,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1.045402101449318</v>
+        <v>1.082468672815592</v>
       </c>
       <c r="D182" t="inlineStr">
         <is>
@@ -5235,11 +5235,11 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>0.8082442268551389</v>
+        <v>1.054868618009125</v>
       </c>
       <c r="D185" t="inlineStr">
         <is>
@@ -5261,11 +5261,11 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>0.7988463550005407</v>
+        <v>0.8082442268551389</v>
       </c>
       <c r="D186" t="inlineStr">
         <is>
@@ -5287,11 +5287,11 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>1.054868618009125</v>
+        <v>0.7988463550005407</v>
       </c>
       <c r="D187" t="inlineStr">
         <is>
@@ -5755,11 +5755,11 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>DevOps</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>1.080289987075832</v>
+        <v>1.039247667390604</v>
       </c>
       <c r="D205" t="inlineStr">
         <is>
@@ -5781,11 +5781,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>DevOps</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>1.039247667390604</v>
+        <v>1.080289987075832</v>
       </c>
       <c r="D206" t="inlineStr">
         <is>
@@ -5989,11 +5989,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>1.294946667666711</v>
+        <v>1.047030124807407</v>
       </c>
       <c r="D214" t="inlineStr">
         <is>
@@ -6015,11 +6015,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>1.047030124807407</v>
+        <v>1.294946667666711</v>
       </c>
       <c r="D215" t="inlineStr">
         <is>
@@ -7679,11 +7679,11 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Hardware</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>0.6905856838873534</v>
+        <v>1.049237009245282</v>
       </c>
       <c r="D279" t="inlineStr">
         <is>
@@ -7705,11 +7705,11 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>1.049237009245282</v>
+        <v>0.6905856838873534</v>
       </c>
       <c r="D280" t="inlineStr">
         <is>
@@ -9031,11 +9031,11 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C331" t="n">
-        <v>1.086979311609661</v>
+        <v>0.9965912285912136</v>
       </c>
       <c r="D331" t="inlineStr">
         <is>
@@ -9057,11 +9057,11 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C332" t="n">
-        <v>0.9965912285912136</v>
+        <v>1.086979311609661</v>
       </c>
       <c r="D332" t="inlineStr">
         <is>
@@ -10227,11 +10227,11 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C377" t="n">
-        <v>1.099147923823703</v>
+        <v>1.046277668348691</v>
       </c>
       <c r="D377" t="inlineStr">
         <is>
@@ -10253,11 +10253,11 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C378" t="n">
-        <v>1.046277668348691</v>
+        <v>1.099147923823703</v>
       </c>
       <c r="D378" t="inlineStr">
         <is>
@@ -10305,11 +10305,11 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C380" t="n">
-        <v>1.010432249814712</v>
+        <v>1.064043360835601</v>
       </c>
       <c r="D380" t="inlineStr">
         <is>
@@ -10331,11 +10331,11 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C381" t="n">
-        <v>1.064043360835601</v>
+        <v>1.010432249814712</v>
       </c>
       <c r="D381" t="inlineStr">
         <is>
@@ -10357,11 +10357,11 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C382" t="n">
-        <v>1.314739329745646</v>
+        <v>1.056615399094345</v>
       </c>
       <c r="D382" t="inlineStr">
         <is>
@@ -10383,11 +10383,11 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C383" t="n">
-        <v>1.109754165537558</v>
+        <v>1.314739329745646</v>
       </c>
       <c r="D383" t="inlineStr">
         <is>
@@ -10409,11 +10409,11 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C384" t="n">
-        <v>1.056615399094345</v>
+        <v>1.109754165537558</v>
       </c>
       <c r="D384" t="inlineStr">
         <is>
@@ -10851,11 +10851,11 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C401" t="n">
-        <v>1.306622699698165</v>
+        <v>1.049407807327577</v>
       </c>
       <c r="D401" t="inlineStr">
         <is>
@@ -10877,11 +10877,11 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>Healthcare</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C402" t="n">
-        <v>1.085710095892315</v>
+        <v>1.306622699698165</v>
       </c>
       <c r="D402" t="inlineStr">
         <is>
@@ -10903,11 +10903,11 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Healthcare</t>
         </is>
       </c>
       <c r="C403" t="n">
-        <v>1.049407807327577</v>
+        <v>1.085710095892315</v>
       </c>
       <c r="D403" t="inlineStr">
         <is>
@@ -11059,11 +11059,11 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C409" t="n">
-        <v>1.328896734761429</v>
+        <v>1.12265500806447</v>
       </c>
       <c r="D409" t="inlineStr">
         <is>
@@ -11085,11 +11085,11 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C410" t="n">
-        <v>1.12265500806447</v>
+        <v>1.069190500093204</v>
       </c>
       <c r="D410" t="inlineStr">
         <is>
@@ -11111,11 +11111,11 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>Hardware</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C411" t="n">
-        <v>1.383283339117241</v>
+        <v>1.328896734761429</v>
       </c>
       <c r="D411" t="inlineStr">
         <is>
@@ -11137,11 +11137,11 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="C412" t="n">
-        <v>1.069190500093204</v>
+        <v>1.383283339117241</v>
       </c>
       <c r="D412" t="inlineStr">
         <is>
@@ -11345,11 +11345,11 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>DevOps</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C420" t="n">
-        <v>0.4093440614403802</v>
+        <v>1.064232031979684</v>
       </c>
       <c r="D420" t="inlineStr">
         <is>
@@ -11371,11 +11371,11 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>DevOps</t>
         </is>
       </c>
       <c r="C421" t="n">
-        <v>1.064232031979684</v>
+        <v>0.4093440614403802</v>
       </c>
       <c r="D421" t="inlineStr">
         <is>
@@ -11553,11 +11553,11 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C428" t="n">
-        <v>1.095362611778106</v>
+        <v>0.8604093657647406</v>
       </c>
       <c r="D428" t="inlineStr">
         <is>
@@ -11579,11 +11579,11 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C429" t="n">
-        <v>0.8604093657647406</v>
+        <v>1.095362611778106</v>
       </c>
       <c r="D429" t="inlineStr">
         <is>
@@ -11839,11 +11839,11 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C439" t="n">
-        <v>1.102652809700569</v>
+        <v>1.065225681702834</v>
       </c>
       <c r="D439" t="inlineStr">
         <is>
@@ -11865,11 +11865,11 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C440" t="n">
-        <v>1.315353527948743</v>
+        <v>1.102652809700569</v>
       </c>
       <c r="D440" t="inlineStr">
         <is>
@@ -11891,11 +11891,11 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C441" t="n">
-        <v>1.065225681702834</v>
+        <v>1.315353527948743</v>
       </c>
       <c r="D441" t="inlineStr">
         <is>
@@ -12203,11 +12203,11 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C453" t="n">
-        <v>0.9030071338759323</v>
+        <v>1.166975145422432</v>
       </c>
       <c r="D453" t="inlineStr">
         <is>
@@ -12229,11 +12229,11 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C454" t="n">
-        <v>1.166975145422432</v>
+        <v>0.9030071338759323</v>
       </c>
       <c r="D454" t="inlineStr">
         <is>
@@ -12281,11 +12281,11 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>Cybersecurity</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C456" t="n">
-        <v>0</v>
+        <v>1.171380779405432</v>
       </c>
       <c r="D456" t="inlineStr">
         <is>
@@ -12333,11 +12333,11 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Cybersecurity</t>
         </is>
       </c>
       <c r="C458" t="n">
-        <v>1.171380779405432</v>
+        <v>0</v>
       </c>
       <c r="D458" t="inlineStr">
         <is>
@@ -12749,11 +12749,11 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C474" t="n">
-        <v>0.8811088670264807</v>
+        <v>1.26867825078507</v>
       </c>
       <c r="D474" t="inlineStr">
         <is>
@@ -12775,11 +12775,11 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C475" t="n">
-        <v>1.26867825078507</v>
+        <v>0.8811088670264807</v>
       </c>
       <c r="D475" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
LDA Hyper Tuning and KL calculations
</commit_message>
<xml_diff>
--- a/src/results/kl_content_vs_domain.xlsx
+++ b/src/results/kl_content_vs_domain.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9251511857443364</v>
+        <v>2.711978678030391</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7620693316763634</v>
+        <v>2.811086312970962</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.7842021244848932</v>
+        <v>4.095189441585775</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9805763031769701</v>
+        <v>3.788451271358973</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9228475915176979</v>
+        <v>3.525981028549917</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.7936678103050605</v>
+        <v>2.341822043970831</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -633,7 +633,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.021656157081017</v>
+        <v>4.424020729188626</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.202232665100662</v>
+        <v>5.245126235711101</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.195083493543541</v>
+        <v>5.194454554333685</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9048165736872354</v>
+        <v>3.143104182736366</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.879107954112294</v>
+        <v>2.968472608332762</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -763,7 +763,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1.003431014672907</v>
+        <v>3.905367147028273</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -789,7 +789,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.10254227034616</v>
+        <v>4.167934023936781</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.9454770549090322</v>
+        <v>3.477793352621579</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -837,11 +837,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1.655622795138359</v>
+        <v>3.597212426864761</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -863,11 +863,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1.051825159337061</v>
+        <v>3.039860480908064</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -893,7 +893,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.309345107064612</v>
+        <v>3.7021158170832</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -919,7 +919,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.078862827749338</v>
+        <v>4.976128255929501</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.81612081962609</v>
+        <v>2.606996790034425</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.7725947570821188</v>
+        <v>3.53082817950725</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.061984453095498</v>
+        <v>3.681063449567651</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1023,7 +1023,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.32078453497408</v>
+        <v>5.754468870631289</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.7658686418432765</v>
+        <v>2.271028857805698</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.158926839087477</v>
+        <v>4.682608470168031</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1097,11 +1097,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.8923965870319139</v>
+        <v>2.985317840491363</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1123,11 +1123,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.8828807322248121</v>
+        <v>3.674979831390265</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.7961545396071323</v>
+        <v>4.644235257846269</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1179,7 +1179,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.7940398241272142</v>
+        <v>2.34293571944496</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1205,7 +1205,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.9763419090948953</v>
+        <v>3.259461633739601</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1.088159863689639</v>
+        <v>3.359509940780391</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.8093659912769549</v>
+        <v>2.597575832410767</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1283,7 +1283,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.8097386869533613</v>
+        <v>4.053483233114857</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1309,7 +1309,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.8002194508143495</v>
+        <v>3.004663560739919</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1331,11 +1331,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.8045413470862837</v>
+        <v>2.987345390929563</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1357,11 +1357,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.8839604572400914</v>
+        <v>3.021547465853074</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.5163440213014413</v>
+        <v>1.723702701202609</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1413,7 +1413,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.958535990820544</v>
+        <v>3.355555361901345</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1439,7 +1439,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1.162657416639946</v>
+        <v>3.68424227249903</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.780416014936605</v>
+        <v>4.085025941823573</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1491,7 +1491,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>-0.009328921433373671</v>
+        <v>2.939517435372488</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1.152525195679933</v>
+        <v>5.352952274063424</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1543,7 +1543,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.9736341010902606</v>
+        <v>3.259957067061348</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.297472128273978</v>
+        <v>3.007193096895661</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1595,7 +1595,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.9230993929333375</v>
+        <v>4.724886495544438</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1617,11 +1617,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.9770271529592774</v>
+        <v>3.015775862538224</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1643,11 +1643,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1.300188020951307</v>
+        <v>3.050461426771327</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1673,7 +1673,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.546153676316226</v>
+        <v>5.771629922421908</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1699,7 +1699,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.20609419516364</v>
+        <v>5.471935055275102</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.019139453594172</v>
+        <v>4.20276988500293</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1751,7 +1751,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1.196628386353387</v>
+        <v>4.66983804451761</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.8406185143355298</v>
+        <v>3.357183674881658</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1.161778438445792</v>
+        <v>4.239917986765248</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1829,7 +1829,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.8019126382143702</v>
+        <v>2.587425524030488</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1855,7 +1855,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1.19045678195221</v>
+        <v>5.162069170945258</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1881,7 +1881,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1.64406325608195</v>
+        <v>3.009224957805241</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1.299300129651006</v>
+        <v>3.661319754448255</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.8060291675244182</v>
+        <v>3.363410551772938</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1959,7 +1959,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.9968093941272378</v>
+        <v>5.384878808790114</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1985,7 +1985,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.8160782051549252</v>
+        <v>2.606859326075734</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -2007,11 +2007,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.808228217767328</v>
+        <v>3.592197736919162</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -2033,11 +2033,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1.149662857102538</v>
+        <v>3.035937121254685</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -2063,7 +2063,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.8973516234105906</v>
+        <v>3.696889521089056</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1.371301553812185</v>
+        <v>1.977863906900977</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -2115,7 +2115,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.8979241089680022</v>
+        <v>3.668642666771185</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -2137,11 +2137,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1.058689616851366</v>
+        <v>4.144999753578629</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -2163,11 +2163,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.8117268046484413</v>
+        <v>5.186661523136146</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -2189,11 +2189,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.8023308361177167</v>
+        <v>3.58027399992297</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -2219,7 +2219,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.9597311102219686</v>
+        <v>3.901629326130327</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -2245,7 +2245,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.793655383802047</v>
+        <v>4.556104016270843</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -2271,7 +2271,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.8820544615209158</v>
+        <v>3.589826023657684</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -2297,7 +2297,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.9002505895642162</v>
+        <v>4.123937244634946</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -2319,11 +2319,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1.65331287479124</v>
+        <v>4.170539772886846</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -2345,11 +2345,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1.103010743362235</v>
+        <v>5.965368039601065</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -2375,7 +2375,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.144124984441628</v>
+        <v>5.114413432032268</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -2397,11 +2397,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.7992675294739581</v>
+        <v>4.192957180144703</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2423,11 +2423,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.87845264203492</v>
+        <v>4.597277769130899</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.7977031503880849</v>
+        <v>2.353202152215462</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2479,7 +2479,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1.004918637784497</v>
+        <v>4.049145415627207</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2505,7 +2505,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.8128335718637812</v>
+        <v>2.602445925959741</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2527,11 +2527,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1.656729989157039</v>
+        <v>3.62149523725919</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2553,11 +2553,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1.052679628979815</v>
+        <v>3.254535006844541</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2583,7 +2583,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1.310307363760873</v>
+        <v>3.354361417925618</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2609,7 +2609,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.9736341010902606</v>
+        <v>3.259957067061348</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2635,7 +2635,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1.191739326397291</v>
+        <v>4.189269835545515</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2661,7 +2661,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0.9133102250669155</v>
+        <v>2.676083942172715</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2687,7 +2687,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.7978591721836809</v>
+        <v>2.353562615834209</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2713,7 +2713,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.8027227852954837</v>
+        <v>2.658205896253776</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2739,7 +2739,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.9953481725579773</v>
+        <v>2.708471792257142</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2765,7 +2765,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.9985257383160193</v>
+        <v>3.699837088062662</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2787,11 +2787,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.9354285654204095</v>
+        <v>4.593114743277579</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2813,11 +2813,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1.177096843518948</v>
+        <v>3.481474445188781</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2843,7 +2843,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1.145872458093022</v>
+        <v>4.155473715078871</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -2869,7 +2869,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1.102173543057682</v>
+        <v>3.415882744397522</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2891,11 +2891,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Electricity</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1.004635220030704</v>
+        <v>1.996257051752005</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2917,11 +2917,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Electricity</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.2885249267089345</v>
+        <v>3.675472453478736</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -2947,7 +2947,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0.8865023898254771</v>
+        <v>2.997413055752284</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2974,7 +2974,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.821578825130743</v>
+        <v>2.614956892436414</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -3000,7 +3000,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1.140922812366161</v>
+        <v>4.572446148629727</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -3026,7 +3026,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0.714503395830094</v>
+        <v>2.951311446820562</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -3048,11 +3048,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0.9724883674677001</v>
+        <v>3.609204510969096</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -3074,11 +3074,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1.046991585851753</v>
+        <v>3.244007597290495</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -3104,7 +3104,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1.084087129779844</v>
+        <v>3.343360140985501</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -3130,7 +3130,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0.9005245002959414</v>
+        <v>3.621214128004835</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -3156,7 +3156,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>0.7994926286410695</v>
+        <v>2.932772137822475</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0.9598427629497396</v>
+        <v>3.901501855848593</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -3204,11 +3204,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Banking</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>0.402040483774579</v>
+        <v>5.444641413076798</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -3230,11 +3230,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Banking</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1.164768315389567</v>
+        <v>2.984714230296576</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -3260,7 +3260,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>0.003015071025280447</v>
+        <v>1.494360333755123</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -3286,7 +3286,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>0.3949164317674301</v>
+        <v>2.950872346255414</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -3312,7 +3312,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1.016867235342934</v>
+        <v>3.584316802803488</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>0.787535684465967</v>
+        <v>4.104745120120812</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -3364,7 +3364,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0.9736341010902606</v>
+        <v>3.259957067061348</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -3390,7 +3390,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>0.7936678103050605</v>
+        <v>2.341822043970831</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -3416,7 +3416,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1.19508138732885</v>
+        <v>5.194463642361002</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0.8856880781593204</v>
+        <v>3.607767692056407</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -3464,11 +3464,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1.309312010068817</v>
+        <v>4.179840760701252</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -3490,11 +3490,11 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1.104809434058442</v>
+        <v>5.666165719188609</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -3520,7 +3520,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0.8130099040738472</v>
+        <v>2.602748266818794</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
@@ -3542,11 +3542,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1.000933600989995</v>
+        <v>4.832460070785934</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
@@ -3568,11 +3568,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1.091519160643542</v>
+        <v>2.725624658281382</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -3594,11 +3594,11 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1.303090774223941</v>
+        <v>3.373047598392492</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -3620,11 +3620,11 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>0.9708822545719143</v>
+        <v>3.61848674480926</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -3646,11 +3646,11 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1.045324440417545</v>
+        <v>5.950091762950752</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -3676,7 +3676,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1.082389595924046</v>
+        <v>5.637780485036386</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -3702,7 +3702,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1.157126597218684</v>
+        <v>5.211063836929208</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -3728,7 +3728,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0.8021783106325583</v>
+        <v>2.587410869283717</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -3754,7 +3754,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>0.8402796965008181</v>
+        <v>3.097607837184779</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
@@ -3780,7 +3780,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1.003931981225926</v>
+        <v>3.89641894606736</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
@@ -3806,7 +3806,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0.8216396937944614</v>
+        <v>2.614761043796963</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
@@ -3832,7 +3832,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>0.9977525088168081</v>
+        <v>5.381695183074451</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -3858,7 +3858,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1.312131528785209</v>
+        <v>3.714212826434402</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
@@ -3884,7 +3884,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.9228475915176979</v>
+        <v>3.525981028549917</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
@@ -3910,7 +3910,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1.150365203900187</v>
+        <v>4.629615619449921</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -3936,7 +3936,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0.9026686090036761</v>
+        <v>4.138071233497964</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
@@ -3962,7 +3962,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1.090453557507115</v>
+        <v>4.071000928486096</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
@@ -3988,7 +3988,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>0.8159920862280736</v>
+        <v>2.606883057989851</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
@@ -4014,7 +4014,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>0.7842022986857551</v>
+        <v>4.095600281339792</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
@@ -4036,11 +4036,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>0.9716699779419523</v>
+        <v>3.605555356627584</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
@@ -4062,11 +4062,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>1.046142100548664</v>
+        <v>3.240881718168308</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>1.083222161725817</v>
+        <v>3.34009363337625</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
@@ -4118,7 +4118,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0.8859548301057605</v>
+        <v>2.029798318117932</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
@@ -4144,7 +4144,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>0.7931090934313132</v>
+        <v>2.14110609791518</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
@@ -4170,7 +4170,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>0.7726264619423427</v>
+        <v>3.899925652309328</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
@@ -4192,11 +4192,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>1.655891769342095</v>
+        <v>3.618736055659375</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
@@ -4218,11 +4218,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1.052032734757469</v>
+        <v>3.252171794374241</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
@@ -4248,7 +4248,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>1.309578869092147</v>
+        <v>3.351891796572891</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
@@ -4274,7 +4274,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>1.153413220353133</v>
+        <v>4.648208157405881</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
@@ -4300,7 +4300,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>1.059995385067475</v>
+        <v>2.329600833067359</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
@@ -4326,7 +4326,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>0.8406185143355298</v>
+        <v>3.36206393899415</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
@@ -4352,7 +4352,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>0.783992099392521</v>
+        <v>4.094627978867123</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>1.202466806333066</v>
+        <v>4.244811025261351</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
@@ -4404,7 +4404,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>1.304865447552159</v>
+        <v>3.68374911371534</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
@@ -4431,7 +4431,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>1.102883248215501</v>
+        <v>4.170243596783871</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
@@ -4453,11 +4453,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>0.9714058884172551</v>
+        <v>3.620348783041</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
@@ -4479,11 +4479,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>1.045867975200999</v>
+        <v>5.953823965023012</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
@@ -4509,7 +4509,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>1.082943039489161</v>
+        <v>5.641247930694018</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
@@ -4535,7 +4535,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>1.190825161130525</v>
+        <v>4.184306509600763</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
@@ -4557,11 +4557,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Electricity</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>1.005197686377464</v>
+        <v>2.000413716224249</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
@@ -4583,11 +4583,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Electricity</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>0.2888858810129574</v>
+        <v>5.453440394502685</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
@@ -4613,7 +4613,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0.8159083644324522</v>
+        <v>2.606831587820099</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
@@ -4639,7 +4639,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>1.107894385802455</v>
+        <v>3.016547471071009</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
@@ -4661,11 +4661,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>0.8110395791943045</v>
+        <v>3.60685750545191</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
@@ -4687,11 +4687,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>1.153008121267897</v>
+        <v>3.04740562910214</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>
@@ -4717,7 +4717,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>0.9003023474705429</v>
+        <v>3.712168101571638</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
@@ -4739,11 +4739,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1.034777040740063</v>
+        <v>2.94776620688222</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
@@ -4765,11 +4765,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1.290141852419778</v>
+        <v>3.522401995843224</v>
       </c>
       <c r="D167" t="inlineStr">
         <is>
@@ -4791,11 +4791,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>1.08734780026408</v>
+        <v>3.624156417817094</v>
       </c>
       <c r="D168" t="inlineStr">
         <is>
@@ -4821,7 +4821,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>0.9673891174138604</v>
+        <v>3.557014440800374</v>
       </c>
       <c r="D169" t="inlineStr">
         <is>
@@ -4843,11 +4843,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>1.049620302549755</v>
+        <v>2.998804899888139</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
@@ -4869,11 +4869,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>1.102577451388186</v>
+        <v>3.588701688868807</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
@@ -4900,7 +4900,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>0.9620680614896875</v>
+        <v>3.362540288211578</v>
       </c>
       <c r="D172" t="inlineStr">
         <is>
@@ -4927,7 +4927,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>1.192826672629859</v>
+        <v>4.636256294628171</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>0.8219952608780432</v>
+        <v>2.615071378084162</v>
       </c>
       <c r="D174" t="inlineStr">
         <is>
@@ -4979,7 +4979,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>0.909890661523359</v>
+        <v>2.664724887842877</v>
       </c>
       <c r="D175" t="inlineStr">
         <is>
@@ -5005,7 +5005,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>0.9005245002959414</v>
+        <v>3.621214128004835</v>
       </c>
       <c r="D176" t="inlineStr">
         <is>
@@ -5031,7 +5031,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>0.7866742383695804</v>
+        <v>2.913335717061498</v>
       </c>
       <c r="D177" t="inlineStr">
         <is>
@@ -5057,7 +5057,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>0.8187628032829893</v>
+        <v>4.741916515047127</v>
       </c>
       <c r="D178" t="inlineStr">
         <is>
@@ -5083,7 +5083,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>1.096984294537662</v>
+        <v>2.615347097818801</v>
       </c>
       <c r="D179" t="inlineStr">
         <is>
@@ -5105,11 +5105,11 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>0.9709570719707696</v>
+        <v>3.618382889995565</v>
       </c>
       <c r="D180" t="inlineStr">
         <is>
@@ -5131,11 +5131,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>1.045402101449318</v>
+        <v>5.949883610554298</v>
       </c>
       <c r="D181" t="inlineStr">
         <is>
@@ -5161,7 +5161,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1.082468672815592</v>
+        <v>5.637587097553423</v>
       </c>
       <c r="D182" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1.197423670884637</v>
+        <v>4.675474101569423</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
@@ -5213,7 +5213,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>0.9226375361752605</v>
+        <v>3.206565117306952</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
@@ -5235,11 +5235,11 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1.054868618009125</v>
+        <v>2.931920996799751</v>
       </c>
       <c r="D185" t="inlineStr">
         <is>
@@ -5261,11 +5261,11 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>0.8082442268551389</v>
+        <v>3.501834769147191</v>
       </c>
       <c r="D186" t="inlineStr">
         <is>
@@ -5287,11 +5287,11 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>0.7988463550005407</v>
+        <v>3.602726426861746</v>
       </c>
       <c r="D187" t="inlineStr">
         <is>
@@ -5317,7 +5317,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>0.2783237528758306</v>
+        <v>1.969462346184545</v>
       </c>
       <c r="D188" t="inlineStr">
         <is>
@@ -5343,7 +5343,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>0.9047861053116246</v>
+        <v>3.717557239793742</v>
       </c>
       <c r="D189" t="inlineStr">
         <is>
@@ -5369,7 +5369,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>0.81806566225674</v>
+        <v>4.735706596535085</v>
       </c>
       <c r="D190" t="inlineStr">
         <is>
@@ -5395,7 +5395,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>0.4023500350798024</v>
+        <v>1.494776924448729</v>
       </c>
       <c r="D191" t="inlineStr">
         <is>
@@ -5421,7 +5421,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>0.8406185143355298</v>
+        <v>3.357183674881658</v>
       </c>
       <c r="D192" t="inlineStr">
         <is>
@@ -5447,7 +5447,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>0.958535990820544</v>
+        <v>3.355555361901345</v>
       </c>
       <c r="D193" t="inlineStr">
         <is>
@@ -5473,7 +5473,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>1.285794488867437</v>
+        <v>4.204290789334585</v>
       </c>
       <c r="D194" t="inlineStr">
         <is>
@@ -5499,7 +5499,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>0.9739088391417525</v>
+        <v>4.668531407772891</v>
       </c>
       <c r="D195" t="inlineStr">
         <is>
@@ -5525,7 +5525,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>0.7933492809089383</v>
+        <v>2.341547991209719</v>
       </c>
       <c r="D196" t="inlineStr">
         <is>
@@ -5551,7 +5551,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>0.8437139661855002</v>
+        <v>3.198357933822101</v>
       </c>
       <c r="D197" t="inlineStr">
         <is>
@@ -5577,7 +5577,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>0.7717237840964803</v>
+        <v>3.618921441739625</v>
       </c>
       <c r="D198" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>0.904715844874459</v>
+        <v>4.150457196141846</v>
       </c>
       <c r="D199" t="inlineStr">
         <is>
@@ -5629,7 +5629,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>1.191936519506979</v>
+        <v>5.173443819229684</v>
       </c>
       <c r="D200" t="inlineStr">
         <is>
@@ -5655,7 +5655,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>0.9469300328248199</v>
+        <v>3.472760292405569</v>
       </c>
       <c r="D201" t="inlineStr">
         <is>
@@ -5681,7 +5681,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>0.7906259106340428</v>
+        <v>4.113028441293737</v>
       </c>
       <c r="D202" t="inlineStr">
         <is>
@@ -5707,7 +5707,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>0.9612751316359143</v>
+        <v>3.700196332652877</v>
       </c>
       <c r="D203" t="inlineStr">
         <is>
@@ -5733,7 +5733,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>1.189805315787567</v>
+        <v>4.629584586133598</v>
       </c>
       <c r="D204" t="inlineStr">
         <is>
@@ -5759,7 +5759,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>1.039247667390604</v>
+        <v>3.578397050518015</v>
       </c>
       <c r="D205" t="inlineStr">
         <is>
@@ -5785,7 +5785,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>1.080289987075832</v>
+        <v>2.939338043295907</v>
       </c>
       <c r="D206" t="inlineStr">
         <is>
@@ -5811,7 +5811,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>0.98741648837243</v>
+        <v>3.593269604306236</v>
       </c>
       <c r="D207" t="inlineStr">
         <is>
@@ -5837,7 +5837,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>0.7838171772697139</v>
+        <v>2.316424329988281</v>
       </c>
       <c r="D208" t="inlineStr">
         <is>
@@ -5863,7 +5863,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>0.9053906674357205</v>
+        <v>2.732516097666648</v>
       </c>
       <c r="D209" t="inlineStr">
         <is>
@@ -5889,7 +5889,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>1.010574966033383</v>
+        <v>3.557200934528244</v>
       </c>
       <c r="D210" t="inlineStr">
         <is>
@@ -5915,7 +5915,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>0.9716635923413418</v>
+        <v>3.745783097423464</v>
       </c>
       <c r="D211" t="inlineStr">
         <is>
@@ -5941,7 +5941,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>1.183728486429264</v>
+        <v>4.147443662932175</v>
       </c>
       <c r="D212" t="inlineStr">
         <is>
@@ -5967,7 +5967,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>1.040350276124655</v>
+        <v>4.473398992690782</v>
       </c>
       <c r="D213" t="inlineStr">
         <is>
@@ -5989,11 +5989,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>1.047030124807407</v>
+        <v>2.999221436975841</v>
       </c>
       <c r="D214" t="inlineStr">
         <is>
@@ -6015,11 +6015,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>1.294946667666711</v>
+        <v>3.589243092099721</v>
       </c>
       <c r="D215" t="inlineStr">
         <is>
@@ -6045,7 +6045,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>0.9343678160062792</v>
+        <v>3.489041197247275</v>
       </c>
       <c r="D216" t="inlineStr">
         <is>
@@ -6071,7 +6071,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>0.9805763031769701</v>
+        <v>3.788451271358973</v>
       </c>
       <c r="D217" t="inlineStr">
         <is>
@@ -6097,7 +6097,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>0.8096937291822263</v>
+        <v>2.598197852716025</v>
       </c>
       <c r="D218" t="inlineStr">
         <is>
@@ -6123,7 +6123,7 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>0.8247297348223899</v>
+        <v>2.61892145939897</v>
       </c>
       <c r="D219" t="inlineStr">
         <is>
@@ -6149,7 +6149,7 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>0.9218615071990631</v>
+        <v>2.7017710835137</v>
       </c>
       <c r="D220" t="inlineStr">
         <is>
@@ -6175,7 +6175,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>1.045300624997171</v>
+        <v>4.991686905402128</v>
       </c>
       <c r="D221" t="inlineStr">
         <is>
@@ -6201,7 +6201,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>1.19847753556293</v>
+        <v>4.223374605296272</v>
       </c>
       <c r="D222" t="inlineStr">
         <is>
@@ -6227,7 +6227,7 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>0.8190686780079089</v>
+        <v>4.077997237262826</v>
       </c>
       <c r="D223" t="inlineStr">
         <is>
@@ -6253,7 +6253,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>0.9349921379667659</v>
+        <v>3.489966244665095</v>
       </c>
       <c r="D224" t="inlineStr">
         <is>
@@ -6279,7 +6279,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>0.801818688443401</v>
+        <v>2.587400794206121</v>
       </c>
       <c r="D225" t="inlineStr">
         <is>
@@ -6305,7 +6305,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>0.7838549960904776</v>
+        <v>2.316893276006442</v>
       </c>
       <c r="D226" t="inlineStr">
         <is>
@@ -6331,7 +6331,7 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>1.182327166446044</v>
+        <v>5.105452887390057</v>
       </c>
       <c r="D227" t="inlineStr">
         <is>
@@ -6357,7 +6357,7 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>1.161605015643351</v>
+        <v>4.699158818734517</v>
       </c>
       <c r="D228" t="inlineStr">
         <is>
@@ -6379,11 +6379,11 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>1.663130660002236</v>
+        <v>4.212958909348212</v>
       </c>
       <c r="D229" t="inlineStr">
         <is>
@@ -6405,11 +6405,11 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>1.110784904955627</v>
+        <v>6.03507902097005</v>
       </c>
       <c r="D230" t="inlineStr">
         <is>
@@ -6435,7 +6435,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>0.8852475101494343</v>
+        <v>3.606573091120666</v>
       </c>
       <c r="D231" t="inlineStr">
         <is>
@@ -6461,7 +6461,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>1.009453232784819</v>
+        <v>4.152690296247315</v>
       </c>
       <c r="D232" t="inlineStr">
         <is>
@@ -6487,7 +6487,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>1.182299727162589</v>
+        <v>5.105172628305542</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -6513,7 +6513,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>0.7485515355909331</v>
+        <v>2.987473977216064</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -6539,7 +6539,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>0.9035284669797958</v>
+        <v>3.061177540496788</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -6565,7 +6565,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>1.180540922939193</v>
+        <v>5.093466093824063</v>
       </c>
       <c r="D236" t="inlineStr">
         <is>
@@ -6591,7 +6591,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>1.17049186955002</v>
+        <v>4.75503565695636</v>
       </c>
       <c r="D237" t="inlineStr">
         <is>
@@ -6617,7 +6617,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>0.904961133294546</v>
+        <v>2.649079173705837</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
@@ -6643,7 +6643,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>0.8735872506309847</v>
+        <v>2.898662233460566</v>
       </c>
       <c r="D239" t="inlineStr">
         <is>
@@ -6669,7 +6669,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>0.8220602544230596</v>
+        <v>2.615158638954221</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>
@@ -6695,7 +6695,7 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>1.157822765181761</v>
+        <v>4.675997756300557</v>
       </c>
       <c r="D241" t="inlineStr">
         <is>
@@ -6721,7 +6721,7 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>0.8187712083289204</v>
+        <v>5.023731097373726</v>
       </c>
       <c r="D242" t="inlineStr">
         <is>
@@ -6747,7 +6747,7 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>0.9166075345436369</v>
+        <v>2.685318006345247</v>
       </c>
       <c r="D243" t="inlineStr">
         <is>
@@ -6773,7 +6773,7 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>0.901234518440594</v>
+        <v>2.637777468960611</v>
       </c>
       <c r="D244" t="inlineStr">
         <is>
@@ -6799,7 +6799,7 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>0.8097351777541896</v>
+        <v>2.598021998617728</v>
       </c>
       <c r="D245" t="inlineStr">
         <is>
@@ -6825,7 +6825,7 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>1.183779967035533</v>
+        <v>4.14769671091283</v>
       </c>
       <c r="D246" t="inlineStr">
         <is>
@@ -6851,7 +6851,7 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>0.9736341010902606</v>
+        <v>3.259957067061348</v>
       </c>
       <c r="D247" t="inlineStr">
         <is>
@@ -6877,7 +6877,7 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>0.9992578928547016</v>
+        <v>3.357419791724249</v>
       </c>
       <c r="D248" t="inlineStr">
         <is>
@@ -6903,7 +6903,7 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>1.296976663779622</v>
+        <v>3.005117202885903</v>
       </c>
       <c r="D249" t="inlineStr">
         <is>
@@ -6929,7 +6929,7 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>0.8248289664701212</v>
+        <v>2.619051664843498</v>
       </c>
       <c r="D250" t="inlineStr">
         <is>
@@ -6955,7 +6955,7 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>0.822007614376669</v>
+        <v>2.615087777896788</v>
       </c>
       <c r="D251" t="inlineStr">
         <is>
@@ -6981,7 +6981,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>0.8859548301057605</v>
+        <v>2.029798318117932</v>
       </c>
       <c r="D252" t="inlineStr">
         <is>
@@ -7007,7 +7007,7 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>0.6836071386768621</v>
+        <v>2.072556400942394</v>
       </c>
       <c r="D253" t="inlineStr">
         <is>
@@ -7033,7 +7033,7 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>0.9171012635629811</v>
+        <v>3.765588971135279</v>
       </c>
       <c r="D254" t="inlineStr">
         <is>
@@ -7059,7 +7059,7 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>0.006383140819778305</v>
+        <v>1.50229230678545</v>
       </c>
       <c r="D255" t="inlineStr">
         <is>
@@ -7085,7 +7085,7 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>1.084647289073029</v>
+        <v>3.345437850085732</v>
       </c>
       <c r="D256" t="inlineStr">
         <is>
@@ -7107,11 +7107,11 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>1.317788614706045</v>
+        <v>4.222451998610048</v>
       </c>
       <c r="D257" t="inlineStr">
         <is>
@@ -7133,11 +7133,11 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>1.112532527464772</v>
+        <v>5.731231512833478</v>
       </c>
       <c r="D258" t="inlineStr">
         <is>
@@ -7163,7 +7163,7 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>0.7664692548041706</v>
+        <v>2.909939165484229</v>
       </c>
       <c r="D259" t="inlineStr">
         <is>
@@ -7189,7 +7189,7 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>1.080308649558468</v>
+        <v>1.475441206519702</v>
       </c>
       <c r="D260" t="inlineStr">
         <is>
@@ -7215,7 +7215,7 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>1.202170835770731</v>
+        <v>4.243044992770677</v>
       </c>
       <c r="D261" t="inlineStr">
         <is>
@@ -7241,7 +7241,7 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>1.140067129806242</v>
+        <v>4.567926160007067</v>
       </c>
       <c r="D262" t="inlineStr">
         <is>
@@ -7267,7 +7267,7 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>1.138659808989161</v>
+        <v>3.581904730235753</v>
       </c>
       <c r="D263" t="inlineStr">
         <is>
@@ -7293,7 +7293,7 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>0.7888125846860762</v>
+        <v>2.329204471261485</v>
       </c>
       <c r="D264" t="inlineStr">
         <is>
@@ -7319,7 +7319,7 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>1.159653805646729</v>
+        <v>4.687298480222417</v>
       </c>
       <c r="D265" t="inlineStr">
         <is>
@@ -7345,7 +7345,7 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>0.8095296850537064</v>
+        <v>2.597937606260176</v>
       </c>
       <c r="D266" t="inlineStr">
         <is>
@@ -7371,7 +7371,7 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>1.091620561568922</v>
+        <v>3.373292488816401</v>
       </c>
       <c r="D267" t="inlineStr">
         <is>
@@ -7397,7 +7397,7 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>1.194325578929917</v>
+        <v>5.189709780950952</v>
       </c>
       <c r="D268" t="inlineStr">
         <is>
@@ -7423,7 +7423,7 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>1.100191201786831</v>
+        <v>5.044609277642346</v>
       </c>
       <c r="D269" t="inlineStr">
         <is>
@@ -7449,7 +7449,7 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>1.156267262962512</v>
+        <v>4.666422165645612</v>
       </c>
       <c r="D270" t="inlineStr">
         <is>
@@ -7475,7 +7475,7 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>0.8161271876364102</v>
+        <v>2.607301030886576</v>
       </c>
       <c r="D271" t="inlineStr">
         <is>
@@ -7501,7 +7501,7 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>1.041139135198765</v>
+        <v>4.474507413279904</v>
       </c>
       <c r="D272" t="inlineStr">
         <is>
@@ -7527,7 +7527,7 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>0.8893724982224133</v>
+        <v>3.008372529934013</v>
       </c>
       <c r="D273" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>0.8056253464069706</v>
+        <v>2.59308152118116</v>
       </c>
       <c r="D274" t="inlineStr">
         <is>
@@ -7579,7 +7579,7 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>0.8164495691285552</v>
+        <v>2.607419718533259</v>
       </c>
       <c r="D275" t="inlineStr">
         <is>
@@ -7605,7 +7605,7 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>0.7981955945459819</v>
+        <v>2.353809873750596</v>
       </c>
       <c r="D276" t="inlineStr">
         <is>
@@ -7631,7 +7631,7 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>0.8098260913854762</v>
+        <v>2.592971615827593</v>
       </c>
       <c r="D277" t="inlineStr">
         <is>
@@ -7657,7 +7657,7 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>1.297422262911572</v>
+        <v>4.797858860546123</v>
       </c>
       <c r="D278" t="inlineStr">
         <is>
@@ -7683,7 +7683,7 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>1.049237009245282</v>
+        <v>3.619159503783275</v>
       </c>
       <c r="D279" t="inlineStr">
         <is>
@@ -7709,7 +7709,7 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>0.6905856838873534</v>
+        <v>1.994282930077837</v>
       </c>
       <c r="D280" t="inlineStr">
         <is>
@@ -7735,7 +7735,7 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>1.003931981225926</v>
+        <v>3.89641894606736</v>
       </c>
       <c r="D281" t="inlineStr">
         <is>
@@ -7761,7 +7761,7 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>0.9107387317951309</v>
+        <v>3.733091835598265</v>
       </c>
       <c r="D282" t="inlineStr">
         <is>
@@ -7787,7 +7787,7 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>0.4045992360076677</v>
+        <v>1.498538147741945</v>
       </c>
       <c r="D283" t="inlineStr">
         <is>
@@ -7813,7 +7813,7 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>0.9494829025377663</v>
+        <v>2.872379882629405</v>
       </c>
       <c r="D284" t="inlineStr">
         <is>
@@ -7839,7 +7839,7 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>0.9228475915176979</v>
+        <v>3.525981028549917</v>
       </c>
       <c r="D285" t="inlineStr">
         <is>
@@ -7865,7 +7865,7 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>0.8846132081003446</v>
+        <v>2.932946609960803</v>
       </c>
       <c r="D286" t="inlineStr">
         <is>
@@ -7891,7 +7891,7 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>0.7485515355909331</v>
+        <v>2.987473977216064</v>
       </c>
       <c r="D287" t="inlineStr">
         <is>
@@ -7917,7 +7917,7 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>0.9812396747978469</v>
+        <v>3.789442118817522</v>
       </c>
       <c r="D288" t="inlineStr">
         <is>
@@ -7943,7 +7943,7 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>0.989738072531985</v>
+        <v>3.829327921147557</v>
       </c>
       <c r="D289" t="inlineStr">
         <is>
@@ -7969,7 +7969,7 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>1.161805099536567</v>
+        <v>4.24001178265268</v>
       </c>
       <c r="D290" t="inlineStr">
         <is>
@@ -7995,7 +7995,7 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>0.799965221053682</v>
+        <v>3.19129945316457</v>
       </c>
       <c r="D291" t="inlineStr">
         <is>
@@ -8021,7 +8021,7 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>1.161492035442104</v>
+        <v>4.698727592734974</v>
       </c>
       <c r="D292" t="inlineStr">
         <is>
@@ -8047,7 +8047,7 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>1.213746462992864</v>
+        <v>4.304732049075964</v>
       </c>
       <c r="D293" t="inlineStr">
         <is>
@@ -8073,7 +8073,7 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>0.7979124913723817</v>
+        <v>2.353348970742586</v>
       </c>
       <c r="D294" t="inlineStr">
         <is>
@@ -8099,7 +8099,7 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>0.77768632045761</v>
+        <v>2.301950804910139</v>
       </c>
       <c r="D295" t="inlineStr">
         <is>
@@ -8125,7 +8125,7 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>0.9647000843027527</v>
+        <v>2.923275993373967</v>
       </c>
       <c r="D296" t="inlineStr">
         <is>
@@ -8151,7 +8151,7 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>0.7933492809089383</v>
+        <v>2.341547991209719</v>
       </c>
       <c r="D297" t="inlineStr">
         <is>
@@ -8177,7 +8177,7 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>0.8097189976521512</v>
+        <v>2.597900474718702</v>
       </c>
       <c r="D298" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>0.9243621920393591</v>
+        <v>2.709681893946517</v>
       </c>
       <c r="D299" t="inlineStr">
         <is>
@@ -8229,7 +8229,7 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>0.904974404969567</v>
+        <v>2.649346202104921</v>
       </c>
       <c r="D300" t="inlineStr">
         <is>
@@ -8251,11 +8251,11 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>0.897140503265181</v>
+        <v>3.000901900879864</v>
       </c>
       <c r="D301" t="inlineStr">
         <is>
@@ -8277,11 +8277,11 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>0.8876006355793847</v>
+        <v>3.696086647184092</v>
       </c>
       <c r="D302" t="inlineStr">
         <is>
@@ -8303,11 +8303,11 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>1.092744516514538</v>
+        <v>4.841171063756216</v>
       </c>
       <c r="D303" t="inlineStr">
         <is>
@@ -8329,11 +8329,11 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>1.304440538171306</v>
+        <v>3.378275524558605</v>
       </c>
       <c r="D304" t="inlineStr">
         <is>
@@ -8359,7 +8359,7 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>1.070435198633322</v>
+        <v>2.353657853820323</v>
       </c>
       <c r="D305" t="inlineStr">
         <is>
@@ -8385,7 +8385,7 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>1.078851910309706</v>
+        <v>4.976850387520341</v>
       </c>
       <c r="D306" t="inlineStr">
         <is>
@@ -8411,7 +8411,7 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>1.188235858747638</v>
+        <v>3.529712361107113</v>
       </c>
       <c r="D307" t="inlineStr">
         <is>
@@ -8437,7 +8437,7 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>0.8165698000770351</v>
+        <v>2.607589284131392</v>
       </c>
       <c r="D308" t="inlineStr">
         <is>
@@ -8463,7 +8463,7 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>0.9164297500094949</v>
+        <v>2.684850350036473</v>
       </c>
       <c r="D309" t="inlineStr">
         <is>
@@ -8489,7 +8489,7 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>1.179304675031934</v>
+        <v>5.084911946218662</v>
       </c>
       <c r="D310" t="inlineStr">
         <is>
@@ -8515,7 +8515,7 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>1.19722019516806</v>
+        <v>4.216851561928433</v>
       </c>
       <c r="D311" t="inlineStr">
         <is>
@@ -8537,11 +8537,11 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>0.8876790204652035</v>
+        <v>4.191213645559353</v>
       </c>
       <c r="D312" t="inlineStr">
         <is>
@@ -8563,11 +8563,11 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C313" t="n">
-        <v>0.8781870767483215</v>
+        <v>3.617744372304838</v>
       </c>
       <c r="D313" t="inlineStr">
         <is>
@@ -8589,11 +8589,11 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C314" t="n">
-        <v>0.8863505060913084</v>
+        <v>4.183419598532057</v>
       </c>
       <c r="D314" t="inlineStr">
         <is>
@@ -8615,11 +8615,11 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C315" t="n">
-        <v>0.8768653016915404</v>
+        <v>3.611426388481375</v>
       </c>
       <c r="D315" t="inlineStr">
         <is>
@@ -8645,7 +8645,7 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>1.163253050824435</v>
+        <v>4.709545692842298</v>
       </c>
       <c r="D316" t="inlineStr">
         <is>
@@ -8671,7 +8671,7 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>1.164508235182245</v>
+        <v>4.718347457055737</v>
       </c>
       <c r="D317" t="inlineStr">
         <is>
@@ -8697,7 +8697,7 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>0.9114518428328982</v>
+        <v>2.669327153651593</v>
       </c>
       <c r="D318" t="inlineStr">
         <is>
@@ -8723,7 +8723,7 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>0.8989539024575023</v>
+        <v>3.673652339166176</v>
       </c>
       <c r="D319" t="inlineStr">
         <is>
@@ -8749,7 +8749,7 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>1.147991179603878</v>
+        <v>2.656915977828922</v>
       </c>
       <c r="D320" t="inlineStr">
         <is>
@@ -8775,7 +8775,7 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>0.9616363119716375</v>
+        <v>3.700152629316733</v>
       </c>
       <c r="D321" t="inlineStr">
         <is>
@@ -8801,7 +8801,7 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>1.145944945302291</v>
+        <v>4.602681356571948</v>
       </c>
       <c r="D322" t="inlineStr">
         <is>
@@ -8827,7 +8827,7 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>1.148526077313738</v>
+        <v>5.145844930319424</v>
       </c>
       <c r="D323" t="inlineStr">
         <is>
@@ -8853,7 +8853,7 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>1.145289764256723</v>
+        <v>4.1521037293303</v>
       </c>
       <c r="D324" t="inlineStr">
         <is>
@@ -8879,7 +8879,7 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>1.196160152881235</v>
+        <v>4.211124661988829</v>
       </c>
       <c r="D325" t="inlineStr">
         <is>
@@ -8905,7 +8905,7 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>0.8245390871344461</v>
+        <v>2.619042364184185</v>
       </c>
       <c r="D326" t="inlineStr">
         <is>
@@ -8931,7 +8931,7 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>0.9815764878376714</v>
+        <v>3.790568251817275</v>
       </c>
       <c r="D327" t="inlineStr">
         <is>
@@ -8957,7 +8957,7 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>0.9048165736872354</v>
+        <v>3.143104182736366</v>
       </c>
       <c r="D328" t="inlineStr">
         <is>
@@ -8983,7 +8983,7 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>1.192999712469995</v>
+        <v>4.194363328026087</v>
       </c>
       <c r="D329" t="inlineStr">
         <is>
@@ -9009,7 +9009,7 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>1.011069752334873</v>
+        <v>3.560179968504188</v>
       </c>
       <c r="D330" t="inlineStr">
         <is>
@@ -9031,11 +9031,11 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C331" t="n">
-        <v>0.9965912285912136</v>
+        <v>4.801890059915781</v>
       </c>
       <c r="D331" t="inlineStr">
         <is>
@@ -9057,11 +9057,11 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C332" t="n">
-        <v>1.086979311609661</v>
+        <v>2.712222045727824</v>
       </c>
       <c r="D332" t="inlineStr">
         <is>
@@ -9083,11 +9083,11 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C333" t="n">
-        <v>1.298089698803732</v>
+        <v>3.354692289530363</v>
       </c>
       <c r="D333" t="inlineStr">
         <is>
@@ -9113,7 +9113,7 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>0.9736341010902606</v>
+        <v>3.259957067061348</v>
       </c>
       <c r="D334" t="inlineStr">
         <is>
@@ -9139,7 +9139,7 @@
         </is>
       </c>
       <c r="C335" t="n">
-        <v>1.295417156244694</v>
+        <v>4.785278247418089</v>
       </c>
       <c r="D335" t="inlineStr">
         <is>
@@ -9165,7 +9165,7 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>0.799965221053682</v>
+        <v>3.19129945316457</v>
       </c>
       <c r="D336" t="inlineStr">
         <is>
@@ -9191,7 +9191,7 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>1.210980135096017</v>
+        <v>4.289591208288084</v>
       </c>
       <c r="D337" t="inlineStr">
         <is>
@@ -9217,7 +9217,7 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>0.8982734872145269</v>
+        <v>2.628729154086114</v>
       </c>
       <c r="D338" t="inlineStr">
         <is>
@@ -9243,7 +9243,7 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>0.808663669989255</v>
+        <v>3.573534744263261</v>
       </c>
       <c r="D339" t="inlineStr">
         <is>
@@ -9269,7 +9269,7 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>0.9011652575302479</v>
+        <v>2.63753817892738</v>
       </c>
       <c r="D340" t="inlineStr">
         <is>
@@ -9295,7 +9295,7 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>0.9896205918281874</v>
+        <v>3.260722074542648</v>
       </c>
       <c r="D341" t="inlineStr">
         <is>
@@ -9321,7 +9321,7 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>0.9163335731980065</v>
+        <v>5.2137769602022</v>
       </c>
       <c r="D342" t="inlineStr">
         <is>
@@ -9347,7 +9347,7 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>0.9089015200882787</v>
+        <v>3.723947624448577</v>
       </c>
       <c r="D343" t="inlineStr">
         <is>
@@ -9373,7 +9373,7 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>0.799965221053682</v>
+        <v>3.19129945316457</v>
       </c>
       <c r="D344" t="inlineStr">
         <is>
@@ -9399,7 +9399,7 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>1.136549070821849</v>
+        <v>4.546226078801531</v>
       </c>
       <c r="D345" t="inlineStr">
         <is>
@@ -9425,7 +9425,7 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>1.004349073791385</v>
+        <v>3.899143001448363</v>
       </c>
       <c r="D346" t="inlineStr">
         <is>
@@ -9451,7 +9451,7 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>1.175297994823818</v>
+        <v>3.173976747321055</v>
       </c>
       <c r="D347" t="inlineStr">
         <is>
@@ -9477,7 +9477,7 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>0.9063522918568704</v>
+        <v>2.653389409612415</v>
       </c>
       <c r="D348" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>0.9426836346928026</v>
+        <v>2.072378091385907</v>
       </c>
       <c r="D349" t="inlineStr">
         <is>
@@ -9529,7 +9529,7 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>0.9812396747978469</v>
+        <v>3.789442118817522</v>
       </c>
       <c r="D350" t="inlineStr">
         <is>
@@ -9555,7 +9555,7 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>0.8984831630703159</v>
+        <v>2.629109176897537</v>
       </c>
       <c r="D351" t="inlineStr">
         <is>
@@ -9581,7 +9581,7 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>1.152511172722902</v>
+        <v>4.190055759554705</v>
       </c>
       <c r="D352" t="inlineStr">
         <is>
@@ -9607,7 +9607,7 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>0.6986696015812173</v>
+        <v>2.107541645073434</v>
       </c>
       <c r="D353" t="inlineStr">
         <is>
@@ -9633,7 +9633,7 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>0.9202397095788424</v>
+        <v>2.696624532744212</v>
       </c>
       <c r="D354" t="inlineStr">
         <is>
@@ -9659,7 +9659,7 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>1.15150030765314</v>
+        <v>4.63659928462664</v>
       </c>
       <c r="D355" t="inlineStr">
         <is>
@@ -9685,7 +9685,7 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>0.8912788934279851</v>
+        <v>3.667114209647271</v>
       </c>
       <c r="D356" t="inlineStr">
         <is>
@@ -9711,7 +9711,7 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>0.823669758195022</v>
+        <v>4.777739287058305</v>
       </c>
       <c r="D357" t="inlineStr">
         <is>
@@ -9737,7 +9737,7 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>0.913557152338528</v>
+        <v>3.747473999710828</v>
       </c>
       <c r="D358" t="inlineStr">
         <is>
@@ -9763,7 +9763,7 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>0.8738729052802318</v>
+        <v>3.178823753384848</v>
       </c>
       <c r="D359" t="inlineStr">
         <is>
@@ -9789,7 +9789,7 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>0.9011286846481411</v>
+        <v>2.637688318502071</v>
       </c>
       <c r="D360" t="inlineStr">
         <is>
@@ -9815,7 +9815,7 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>0.8060002607660285</v>
+        <v>2.592769882864254</v>
       </c>
       <c r="D361" t="inlineStr">
         <is>
@@ -9841,7 +9841,7 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>1.162257196413647</v>
+        <v>4.243105297341947</v>
       </c>
       <c r="D362" t="inlineStr">
         <is>
@@ -9867,7 +9867,7 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>0.9055445607947552</v>
+        <v>5.127686509976563</v>
       </c>
       <c r="D363" t="inlineStr">
         <is>
@@ -9893,7 +9893,7 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>0.816177947254238</v>
+        <v>2.607503882992366</v>
       </c>
       <c r="D364" t="inlineStr">
         <is>
@@ -9919,7 +9919,7 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>1.18536195278948</v>
+        <v>2.65136683754638</v>
       </c>
       <c r="D365" t="inlineStr">
         <is>
@@ -9941,11 +9941,11 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C366" t="n">
-        <v>0.9917385700172701</v>
+        <v>4.919149019091581</v>
       </c>
       <c r="D366" t="inlineStr">
         <is>
@@ -9967,11 +9967,11 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C367" t="n">
-        <v>1.317310852555214</v>
+        <v>3.322146918630371</v>
       </c>
       <c r="D367" t="inlineStr">
         <is>
@@ -9997,7 +9997,7 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>0.7935096669221362</v>
+        <v>3.539839481957958</v>
       </c>
       <c r="D368" t="inlineStr">
         <is>
@@ -10023,7 +10023,7 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>0.7936083685744214</v>
+        <v>2.978306895644174</v>
       </c>
       <c r="D369" t="inlineStr">
         <is>
@@ -10049,7 +10049,7 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>1.05942309850988</v>
+        <v>3.665743612123725</v>
       </c>
       <c r="D370" t="inlineStr">
         <is>
@@ -10075,7 +10075,7 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>0.8990509251553289</v>
+        <v>4.118067016355094</v>
       </c>
       <c r="D371" t="inlineStr">
         <is>
@@ -10101,7 +10101,7 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>0.8977808369094461</v>
+        <v>3.699102079670697</v>
       </c>
       <c r="D372" t="inlineStr">
         <is>
@@ -10127,7 +10127,7 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>0.8031534166987926</v>
+        <v>3.591480943567036</v>
       </c>
       <c r="D373" t="inlineStr">
         <is>
@@ -10153,7 +10153,7 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>0.7914904501816945</v>
+        <v>2.681421688483532</v>
       </c>
       <c r="D374" t="inlineStr">
         <is>
@@ -10179,7 +10179,7 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>0.9377001146258521</v>
+        <v>3.647309737840444</v>
       </c>
       <c r="D375" t="inlineStr">
         <is>
@@ -10205,7 +10205,7 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>1.046435937996625</v>
+        <v>3.484893938637397</v>
       </c>
       <c r="D376" t="inlineStr">
         <is>
@@ -10227,11 +10227,11 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C377" t="n">
-        <v>1.046277668348691</v>
+        <v>4.150523446997902</v>
       </c>
       <c r="D377" t="inlineStr">
         <is>
@@ -10253,11 +10253,11 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C378" t="n">
-        <v>1.099147923823703</v>
+        <v>3.609709899112628</v>
       </c>
       <c r="D378" t="inlineStr">
         <is>
@@ -10283,7 +10283,7 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>0.6532295078409319</v>
+        <v>2.51932896833973</v>
       </c>
       <c r="D379" t="inlineStr">
         <is>
@@ -10309,7 +10309,7 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>1.064043360835601</v>
+        <v>3.687056469011135</v>
       </c>
       <c r="D380" t="inlineStr">
         <is>
@@ -10335,7 +10335,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>1.010432249814712</v>
+        <v>2.754798200211547</v>
       </c>
       <c r="D381" t="inlineStr">
         <is>
@@ -10357,11 +10357,11 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C382" t="n">
-        <v>1.056615399094345</v>
+        <v>4.207269490689817</v>
       </c>
       <c r="D382" t="inlineStr">
         <is>
@@ -10383,11 +10383,11 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C383" t="n">
-        <v>1.314739329745646</v>
+        <v>3.656186155652314</v>
       </c>
       <c r="D383" t="inlineStr">
         <is>
@@ -10409,11 +10409,11 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C384" t="n">
-        <v>1.109754165537558</v>
+        <v>5.7080402945961</v>
       </c>
       <c r="D384" t="inlineStr">
         <is>
@@ -10439,7 +10439,7 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>0.9027166314437385</v>
+        <v>2.642268354349291</v>
       </c>
       <c r="D385" t="inlineStr">
         <is>
@@ -10465,7 +10465,7 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>0.8974467798892408</v>
+        <v>2.625921621524737</v>
       </c>
       <c r="D386" t="inlineStr">
         <is>
@@ -10491,7 +10491,7 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>0.7696044049798559</v>
+        <v>2.612348389659889</v>
       </c>
       <c r="D387" t="inlineStr">
         <is>
@@ -10513,11 +10513,11 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C388" t="n">
-        <v>1.308371901557461</v>
+        <v>3.064426739748488</v>
       </c>
       <c r="D388" t="inlineStr">
         <is>
@@ -10539,11 +10539,11 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C389" t="n">
-        <v>0.9139881720070478</v>
+        <v>5.496239384526737</v>
       </c>
       <c r="D389" t="inlineStr">
         <is>
@@ -10565,11 +10565,11 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C390" t="n">
-        <v>0.9043632787410276</v>
+        <v>3.782213212681263</v>
       </c>
       <c r="D390" t="inlineStr">
         <is>
@@ -10591,11 +10591,11 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="C391" t="n">
-        <v>1.06699335378894</v>
+        <v>1.959464718904604</v>
       </c>
       <c r="D391" t="inlineStr">
         <is>
@@ -10617,11 +10617,11 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>Hardware</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C392" t="n">
-        <v>0.6749086909127469</v>
+        <v>3.275787769942471</v>
       </c>
       <c r="D392" t="inlineStr">
         <is>
@@ -10647,7 +10647,7 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>0.9716635923413418</v>
+        <v>3.745783097423464</v>
       </c>
       <c r="D393" t="inlineStr">
         <is>
@@ -10673,7 +10673,7 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>0.3786150638679462</v>
+        <v>1.489640934318389</v>
       </c>
       <c r="D394" t="inlineStr">
         <is>
@@ -10695,11 +10695,11 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C395" t="n">
-        <v>1.316844151076587</v>
+        <v>4.217839449628165</v>
       </c>
       <c r="D395" t="inlineStr">
         <is>
@@ -10721,11 +10721,11 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C396" t="n">
-        <v>1.111671961150397</v>
+        <v>5.72418491917407</v>
       </c>
       <c r="D396" t="inlineStr">
         <is>
@@ -10751,7 +10751,7 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>1.191423360700792</v>
+        <v>4.186692748535647</v>
       </c>
       <c r="D397" t="inlineStr">
         <is>
@@ -10777,7 +10777,7 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>1.078876114551234</v>
+        <v>4.976395698067938</v>
       </c>
       <c r="D398" t="inlineStr">
         <is>
@@ -10803,7 +10803,7 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>0.7822924343198053</v>
+        <v>3.191621482712807</v>
       </c>
       <c r="D399" t="inlineStr">
         <is>
@@ -10829,7 +10829,7 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>0.8023666826813944</v>
+        <v>4.033826463265554</v>
       </c>
       <c r="D400" t="inlineStr">
         <is>
@@ -10855,7 +10855,7 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>1.049407807327577</v>
+        <v>3.587098175457623</v>
       </c>
       <c r="D401" t="inlineStr">
         <is>
@@ -10881,7 +10881,7 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>1.306622699698165</v>
+        <v>3.691574849072623</v>
       </c>
       <c r="D402" t="inlineStr">
         <is>
@@ -10907,7 +10907,7 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>1.085710095892315</v>
+        <v>2.957114670953328</v>
       </c>
       <c r="D403" t="inlineStr">
         <is>
@@ -10933,7 +10933,7 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>0.8155656963122825</v>
+        <v>2.61920792214071</v>
       </c>
       <c r="D404" t="inlineStr">
         <is>
@@ -10959,7 +10959,7 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>1.115281131367188</v>
+        <v>3.040868532010132</v>
       </c>
       <c r="D405" t="inlineStr">
         <is>
@@ -10985,7 +10985,7 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>0.6938410490489123</v>
+        <v>4.01113190648849</v>
       </c>
       <c r="D406" t="inlineStr">
         <is>
@@ -11007,11 +11007,11 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C407" t="n">
-        <v>0.8214071023393741</v>
+        <v>5.449116443412637</v>
       </c>
       <c r="D407" t="inlineStr">
         <is>
@@ -11033,11 +11033,11 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C408" t="n">
-        <v>1.165340586769594</v>
+        <v>4.760722134328216</v>
       </c>
       <c r="D408" t="inlineStr">
         <is>
@@ -11063,7 +11063,7 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>1.12265500806447</v>
+        <v>4.278357092242738</v>
       </c>
       <c r="D409" t="inlineStr">
         <is>
@@ -11089,7 +11089,7 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>1.069190500093204</v>
+        <v>3.714366498943337</v>
       </c>
       <c r="D410" t="inlineStr">
         <is>
@@ -11111,11 +11111,11 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="C411" t="n">
-        <v>1.328896734761429</v>
+        <v>3.986543157596581</v>
       </c>
       <c r="D411" t="inlineStr">
         <is>
@@ -11137,11 +11137,11 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>Hardware</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C412" t="n">
-        <v>1.383283339117241</v>
+        <v>5.816702929535777</v>
       </c>
       <c r="D412" t="inlineStr">
         <is>
@@ -11167,7 +11167,7 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>0.9707834229449559</v>
+        <v>4.15250956092703</v>
       </c>
       <c r="D413" t="inlineStr">
         <is>
@@ -11193,7 +11193,7 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>0.8581254374774394</v>
+        <v>2.588253339336453</v>
       </c>
       <c r="D414" t="inlineStr">
         <is>
@@ -11215,11 +11215,11 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C415" t="n">
-        <v>0.8238060149574141</v>
+        <v>4.90829423878745</v>
       </c>
       <c r="D415" t="inlineStr">
         <is>
@@ -11241,11 +11241,11 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C416" t="n">
-        <v>0.9137001346922736</v>
+        <v>3.315925813760587</v>
       </c>
       <c r="D416" t="inlineStr">
         <is>
@@ -11267,11 +11267,11 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C417" t="n">
-        <v>0.9040766917682419</v>
+        <v>3.418523380873872</v>
       </c>
       <c r="D417" t="inlineStr">
         <is>
@@ -11297,7 +11297,7 @@
         </is>
       </c>
       <c r="C418" t="n">
-        <v>1.069671142063382</v>
+        <v>4.478650439101072</v>
       </c>
       <c r="D418" t="inlineStr">
         <is>
@@ -11323,7 +11323,7 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>0.9005175094443117</v>
+        <v>4.428815689971398</v>
       </c>
       <c r="D419" t="inlineStr">
         <is>
@@ -11349,7 +11349,7 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>1.064232031979684</v>
+        <v>5.461462846884182</v>
       </c>
       <c r="D420" t="inlineStr">
         <is>
@@ -11375,7 +11375,7 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>0.4093440614403802</v>
+        <v>2.988458590657185</v>
       </c>
       <c r="D421" t="inlineStr">
         <is>
@@ -11401,7 +11401,7 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>1.103047782530701</v>
+        <v>3.419440696634741</v>
       </c>
       <c r="D422" t="inlineStr">
         <is>
@@ -11427,7 +11427,7 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>1.167365241737782</v>
+        <v>3.706878977886729</v>
       </c>
       <c r="D423" t="inlineStr">
         <is>
@@ -11449,11 +11449,11 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C424" t="n">
-        <v>0.9814441665795927</v>
+        <v>3.65132773309605</v>
       </c>
       <c r="D424" t="inlineStr">
         <is>
@@ -11475,11 +11475,11 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C425" t="n">
-        <v>1.056287246266585</v>
+        <v>3.28008194653524</v>
       </c>
       <c r="D425" t="inlineStr">
         <is>
@@ -11501,11 +11501,11 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C426" t="n">
-        <v>0.8871422948940501</v>
+        <v>4.1878690715375</v>
       </c>
       <c r="D426" t="inlineStr">
         <is>
@@ -11527,11 +11527,11 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C427" t="n">
-        <v>0.877653073587546</v>
+        <v>3.615033277145613</v>
       </c>
       <c r="D427" t="inlineStr">
         <is>
@@ -11553,11 +11553,11 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C428" t="n">
-        <v>0.8604093657647406</v>
+        <v>3.793652524305171</v>
       </c>
       <c r="D428" t="inlineStr">
         <is>
@@ -11579,11 +11579,11 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C429" t="n">
-        <v>1.095362611778106</v>
+        <v>2.906009270826026</v>
       </c>
       <c r="D429" t="inlineStr">
         <is>
@@ -11609,7 +11609,7 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>0.8735872506309847</v>
+        <v>2.898662233460566</v>
       </c>
       <c r="D430" t="inlineStr">
         <is>
@@ -11635,7 +11635,7 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>0.8735872506309847</v>
+        <v>2.898662233460566</v>
       </c>
       <c r="D431" t="inlineStr">
         <is>
@@ -11661,7 +11661,7 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>0.9716635923413418</v>
+        <v>3.745783097423464</v>
       </c>
       <c r="D432" t="inlineStr">
         <is>
@@ -11687,7 +11687,7 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>1.382873000608318</v>
+        <v>3.984730516998706</v>
       </c>
       <c r="D433" t="inlineStr">
         <is>
@@ -11713,7 +11713,7 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>0.9830701586770633</v>
+        <v>3.28694791666735</v>
       </c>
       <c r="D434" t="inlineStr">
         <is>
@@ -11739,7 +11739,7 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>0.8241594161382686</v>
+        <v>3.10017503036091</v>
       </c>
       <c r="D435" t="inlineStr">
         <is>
@@ -11765,7 +11765,7 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>0.9140709783612474</v>
+        <v>3.782523654973498</v>
       </c>
       <c r="D436" t="inlineStr">
         <is>
@@ -11791,7 +11791,7 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>1.078308539597659</v>
+        <v>3.320232107623856</v>
       </c>
       <c r="D437" t="inlineStr">
         <is>
@@ -11813,11 +11813,11 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C438" t="n">
-        <v>0.9900565051540713</v>
+        <v>4.907112878241309</v>
       </c>
       <c r="D438" t="inlineStr">
         <is>
@@ -11843,7 +11843,7 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>1.065225681702834</v>
+        <v>3.692408688167432</v>
       </c>
       <c r="D439" t="inlineStr">
         <is>
@@ -11865,11 +11865,11 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C440" t="n">
-        <v>1.102652809700569</v>
+        <v>3.315248647305011</v>
       </c>
       <c r="D440" t="inlineStr">
         <is>
@@ -11891,11 +11891,11 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C441" t="n">
-        <v>1.315353527948743</v>
+        <v>3.417815575381814</v>
       </c>
       <c r="D441" t="inlineStr">
         <is>
@@ -11917,11 +11917,11 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C442" t="n">
-        <v>0.9635767327337086</v>
+        <v>3.568478059376749</v>
       </c>
       <c r="D442" t="inlineStr">
         <is>
@@ -11943,11 +11943,11 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C443" t="n">
-        <v>1.037740988277038</v>
+        <v>3.209114412476056</v>
       </c>
       <c r="D443" t="inlineStr">
         <is>
@@ -11969,11 +11969,11 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C444" t="n">
-        <v>1.103874616125087</v>
+        <v>4.915412845808926</v>
       </c>
       <c r="D444" t="inlineStr">
         <is>
@@ -11995,11 +11995,11 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C445" t="n">
-        <v>1.316699068736741</v>
+        <v>3.422788037429468</v>
       </c>
       <c r="D445" t="inlineStr">
         <is>
@@ -12025,7 +12025,7 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>0.958535990820544</v>
+        <v>3.355555361901345</v>
       </c>
       <c r="D446" t="inlineStr">
         <is>
@@ -12047,11 +12047,11 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C447" t="n">
-        <v>1.308823887823753</v>
+        <v>4.178562289578681</v>
       </c>
       <c r="D447" t="inlineStr">
         <is>
@@ -12073,11 +12073,11 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C448" t="n">
-        <v>1.104364738837706</v>
+        <v>5.664214632750511</v>
       </c>
       <c r="D448" t="inlineStr">
         <is>
@@ -12103,7 +12103,7 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>0.9430872121692568</v>
+        <v>3.497055246625211</v>
       </c>
       <c r="D449" t="inlineStr">
         <is>
@@ -12129,7 +12129,7 @@
         </is>
       </c>
       <c r="C450" t="n">
-        <v>1.004112965841077</v>
+        <v>2.660134845113467</v>
       </c>
       <c r="D450" t="inlineStr">
         <is>
@@ -12155,7 +12155,7 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>0.9909718761806159</v>
+        <v>3.319025238978161</v>
       </c>
       <c r="D451" t="inlineStr">
         <is>
@@ -12177,11 +12177,11 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Levels</t>
         </is>
       </c>
       <c r="C452" t="n">
-        <v>0.822781614158685</v>
+        <v>3.059198700107313</v>
       </c>
       <c r="D452" t="inlineStr">
         <is>
@@ -12207,7 +12207,7 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>1.166975145422432</v>
+        <v>3.667253000538098</v>
       </c>
       <c r="D453" t="inlineStr">
         <is>
@@ -12229,11 +12229,11 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>Levels</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C454" t="n">
-        <v>0.9030071338759323</v>
+        <v>3.094624939022055</v>
       </c>
       <c r="D454" t="inlineStr">
         <is>
@@ -12259,7 +12259,7 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>0.8566166842415504</v>
+        <v>2.937340330078739</v>
       </c>
       <c r="D455" t="inlineStr">
         <is>
@@ -12281,11 +12281,11 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Cybersecurity</t>
         </is>
       </c>
       <c r="C456" t="n">
-        <v>1.171380779405432</v>
+        <v>1</v>
       </c>
       <c r="D456" t="inlineStr">
         <is>
@@ -12307,11 +12307,11 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C457" t="n">
-        <v>0.9165131788909052</v>
+        <v>5.495384366225682</v>
       </c>
       <c r="D457" t="inlineStr">
         <is>
@@ -12333,11 +12333,11 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>Cybersecurity</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C458" t="n">
-        <v>0</v>
+        <v>3.762643495828875</v>
       </c>
       <c r="D458" t="inlineStr">
         <is>
@@ -12363,7 +12363,7 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>1.148045959020233</v>
+        <v>3.585295489166757</v>
       </c>
       <c r="D459" t="inlineStr">
         <is>
@@ -12389,7 +12389,7 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>0.806067910936006</v>
+        <v>2.592843349327829</v>
       </c>
       <c r="D460" t="inlineStr">
         <is>
@@ -12415,7 +12415,7 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>1.135141591450392</v>
+        <v>3.530453384461424</v>
       </c>
       <c r="D461" t="inlineStr">
         <is>
@@ -12441,7 +12441,7 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>0.9002197389891996</v>
+        <v>2.634616977465053</v>
       </c>
       <c r="D462" t="inlineStr">
         <is>
@@ -12467,7 +12467,7 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>1.173413819128643</v>
+        <v>4.303014010611655</v>
       </c>
       <c r="D463" t="inlineStr">
         <is>
@@ -12493,7 +12493,7 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>1.061115285974553</v>
+        <v>5.413751931676683</v>
       </c>
       <c r="D464" t="inlineStr">
         <is>
@@ -12519,7 +12519,7 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>0.9048165736872354</v>
+        <v>3.143104182736366</v>
       </c>
       <c r="D465" t="inlineStr">
         <is>
@@ -12545,7 +12545,7 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>0.9340233692950888</v>
+        <v>3.489780640629311</v>
       </c>
       <c r="D466" t="inlineStr">
         <is>
@@ -12571,7 +12571,7 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>1.016268812725203</v>
+        <v>4.531534744602277</v>
       </c>
       <c r="D467" t="inlineStr">
         <is>
@@ -12597,7 +12597,7 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>0.9744670698342591</v>
+        <v>3.040659224824976</v>
       </c>
       <c r="D468" t="inlineStr">
         <is>
@@ -12623,7 +12623,7 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>0.8407016319724134</v>
+        <v>2.787005971448859</v>
       </c>
       <c r="D469" t="inlineStr">
         <is>
@@ -12649,7 +12649,7 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>0.8093089943517654</v>
+        <v>2.597611730791097</v>
       </c>
       <c r="D470" t="inlineStr">
         <is>
@@ -12671,11 +12671,11 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C471" t="n">
-        <v>0.6978525031006638</v>
+        <v>3.127901702338698</v>
       </c>
       <c r="D471" t="inlineStr">
         <is>
@@ -12697,11 +12697,11 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C472" t="n">
-        <v>1.026309217954979</v>
+        <v>2.658885305344494</v>
       </c>
       <c r="D472" t="inlineStr">
         <is>
@@ -12727,7 +12727,7 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>0.406950876107914</v>
+        <v>1.513141978705477</v>
       </c>
       <c r="D473" t="inlineStr">
         <is>
@@ -12753,7 +12753,7 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>1.26867825078507</v>
+        <v>3.547770459333335</v>
       </c>
       <c r="D474" t="inlineStr">
         <is>
@@ -12779,7 +12779,7 @@
         </is>
       </c>
       <c r="C475" t="n">
-        <v>0.8811088670264807</v>
+        <v>3.585750336215074</v>
       </c>
       <c r="D475" t="inlineStr">
         <is>
@@ -12805,7 +12805,7 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>0.8937474754957208</v>
+        <v>3.023014906931659</v>
       </c>
       <c r="D476" t="inlineStr">
         <is>
@@ -12827,11 +12827,11 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="C477" t="n">
-        <v>0.8189774297528674</v>
+        <v>5.427244427383135</v>
       </c>
       <c r="D477" t="inlineStr">
         <is>
@@ -12853,11 +12853,11 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="C478" t="n">
-        <v>1.162450975382636</v>
+        <v>4.742570660268941</v>
       </c>
       <c r="D478" t="inlineStr">
         <is>
@@ -12883,7 +12883,7 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>1.065034597790177</v>
+        <v>3.657267801888358</v>
       </c>
       <c r="D479" t="inlineStr">
         <is>
@@ -12909,7 +12909,7 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>1.655545036729936</v>
+        <v>5.981015164616304</v>
       </c>
       <c r="D480" t="inlineStr">
         <is>
@@ -12935,7 +12935,7 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>1.192174635370317</v>
+        <v>5.174168382440834</v>
       </c>
       <c r="D481" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
visualization improvements for Results
</commit_message>
<xml_diff>
--- a/src/results/kl_content_vs_domain.xlsx
+++ b/src/results/kl_content_vs_domain.xlsx
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2.711978678030391</v>
+        <v>0.9976785079640537</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2.811086312970962</v>
+        <v>1.033570996885565</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4.095189441585775</v>
+        <v>1.409812977916502</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3.788451271358973</v>
+        <v>1.33195730005475</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3.525981028549917</v>
+        <v>1.260158703515917</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2.341822043970831</v>
+        <v>0.850929277647569</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -633,7 +633,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.424020729188626</v>
+        <v>1.487048949830355</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5.245126235711101</v>
+        <v>1.65729930937772</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>5.194454554333685</v>
+        <v>1.64759162468542</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3.143104182736366</v>
+        <v>1.145210904811836</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2.968472608332762</v>
+        <v>1.088047547242113</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -763,7 +763,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3.905367147028273</v>
+        <v>1.362351798597622</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -789,7 +789,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4.167934023936781</v>
+        <v>1.427420475135951</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3.477793352621579</v>
+        <v>1.246397998589452</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -841,7 +841,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3.597212426864761</v>
+        <v>1.280159219646041</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -867,7 +867,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3.039860480908064</v>
+        <v>1.111811619926812</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -893,7 +893,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.7021158170832</v>
+        <v>1.308904498665506</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -919,7 +919,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4.976128255929501</v>
+        <v>1.604652130010157</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2.606996790034425</v>
+        <v>0.9581989036634663</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3.53082817950725</v>
+        <v>1.261532455186599</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3.681063449567651</v>
+        <v>1.303201691294688</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1023,7 +1023,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>5.754468870631289</v>
+        <v>1.749976747842099</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2.271028857805698</v>
+        <v>0.8202329701345841</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4.682608470168031</v>
+        <v>1.543855320079661</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2.985317840491363</v>
+        <v>1.093706220402642</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3.674979831390265</v>
+        <v>1.30154764459267</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>4.644235257846269</v>
+        <v>1.535626721003511</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1179,7 +1179,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2.34293571944496</v>
+        <v>0.85140472399991</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1205,7 +1205,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3.259461633739601</v>
+        <v>1.181562038716343</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>3.359509940780391</v>
+        <v>1.211795112379611</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2.597575832410767</v>
+        <v>0.9545786379484534</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1283,7 +1283,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>4.053483233114857</v>
+        <v>1.399576569040094</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1309,7 +1309,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>3.004663560739919</v>
+        <v>1.100165601898876</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1335,7 +1335,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2.987345390929563</v>
+        <v>1.094385163928344</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>3.021547465853074</v>
+        <v>1.105769106063312</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1.723702701202609</v>
+        <v>0.5444747102725365</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1413,7 +1413,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3.355555361901345</v>
+        <v>1.210617289333083</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1439,7 +1439,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3.68424227249903</v>
+        <v>1.304064879666959</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>4.085025941823573</v>
+        <v>1.407328078799408</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1491,7 +1491,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2.939517435372488</v>
+        <v>1.07824543025013</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>5.352952274063424</v>
+        <v>1.677648235635169</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1543,7 +1543,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3.259957067061348</v>
+        <v>1.181714025678813</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.007193096895661</v>
+        <v>1.101007117739678</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1595,7 +1595,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4.724886495544438</v>
+        <v>1.552843538550173</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1621,7 +1621,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3.015775862538224</v>
+        <v>1.103857131249588</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1647,7 +1647,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3.050461426771327</v>
+        <v>1.115292866642535</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1673,7 +1673,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>5.771629922421908</v>
+        <v>1.752954522851585</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1699,7 +1699,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>5.471935055275102</v>
+        <v>1.699632311696291</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.20276988500293</v>
+        <v>1.435743804346387</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1751,7 +1751,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.66983804451761</v>
+        <v>1.541124391104626</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3.357183674881658</v>
+        <v>1.211102430496274</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>4.239917986765248</v>
+        <v>1.444543926312748</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1829,7 +1829,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2.587425524030488</v>
+        <v>0.9506633751938629</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1855,7 +1855,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>5.162069170945258</v>
+        <v>1.641337501234782</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1881,7 +1881,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3.009224957805241</v>
+        <v>1.101682556503525</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>3.661319754448255</v>
+        <v>1.297823671063877</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>3.363410551772938</v>
+        <v>1.212955504335622</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1959,7 +1959,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>5.384878808790114</v>
+        <v>1.683594805023648</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1985,7 +1985,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.606859326075734</v>
+        <v>0.9581461734171146</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -2011,7 +2011,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>3.592197736919162</v>
+        <v>1.278764198178463</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -2037,7 +2037,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>3.035937121254685</v>
+        <v>1.110520148269725</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -2063,7 +2063,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>3.696889521089056</v>
+        <v>1.307491796113078</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1.977863906900977</v>
+        <v>0.6820174274466928</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -2115,7 +2115,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>3.668642666771185</v>
+        <v>1.299821748090305</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -2141,7 +2141,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>4.144999753578629</v>
+        <v>1.421902729136986</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>5.186661523136146</v>
+        <v>1.646090238398382</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -2193,7 +2193,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>3.58027399992297</v>
+        <v>1.275439333775189</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -2219,7 +2219,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>3.901629326130327</v>
+        <v>1.361394241822388</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -2245,7 +2245,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>4.556104016270843</v>
+        <v>1.516467875936885</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -2271,7 +2271,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>3.589826023657684</v>
+        <v>1.278103739949207</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -2297,7 +2297,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>4.123937244634946</v>
+        <v>1.416808348928104</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -2323,7 +2323,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>4.170539772886846</v>
+        <v>1.428045469373117</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -2349,7 +2349,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>5.965368039601065</v>
+        <v>1.78597075349582</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -2375,7 +2375,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>5.114413432032268</v>
+        <v>1.632062716783267</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -2401,7 +2401,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>4.192957180144703</v>
+        <v>1.433406255912465</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>4.597277769130899</v>
+        <v>1.525464338999265</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2.353202152215462</v>
+        <v>0.8557770185987118</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2479,7 +2479,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>4.049145415627207</v>
+        <v>1.398505850365915</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2505,7 +2505,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>2.602445925959741</v>
+        <v>0.9564517435619209</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2531,7 +2531,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>3.62149523725919</v>
+        <v>1.286886989523065</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>3.254535006844541</v>
+        <v>1.1800494104157</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2583,7 +2583,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>3.354361417925618</v>
+        <v>1.210261414878152</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2609,7 +2609,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>3.259957067061348</v>
+        <v>1.181714025678813</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2635,7 +2635,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>4.189269835545515</v>
+        <v>1.432526455155426</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2661,7 +2661,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>2.676083942172715</v>
+        <v>0.9843545102989311</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2687,7 +2687,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>2.353562615834209</v>
+        <v>0.8559301869158958</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2713,7 +2713,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>2.658205896253776</v>
+        <v>0.9776514201403887</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2739,7 +2739,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2.708471792257142</v>
+        <v>0.9963845615358853</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2765,7 +2765,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>3.699837088062662</v>
+        <v>1.308288788427484</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2791,7 +2791,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4.593114743277579</v>
+        <v>1.524558387238786</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2817,7 +2817,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>3.481474445188781</v>
+        <v>1.247455895200835</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2843,7 +2843,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4.155473715078871</v>
+        <v>1.424426432657976</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -2869,7 +2869,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>3.415882744397522</v>
+        <v>1.228435949926632</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2895,7 +2895,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1.996257051752005</v>
+        <v>0.6912739530402849</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2921,7 +2921,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>3.675472453478736</v>
+        <v>1.301681683171554</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -2947,7 +2947,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>2.997413055752284</v>
+        <v>1.097749601911634</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2974,7 +2974,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>2.614956892436414</v>
+        <v>0.9612476126530628</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -3000,7 +3000,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>4.572446148629727</v>
+        <v>1.520048323986572</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -3026,7 +3026,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>2.951311446820562</v>
+        <v>1.082249629809247</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>3.609204510969096</v>
+        <v>1.28348739099033</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>3.244007597290495</v>
+        <v>1.176809478201871</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -3104,7 +3104,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>3.343360140985501</v>
+        <v>1.206976331514516</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -3130,7 +3130,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>3.621214128004835</v>
+        <v>1.286809364081999</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -3156,7 +3156,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2.932772137822475</v>
+        <v>1.075948097861257</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3.901501855848593</v>
+        <v>1.361361570250227</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -3208,7 +3208,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>5.444641413076798</v>
+        <v>1.694631898032067</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -3234,7 +3234,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>2.984714230296576</v>
+        <v>1.093504007017626</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -3260,7 +3260,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1.494360333755123</v>
+        <v>0.4016982448820808</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -3286,7 +3286,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>2.950872346255414</v>
+        <v>1.082100837233023</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -3312,7 +3312,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>3.584316802803488</v>
+        <v>1.276567884845562</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>4.104745120120812</v>
+        <v>1.412143650872169</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -3364,7 +3364,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>3.259957067061348</v>
+        <v>1.181714025678813</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -3390,7 +3390,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>2.341822043970831</v>
+        <v>0.850929277647569</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -3416,7 +3416,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>5.194463642361002</v>
+        <v>1.647593374247241</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>3.607767692056407</v>
+        <v>1.283089213225125</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -3468,7 +3468,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>4.179840760701252</v>
+        <v>1.430273150284996</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -3494,7 +3494,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>5.666165719188609</v>
+        <v>1.734512648984248</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -3520,7 +3520,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>2.602748266818794</v>
+        <v>0.9565679124686688</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
@@ -3546,7 +3546,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>4.832460070785934</v>
+        <v>1.575355669424916</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
@@ -3572,7 +3572,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2.725624658281382</v>
+        <v>1.002697634242313</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>3.373047598392492</v>
+        <v>1.215816667569774</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -3624,7 +3624,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>3.61848674480926</v>
+        <v>1.286055912144546</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -3650,7 +3650,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>5.950091762950752</v>
+        <v>1.783406641783279</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -3676,7 +3676,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>5.637780485036386</v>
+        <v>1.729490457034397</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -3702,7 +3702,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>5.211063836929208</v>
+        <v>1.650784026270236</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -3728,7 +3728,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>2.587410869283717</v>
+        <v>0.950657711344552</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -3754,7 +3754,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>3.097607837184779</v>
+        <v>1.130630148179816</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
@@ -3780,7 +3780,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>3.89641894606736</v>
+        <v>1.360057912357251</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
@@ -3806,7 +3806,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>2.614761043796963</v>
+        <v>0.9611727142964286</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
@@ -3832,7 +3832,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>5.381695183074451</v>
+        <v>1.68300341433412</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -3858,7 +3858,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>3.714212826434402</v>
+        <v>1.312166765121346</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
@@ -3884,7 +3884,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>3.525981028549917</v>
+        <v>1.260158703515917</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
@@ -3910,7 +3910,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>4.629615619449921</v>
+        <v>1.532473845094576</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -3936,7 +3936,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>4.138071233497964</v>
+        <v>1.420229793650284</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
@@ -3962,7 +3962,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>4.071000928486096</v>
+        <v>1.40388889759404</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
@@ -3988,7 +3988,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2.606883057989851</v>
+        <v>0.9581552770177028</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
@@ -4014,7 +4014,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>4.095600281339792</v>
+        <v>1.409913295411703</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
@@ -4040,7 +4040,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>3.605555356627584</v>
+        <v>1.282475810641251</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
@@ -4066,7 +4066,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>3.240881718168308</v>
+        <v>1.175845428019293</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>3.34009363337625</v>
+        <v>1.20599884054065</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
@@ -4118,7 +4118,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>2.029798318117932</v>
+        <v>0.7079364374372685</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
@@ -4144,7 +4144,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>2.14110609791518</v>
+        <v>0.7613225636880731</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
@@ -4170,7 +4170,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>3.899925652309328</v>
+        <v>1.360957489443461</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
@@ -4196,7 +4196,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>3.618736055659375</v>
+        <v>1.286124808973367</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
@@ -4222,7 +4222,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>3.252171794374241</v>
+        <v>1.179323017588604</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
@@ -4248,7 +4248,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>3.351891796572891</v>
+        <v>1.209524901840134</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
@@ -4274,7 +4274,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>4.648208157405881</v>
+        <v>1.536481802842409</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
@@ -4300,7 +4300,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>2.329600833067359</v>
+        <v>0.8456969366211955</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
@@ -4326,7 +4326,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>3.36206393899415</v>
+        <v>1.212555052947803</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
@@ -4352,7 +4352,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>4.094627978867123</v>
+        <v>1.409675865526639</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>4.244811025261351</v>
+        <v>1.445697301755049</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
@@ -4404,7 +4404,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>3.68374911371534</v>
+        <v>1.303931014476685</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
@@ -4431,7 +4431,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>4.170243596783871</v>
+        <v>1.427974450599466</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
@@ -4457,7 +4457,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>3.620348783041</v>
+        <v>1.286570370102776</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
@@ -4483,7 +4483,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>5.953823965023012</v>
+        <v>1.78403369632228</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
@@ -4509,7 +4509,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>5.641247930694018</v>
+        <v>1.730105305342081</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
@@ -4535,7 +4535,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>4.184306509600763</v>
+        <v>1.431340981632182</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
@@ -4561,7 +4561,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>2.000413716224249</v>
+        <v>0.6933540172798808</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
@@ -4587,7 +4587,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>5.453440394502685</v>
+        <v>1.69624667455755</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
@@ -4613,7 +4613,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>2.606831587820099</v>
+        <v>0.958135532872405</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
@@ -4639,7 +4639,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>3.016547471071009</v>
+        <v>1.10411295591094</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
@@ -4665,7 +4665,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>3.60685750545191</v>
+        <v>1.28283689613743</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
@@ -4691,7 +4691,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>3.04740562910214</v>
+        <v>1.114290615233317</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>
@@ -4717,7 +4717,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>3.712168101571638</v>
+        <v>1.311616099882314</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
@@ -4743,7 +4743,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>2.94776620688222</v>
+        <v>1.081047665511341</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
@@ -4769,7 +4769,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>3.522401995843224</v>
+        <v>1.259143142073834</v>
       </c>
       <c r="D167" t="inlineStr">
         <is>
@@ -4795,7 +4795,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>3.624156417817094</v>
+        <v>1.287621548898604</v>
       </c>
       <c r="D168" t="inlineStr">
         <is>
@@ -4821,7 +4821,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>3.557014440800374</v>
+        <v>1.268921552783878</v>
       </c>
       <c r="D169" t="inlineStr">
         <is>
@@ -4847,7 +4847,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>2.998804899888139</v>
+        <v>1.098213842595061</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
@@ -4873,7 +4873,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>3.588701688868807</v>
+        <v>1.277790490535652</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
@@ -4900,7 +4900,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>3.362540288211578</v>
+        <v>1.21269672648044</v>
       </c>
       <c r="D172" t="inlineStr">
         <is>
@@ -4927,7 +4927,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>4.636256294628171</v>
+        <v>1.533907207518918</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>2.615071378084162</v>
+        <v>0.9612913927788458</v>
       </c>
       <c r="D174" t="inlineStr">
         <is>
@@ -4979,7 +4979,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>2.664724887842877</v>
+        <v>0.9801008207104039</v>
       </c>
       <c r="D175" t="inlineStr">
         <is>
@@ -5005,7 +5005,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>3.621214128004835</v>
+        <v>1.286809364081999</v>
       </c>
       <c r="D176" t="inlineStr">
         <is>
@@ -5031,7 +5031,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>2.913335717061498</v>
+        <v>1.069298719212328</v>
       </c>
       <c r="D177" t="inlineStr">
         <is>
@@ -5057,7 +5057,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>4.741916515047127</v>
+        <v>1.556441382057432</v>
       </c>
       <c r="D178" t="inlineStr">
         <is>
@@ -5083,7 +5083,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>2.615347097818801</v>
+        <v>0.9613968221000999</v>
       </c>
       <c r="D179" t="inlineStr">
         <is>
@@ -5109,7 +5109,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>3.618382889995565</v>
+        <v>1.286027210559761</v>
       </c>
       <c r="D180" t="inlineStr">
         <is>
@@ -5135,7 +5135,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>5.949883610554298</v>
+        <v>1.783371658114836</v>
       </c>
       <c r="D181" t="inlineStr">
         <is>
@@ -5161,7 +5161,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>5.637587097553423</v>
+        <v>1.729456154386334</v>
       </c>
       <c r="D182" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>4.675474101569423</v>
+        <v>1.542330569699202</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
@@ -5213,7 +5213,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>3.206565117306952</v>
+        <v>1.165200307308562</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
@@ -5239,7 +5239,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>2.931920996799751</v>
+        <v>1.075657838504403</v>
       </c>
       <c r="D185" t="inlineStr">
         <is>
@@ -5265,7 +5265,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>3.501834769147191</v>
+        <v>1.253287050896533</v>
       </c>
       <c r="D186" t="inlineStr">
         <is>
@@ -5291,7 +5291,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>3.602726426861746</v>
+        <v>1.281690899619166</v>
       </c>
       <c r="D187" t="inlineStr">
         <is>
@@ -5317,7 +5317,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>1.969462346184545</v>
+        <v>0.6777605847817549</v>
       </c>
       <c r="D188" t="inlineStr">
         <is>
@@ -5343,7 +5343,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>3.717557239793742</v>
+        <v>1.313066796622671</v>
       </c>
       <c r="D189" t="inlineStr">
         <is>
@@ -5369,7 +5369,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>4.735706596535085</v>
+        <v>1.55513094391749</v>
       </c>
       <c r="D190" t="inlineStr">
         <is>
@@ -5395,7 +5395,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>1.494776924448729</v>
+        <v>0.4019769812935054</v>
       </c>
       <c r="D191" t="inlineStr">
         <is>
@@ -5421,7 +5421,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>3.357183674881658</v>
+        <v>1.211102430496274</v>
       </c>
       <c r="D192" t="inlineStr">
         <is>
@@ -5447,7 +5447,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>3.355555361901345</v>
+        <v>1.210617289333083</v>
       </c>
       <c r="D193" t="inlineStr">
         <is>
@@ -5473,7 +5473,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>4.204290789334585</v>
+        <v>1.43610562030256</v>
       </c>
       <c r="D194" t="inlineStr">
         <is>
@@ -5499,7 +5499,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>4.668531407772891</v>
+        <v>1.540844548513278</v>
       </c>
       <c r="D195" t="inlineStr">
         <is>
@@ -5525,7 +5525,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>2.341547991209719</v>
+        <v>0.8508122453569895</v>
       </c>
       <c r="D196" t="inlineStr">
         <is>
@@ -5551,7 +5551,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>3.198357933822101</v>
+        <v>1.162637532420785</v>
       </c>
       <c r="D197" t="inlineStr">
         <is>
@@ -5577,7 +5577,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>3.618921441739625</v>
+        <v>1.286176037172645</v>
       </c>
       <c r="D198" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>4.150457196141846</v>
+        <v>1.42321849591961</v>
       </c>
       <c r="D199" t="inlineStr">
         <is>
@@ -5629,7 +5629,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>5.173443819229684</v>
+        <v>1.643538582668771</v>
       </c>
       <c r="D200" t="inlineStr">
         <is>
@@ -5655,7 +5655,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>3.472760292405569</v>
+        <v>1.244949751053282</v>
       </c>
       <c r="D201" t="inlineStr">
         <is>
@@ -5681,7 +5681,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>4.113028441293737</v>
+        <v>1.414159604199759</v>
       </c>
       <c r="D202" t="inlineStr">
         <is>
@@ -5707,7 +5707,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>3.700196332652877</v>
+        <v>1.30838588112155</v>
       </c>
       <c r="D203" t="inlineStr">
         <is>
@@ -5733,7 +5733,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>4.629584586133598</v>
+        <v>1.532467141855498</v>
       </c>
       <c r="D204" t="inlineStr">
         <is>
@@ -5759,7 +5759,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>3.578397050518015</v>
+        <v>1.274914948890134</v>
       </c>
       <c r="D205" t="inlineStr">
         <is>
@@ -5785,7 +5785,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>2.939338043295907</v>
+        <v>1.078184400657793</v>
       </c>
       <c r="D206" t="inlineStr">
         <is>
@@ -5811,7 +5811,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>3.593269604306236</v>
+        <v>1.279062541304699</v>
       </c>
       <c r="D207" t="inlineStr">
         <is>
@@ -5837,7 +5837,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>2.316424329988281</v>
+        <v>0.8400247596765728</v>
       </c>
       <c r="D208" t="inlineStr">
         <is>
@@ -5863,7 +5863,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>2.732516097666648</v>
+        <v>1.005222832237534</v>
       </c>
       <c r="D209" t="inlineStr">
         <is>
@@ -5889,7 +5889,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>3.557200934528244</v>
+        <v>1.268973981257877</v>
       </c>
       <c r="D210" t="inlineStr">
         <is>
@@ -5915,7 +5915,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>3.745783097423464</v>
+        <v>1.320630699895796</v>
       </c>
       <c r="D211" t="inlineStr">
         <is>
@@ -5941,7 +5941,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>4.147443662932175</v>
+        <v>1.422492159610382</v>
       </c>
       <c r="D212" t="inlineStr">
         <is>
@@ -5967,7 +5967,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>4.473398992690782</v>
+        <v>1.498148520716465</v>
       </c>
       <c r="D213" t="inlineStr">
         <is>
@@ -5993,7 +5993,7 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>2.999221436975841</v>
+        <v>1.098352733978652</v>
       </c>
       <c r="D214" t="inlineStr">
         <is>
@@ -6019,7 +6019,7 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>3.589243092099721</v>
+        <v>1.277941342415531</v>
       </c>
       <c r="D215" t="inlineStr">
         <is>
@@ -6045,7 +6045,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>3.489041197247275</v>
+        <v>1.249626969887083</v>
       </c>
       <c r="D216" t="inlineStr">
         <is>
@@ -6071,7 +6071,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>3.788451271358973</v>
+        <v>1.33195730005475</v>
       </c>
       <c r="D217" t="inlineStr">
         <is>
@@ -6097,7 +6097,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>2.598197852716025</v>
+        <v>0.954818071128544</v>
       </c>
       <c r="D218" t="inlineStr">
         <is>
@@ -6123,7 +6123,7 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>2.61892145939897</v>
+        <v>0.962762576301168</v>
       </c>
       <c r="D219" t="inlineStr">
         <is>
@@ -6149,7 +6149,7 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>2.7017710835137</v>
+        <v>0.9939075148215456</v>
       </c>
       <c r="D220" t="inlineStr">
         <is>
@@ -6175,7 +6175,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4.991686905402128</v>
+        <v>1.607773909829784</v>
       </c>
       <c r="D221" t="inlineStr">
         <is>
@@ -6201,7 +6201,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4.223374605296272</v>
+        <v>1.440634477984104</v>
       </c>
       <c r="D222" t="inlineStr">
         <is>
@@ -6227,7 +6227,7 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>4.077997237262826</v>
+        <v>1.405605994678475</v>
       </c>
       <c r="D223" t="inlineStr">
         <is>
@@ -6253,7 +6253,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>3.489966244665095</v>
+        <v>1.249892064151829</v>
       </c>
       <c r="D224" t="inlineStr">
         <is>
@@ -6279,7 +6279,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>2.587400794206121</v>
+        <v>0.9506538174530438</v>
       </c>
       <c r="D225" t="inlineStr">
         <is>
@@ -6305,7 +6305,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>2.316893276006442</v>
+        <v>0.8402271831060203</v>
       </c>
       <c r="D226" t="inlineStr">
         <is>
@@ -6331,7 +6331,7 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>5.105452887390057</v>
+        <v>1.630309162155789</v>
       </c>
       <c r="D227" t="inlineStr">
         <is>
@@ -6357,7 +6357,7 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>4.699158818734517</v>
+        <v>1.547383517960787</v>
       </c>
       <c r="D228" t="inlineStr">
         <is>
@@ -6383,7 +6383,7 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>4.212958909348212</v>
+        <v>1.43816522964958</v>
       </c>
       <c r="D229" t="inlineStr">
         <is>
@@ -6409,7 +6409,7 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>6.03507902097005</v>
+        <v>1.797588948245056</v>
       </c>
       <c r="D230" t="inlineStr">
         <is>
@@ -6435,7 +6435,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>3.606573091120666</v>
+        <v>1.282758039253016</v>
       </c>
       <c r="D231" t="inlineStr">
         <is>
@@ -6461,7 +6461,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>4.152690296247315</v>
+        <v>1.423756388366145</v>
       </c>
       <c r="D232" t="inlineStr">
         <is>
@@ -6487,7 +6487,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>5.105172628305542</v>
+        <v>1.630254266579773</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -6513,7 +6513,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>2.987473977216064</v>
+        <v>1.0944282066644</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -6539,7 +6539,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>3.061177540496788</v>
+        <v>1.11879965909697</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -6565,7 +6565,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>5.093466093824063</v>
+        <v>1.627958560271938</v>
       </c>
       <c r="D236" t="inlineStr">
         <is>
@@ -6591,7 +6591,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>4.75503565695636</v>
+        <v>1.559204194803383</v>
       </c>
       <c r="D237" t="inlineStr">
         <is>
@@ -6617,7 +6617,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>2.649079173705837</v>
+        <v>0.9742120979919646</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
@@ -6643,7 +6643,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>2.898662233460566</v>
+        <v>1.0642493317547</v>
       </c>
       <c r="D239" t="inlineStr">
         <is>
@@ -6669,7 +6669,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2.615158638954221</v>
+        <v>0.9613247606688939</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>
@@ -6695,7 +6695,7 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>4.675997756300557</v>
+        <v>1.542442563776635</v>
       </c>
       <c r="D241" t="inlineStr">
         <is>
@@ -6721,7 +6721,7 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>5.023731097373726</v>
+        <v>1.61417290412154</v>
       </c>
       <c r="D242" t="inlineStr">
         <is>
@@ -6747,7 +6747,7 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>2.685318006345247</v>
+        <v>0.9877991590649984</v>
       </c>
       <c r="D243" t="inlineStr">
         <is>
@@ -6773,7 +6773,7 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>2.637777468960611</v>
+        <v>0.9699366947705483</v>
       </c>
       <c r="D244" t="inlineStr">
         <is>
@@ -6799,7 +6799,7 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>2.598021998617728</v>
+        <v>0.9547503857328542</v>
       </c>
       <c r="D245" t="inlineStr">
         <is>
@@ -6825,7 +6825,7 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>4.14769671091283</v>
+        <v>1.422553170749273</v>
       </c>
       <c r="D246" t="inlineStr">
         <is>
@@ -6851,7 +6851,7 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>3.259957067061348</v>
+        <v>1.181714025678813</v>
       </c>
       <c r="D247" t="inlineStr">
         <is>
@@ -6877,7 +6877,7 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>3.357419791724249</v>
+        <v>1.211172759844496</v>
       </c>
       <c r="D248" t="inlineStr">
         <is>
@@ -6903,7 +6903,7 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>3.005117202885903</v>
+        <v>1.100316569850849</v>
       </c>
       <c r="D249" t="inlineStr">
         <is>
@@ -6929,7 +6929,7 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>2.619051664843498</v>
+        <v>0.9628122922662813</v>
       </c>
       <c r="D250" t="inlineStr">
         <is>
@@ -6955,7 +6955,7 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>2.615087777896788</v>
+        <v>0.9612976640268662</v>
       </c>
       <c r="D251" t="inlineStr">
         <is>
@@ -6981,7 +6981,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>2.029798318117932</v>
+        <v>0.7079364374372685</v>
       </c>
       <c r="D252" t="inlineStr">
         <is>
@@ -7007,7 +7007,7 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>2.072556400942394</v>
+        <v>0.7287828216219867</v>
       </c>
       <c r="D253" t="inlineStr">
         <is>
@@ -7033,7 +7033,7 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>3.765588971135279</v>
+        <v>1.325904282253916</v>
       </c>
       <c r="D254" t="inlineStr">
         <is>
@@ -7059,7 +7059,7 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>1.50229230678545</v>
+        <v>0.4069921461155636</v>
       </c>
       <c r="D255" t="inlineStr">
         <is>
@@ -7085,7 +7085,7 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>3.345437850085732</v>
+        <v>1.207597581900558</v>
       </c>
       <c r="D256" t="inlineStr">
         <is>
@@ -7111,7 +7111,7 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4.222451998610048</v>
+        <v>1.440416001632845</v>
       </c>
       <c r="D257" t="inlineStr">
         <is>
@@ -7137,7 +7137,7 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>5.731231512833478</v>
+        <v>1.745930431339525</v>
       </c>
       <c r="D258" t="inlineStr">
         <is>
@@ -7163,7 +7163,7 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>2.909939165484229</v>
+        <v>1.068132175633002</v>
       </c>
       <c r="D259" t="inlineStr">
         <is>
@@ -7189,7 +7189,7 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>1.475441206519702</v>
+        <v>0.3889570681276036</v>
       </c>
       <c r="D260" t="inlineStr">
         <is>
@@ -7215,7 +7215,7 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>4.243044992770677</v>
+        <v>1.445281170163654</v>
       </c>
       <c r="D261" t="inlineStr">
         <is>
@@ -7241,7 +7241,7 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>4.567926160007067</v>
+        <v>1.51905930760114</v>
       </c>
       <c r="D262" t="inlineStr">
         <is>
@@ -7267,7 +7267,7 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>3.581904730235753</v>
+        <v>1.275894706477379</v>
       </c>
       <c r="D263" t="inlineStr">
         <is>
@@ -7293,7 +7293,7 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>2.329204471261485</v>
+        <v>0.8455267806344401</v>
       </c>
       <c r="D264" t="inlineStr">
         <is>
@@ -7319,7 +7319,7 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>4.687298480222417</v>
+        <v>1.54485639948651</v>
       </c>
       <c r="D265" t="inlineStr">
         <is>
@@ -7345,7 +7345,7 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>2.597937606260176</v>
+        <v>0.9547179018938803</v>
       </c>
       <c r="D266" t="inlineStr">
         <is>
@@ -7371,7 +7371,7 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>3.373292488816401</v>
+        <v>1.215889267059528</v>
       </c>
       <c r="D267" t="inlineStr">
         <is>
@@ -7397,7 +7397,7 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>5.189709780950952</v>
+        <v>1.646677776722361</v>
       </c>
       <c r="D268" t="inlineStr">
         <is>
@@ -7423,7 +7423,7 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>5.044609277642346</v>
+        <v>1.618320203361834</v>
       </c>
       <c r="D269" t="inlineStr">
         <is>
@@ -7449,7 +7449,7 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>4.666422165645612</v>
+        <v>1.540392646498643</v>
       </c>
       <c r="D270" t="inlineStr">
         <is>
@@ -7475,7 +7475,7 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>2.607301030886576</v>
+        <v>0.9583155985140274</v>
       </c>
       <c r="D271" t="inlineStr">
         <is>
@@ -7501,7 +7501,7 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>4.474507413279904</v>
+        <v>1.49839627042338</v>
       </c>
       <c r="D272" t="inlineStr">
         <is>
@@ -7527,7 +7527,7 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>3.008372529934013</v>
+        <v>1.1013992448069</v>
       </c>
       <c r="D273" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>2.59308152118116</v>
+        <v>0.9528469450060904</v>
       </c>
       <c r="D274" t="inlineStr">
         <is>
@@ -7579,7 +7579,7 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>2.607419718533259</v>
+        <v>0.9583611187450835</v>
       </c>
       <c r="D275" t="inlineStr">
         <is>
@@ -7605,7 +7605,7 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>2.353809873750596</v>
+        <v>0.8560352382655233</v>
       </c>
       <c r="D276" t="inlineStr">
         <is>
@@ -7631,7 +7631,7 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>2.592971615827593</v>
+        <v>0.9528045600359869</v>
       </c>
       <c r="D277" t="inlineStr">
         <is>
@@ -7657,7 +7657,7 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>4.797858860546123</v>
+        <v>1.568169747675148</v>
       </c>
       <c r="D278" t="inlineStr">
         <is>
@@ -7683,7 +7683,7 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>3.619159503783275</v>
+        <v>1.286241817604096</v>
       </c>
       <c r="D279" t="inlineStr">
         <is>
@@ -7709,7 +7709,7 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>1.994282930077837</v>
+        <v>0.6902845521851635</v>
       </c>
       <c r="D280" t="inlineStr">
         <is>
@@ -7735,7 +7735,7 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>3.89641894606736</v>
+        <v>1.360057912357251</v>
       </c>
       <c r="D281" t="inlineStr">
         <is>
@@ -7761,7 +7761,7 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>3.733091835598265</v>
+        <v>1.31723680064733</v>
       </c>
       <c r="D282" t="inlineStr">
         <is>
@@ -7787,7 +7787,7 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>1.498538147741945</v>
+        <v>0.4044900647357982</v>
       </c>
       <c r="D283" t="inlineStr">
         <is>
@@ -7813,7 +7813,7 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>2.872379882629405</v>
+        <v>1.055140913549443</v>
       </c>
       <c r="D284" t="inlineStr">
         <is>
@@ -7839,7 +7839,7 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>3.525981028549917</v>
+        <v>1.260158703515917</v>
       </c>
       <c r="D285" t="inlineStr">
         <is>
@@ -7865,7 +7865,7 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>2.932946609960803</v>
+        <v>1.076007586611359</v>
       </c>
       <c r="D286" t="inlineStr">
         <is>
@@ -7891,7 +7891,7 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>2.987473977216064</v>
+        <v>1.0944282066644</v>
       </c>
       <c r="D287" t="inlineStr">
         <is>
@@ -7917,7 +7917,7 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>3.789442118817522</v>
+        <v>1.332218810058435</v>
       </c>
       <c r="D288" t="inlineStr">
         <is>
@@ -7943,7 +7943,7 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>3.829327921147557</v>
+        <v>1.34268931028741</v>
       </c>
       <c r="D289" t="inlineStr">
         <is>
@@ -7969,7 +7969,7 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>4.24001178265268</v>
+        <v>1.444566048167524</v>
       </c>
       <c r="D290" t="inlineStr">
         <is>
@@ -7995,7 +7995,7 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>3.19129945316457</v>
+        <v>1.160428185940622</v>
       </c>
       <c r="D291" t="inlineStr">
         <is>
@@ -8021,7 +8021,7 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>4.698727592734974</v>
+        <v>1.547291747113393</v>
       </c>
       <c r="D292" t="inlineStr">
         <is>
@@ -8047,7 +8047,7 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>4.304732049075964</v>
+        <v>1.459714894148392</v>
       </c>
       <c r="D293" t="inlineStr">
         <is>
@@ -8073,7 +8073,7 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>2.353348970742586</v>
+        <v>0.8558394076064316</v>
       </c>
       <c r="D294" t="inlineStr">
         <is>
@@ -8099,7 +8099,7 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>2.301950804910139</v>
+        <v>0.8337569394849506</v>
       </c>
       <c r="D295" t="inlineStr">
         <is>
@@ -8125,7 +8125,7 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>2.923275993373967</v>
+        <v>1.072704902942303</v>
       </c>
       <c r="D296" t="inlineStr">
         <is>
@@ -8151,7 +8151,7 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>2.341547991209719</v>
+        <v>0.8508122453569895</v>
       </c>
       <c r="D297" t="inlineStr">
         <is>
@@ -8177,7 +8177,7 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>2.597900474718702</v>
+        <v>0.9547036090922589</v>
       </c>
       <c r="D298" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>2.709681893946517</v>
+        <v>0.996831245694209</v>
       </c>
       <c r="D299" t="inlineStr">
         <is>
@@ -8229,7 +8229,7 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>2.649346202104921</v>
+        <v>0.9743128933718636</v>
       </c>
       <c r="D300" t="inlineStr">
         <is>
@@ -8255,7 +8255,7 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>3.000901900879864</v>
+        <v>1.098912877113497</v>
       </c>
       <c r="D301" t="inlineStr">
         <is>
@@ -8281,7 +8281,7 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>3.696086647184092</v>
+        <v>1.307274597006832</v>
       </c>
       <c r="D302" t="inlineStr">
         <is>
@@ -8307,7 +8307,7 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>4.841171063756216</v>
+        <v>1.577156646783604</v>
       </c>
       <c r="D303" t="inlineStr">
         <is>
@@ -8333,7 +8333,7 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>3.378275524558605</v>
+        <v>1.217365379463974</v>
       </c>
       <c r="D304" t="inlineStr">
         <is>
@@ -8359,7 +8359,7 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>2.353657853820323</v>
+        <v>0.8559706515538882</v>
       </c>
       <c r="D305" t="inlineStr">
         <is>
@@ -8385,7 +8385,7 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>4.976850387520341</v>
+        <v>1.604797238649084</v>
       </c>
       <c r="D306" t="inlineStr">
         <is>
@@ -8411,7 +8411,7 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>3.529712361107113</v>
+        <v>1.261216383519562</v>
       </c>
       <c r="D307" t="inlineStr">
         <is>
@@ -8437,7 +8437,7 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>2.607589284131392</v>
+        <v>0.9584261485841903</v>
       </c>
       <c r="D308" t="inlineStr">
         <is>
@@ -8463,7 +8463,7 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>2.684850350036473</v>
+        <v>0.9876249908531581</v>
       </c>
       <c r="D309" t="inlineStr">
         <is>
@@ -8489,7 +8489,7 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>5.084911946218662</v>
+        <v>1.626277712972749</v>
       </c>
       <c r="D310" t="inlineStr">
         <is>
@@ -8515,7 +8515,7 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>4.216851561928433</v>
+        <v>1.439088774222774</v>
       </c>
       <c r="D311" t="inlineStr">
         <is>
@@ -8541,7 +8541,7 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>4.191213645559353</v>
+        <v>1.432990344870877</v>
       </c>
       <c r="D312" t="inlineStr">
         <is>
@@ -8567,7 +8567,7 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>3.617744372304838</v>
+        <v>1.285850730055967</v>
       </c>
       <c r="D313" t="inlineStr">
         <is>
@@ -8593,7 +8593,7 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>4.183419598532057</v>
+        <v>1.431128997860111</v>
       </c>
       <c r="D314" t="inlineStr">
         <is>
@@ -8619,7 +8619,7 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>3.611426388481375</v>
+        <v>1.284102815767845</v>
       </c>
       <c r="D315" t="inlineStr">
         <is>
@@ -8645,7 +8645,7 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>4.709545692842298</v>
+        <v>1.549591447504036</v>
       </c>
       <c r="D316" t="inlineStr">
         <is>
@@ -8671,7 +8671,7 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>4.718347457055737</v>
+        <v>1.551458623262323</v>
       </c>
       <c r="D317" t="inlineStr">
         <is>
@@ -8697,7 +8697,7 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>2.669327153651593</v>
+        <v>0.9818264382765428</v>
       </c>
       <c r="D318" t="inlineStr">
         <is>
@@ -8723,7 +8723,7 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>3.673652339166176</v>
+        <v>1.301186354979115</v>
       </c>
       <c r="D319" t="inlineStr">
         <is>
@@ -8749,7 +8749,7 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>2.656915977828922</v>
+        <v>0.9771660433303223</v>
       </c>
       <c r="D320" t="inlineStr">
         <is>
@@ -8775,7 +8775,7 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>3.700152629316733</v>
+        <v>1.308374069966058</v>
       </c>
       <c r="D321" t="inlineStr">
         <is>
@@ -8801,7 +8801,7 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>4.602681356571948</v>
+        <v>1.526639037275332</v>
       </c>
       <c r="D322" t="inlineStr">
         <is>
@@ -8827,7 +8827,7 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>5.145844930319424</v>
+        <v>1.63818957938286</v>
       </c>
       <c r="D323" t="inlineStr">
         <is>
@@ -8853,7 +8853,7 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>4.1521037293303</v>
+        <v>1.423615128530877</v>
       </c>
       <c r="D324" t="inlineStr">
         <is>
@@ -8879,7 +8879,7 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>4.211124661988829</v>
+        <v>1.437729752633513</v>
       </c>
       <c r="D325" t="inlineStr">
         <is>
@@ -8905,7 +8905,7 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>2.619042364184185</v>
+        <v>0.9628087411046331</v>
       </c>
       <c r="D326" t="inlineStr">
         <is>
@@ -8931,7 +8931,7 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>3.790568251817275</v>
+        <v>1.33251594237171</v>
       </c>
       <c r="D327" t="inlineStr">
         <is>
@@ -8957,7 +8957,7 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>3.143104182736366</v>
+        <v>1.145210904811836</v>
       </c>
       <c r="D328" t="inlineStr">
         <is>
@@ -8983,7 +8983,7 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>4.194363328026087</v>
+        <v>1.433741559158165</v>
       </c>
       <c r="D329" t="inlineStr">
         <is>
@@ -9009,7 +9009,7 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>3.560179968504188</v>
+        <v>1.269811096536796</v>
       </c>
       <c r="D330" t="inlineStr">
         <is>
@@ -9035,7 +9035,7 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>4.801890059915781</v>
+        <v>1.569009602892198</v>
       </c>
       <c r="D331" t="inlineStr">
         <is>
@@ -9061,7 +9061,7 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>2.712222045727824</v>
+        <v>0.9977682419949241</v>
       </c>
       <c r="D332" t="inlineStr">
         <is>
@@ -9087,7 +9087,7 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>3.354692289530363</v>
+        <v>1.210360049236868</v>
       </c>
       <c r="D333" t="inlineStr">
         <is>
@@ -9113,7 +9113,7 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>3.259957067061348</v>
+        <v>1.181714025678813</v>
       </c>
       <c r="D334" t="inlineStr">
         <is>
@@ -9139,7 +9139,7 @@
         </is>
       </c>
       <c r="C335" t="n">
-        <v>4.785278247418089</v>
+        <v>1.565544173144911</v>
       </c>
       <c r="D335" t="inlineStr">
         <is>
@@ -9165,7 +9165,7 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>3.19129945316457</v>
+        <v>1.160428185940622</v>
       </c>
       <c r="D336" t="inlineStr">
         <is>
@@ -9191,7 +9191,7 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>4.289591208288084</v>
+        <v>1.456191438956261</v>
       </c>
       <c r="D337" t="inlineStr">
         <is>
@@ -9217,7 +9217,7 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>2.628729154086114</v>
+        <v>0.9665005180313336</v>
       </c>
       <c r="D338" t="inlineStr">
         <is>
@@ -9243,7 +9243,7 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>3.573534744263261</v>
+        <v>1.273555230385146</v>
       </c>
       <c r="D339" t="inlineStr">
         <is>
@@ -9269,7 +9269,7 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>2.63753817892738</v>
+        <v>0.9698459741201202</v>
       </c>
       <c r="D340" t="inlineStr">
         <is>
@@ -9295,7 +9295,7 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>3.260722074542648</v>
+        <v>1.181948666110644</v>
       </c>
       <c r="D341" t="inlineStr">
         <is>
@@ -9321,7 +9321,7 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>5.2137769602022</v>
+        <v>1.651304537496651</v>
       </c>
       <c r="D342" t="inlineStr">
         <is>
@@ -9347,7 +9347,7 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>3.723947624448577</v>
+        <v>1.314784294989541</v>
       </c>
       <c r="D343" t="inlineStr">
         <is>
@@ -9373,7 +9373,7 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>3.19129945316457</v>
+        <v>1.160428185940622</v>
       </c>
       <c r="D344" t="inlineStr">
         <is>
@@ -9399,7 +9399,7 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>4.546226078801531</v>
+        <v>1.514297455562361</v>
       </c>
       <c r="D345" t="inlineStr">
         <is>
@@ -9425,7 +9425,7 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>3.899143001448363</v>
+        <v>1.360756785770154</v>
       </c>
       <c r="D346" t="inlineStr">
         <is>
@@ -9451,7 +9451,7 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>3.173976747321055</v>
+        <v>1.154985296091577</v>
       </c>
       <c r="D347" t="inlineStr">
         <is>
@@ -9477,7 +9477,7 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>2.653389409612415</v>
+        <v>0.9758378452408922</v>
       </c>
       <c r="D348" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>2.072378091385907</v>
+        <v>0.7286967842880184</v>
       </c>
       <c r="D349" t="inlineStr">
         <is>
@@ -9529,7 +9529,7 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>3.789442118817522</v>
+        <v>1.332218810058435</v>
       </c>
       <c r="D350" t="inlineStr">
         <is>
@@ -9555,7 +9555,7 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>2.629109176897537</v>
+        <v>0.966645072803908</v>
       </c>
       <c r="D351" t="inlineStr">
         <is>
@@ -9581,7 +9581,7 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>4.190055759554705</v>
+        <v>1.432714041615118</v>
       </c>
       <c r="D352" t="inlineStr">
         <is>
@@ -9607,7 +9607,7 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>2.107541645073434</v>
+        <v>0.7455221711130796</v>
       </c>
       <c r="D353" t="inlineStr">
         <is>
@@ -9633,7 +9633,7 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>2.696624532744212</v>
+        <v>0.9920008178343235</v>
       </c>
       <c r="D354" t="inlineStr">
         <is>
@@ -9659,7 +9659,7 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>4.63659928462664</v>
+        <v>1.533981184730295</v>
       </c>
       <c r="D355" t="inlineStr">
         <is>
@@ -9685,7 +9685,7 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>3.667114209647271</v>
+        <v>1.299405033858418</v>
       </c>
       <c r="D356" t="inlineStr">
         <is>
@@ -9711,7 +9711,7 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>4.777739287058305</v>
+        <v>1.563967482127793</v>
       </c>
       <c r="D357" t="inlineStr">
         <is>
@@ -9737,7 +9737,7 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>3.747473999710828</v>
+        <v>1.321082012934744</v>
       </c>
       <c r="D358" t="inlineStr">
         <is>
@@ -9763,7 +9763,7 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>3.178823753384848</v>
+        <v>1.156511239493633</v>
       </c>
       <c r="D359" t="inlineStr">
         <is>
@@ -9789,7 +9789,7 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>2.637688318502071</v>
+        <v>0.9699028966332314</v>
       </c>
       <c r="D360" t="inlineStr">
         <is>
@@ -9815,7 +9815,7 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>2.592769882864254</v>
+        <v>0.9527267570974906</v>
       </c>
       <c r="D361" t="inlineStr">
         <is>
@@ -9841,7 +9841,7 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>4.243105297341947</v>
+        <v>1.445295382632019</v>
       </c>
       <c r="D362" t="inlineStr">
         <is>
@@ -9867,7 +9867,7 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>5.127686509976563</v>
+        <v>1.634654584749781</v>
       </c>
       <c r="D363" t="inlineStr">
         <is>
@@ -9893,7 +9893,7 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>2.607503882992366</v>
+        <v>0.9583933970546216</v>
       </c>
       <c r="D364" t="inlineStr">
         <is>
@@ -9919,7 +9919,7 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>2.65136683754638</v>
+        <v>0.9750752947787003</v>
       </c>
       <c r="D365" t="inlineStr">
         <is>
@@ -9945,7 +9945,7 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>4.919149019091581</v>
+        <v>1.593135551945016</v>
       </c>
       <c r="D366" t="inlineStr">
         <is>
@@ -9971,7 +9971,7 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>3.322146918630371</v>
+        <v>1.200611236170531</v>
       </c>
       <c r="D367" t="inlineStr">
         <is>
@@ -9997,7 +9997,7 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>3.539839481957958</v>
+        <v>1.264081382037936</v>
       </c>
       <c r="D368" t="inlineStr">
         <is>
@@ -10023,7 +10023,7 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>2.978306895644174</v>
+        <v>1.09135498323153</v>
       </c>
       <c r="D369" t="inlineStr">
         <is>
@@ -10049,7 +10049,7 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>3.665743612123725</v>
+        <v>1.299031210289812</v>
       </c>
       <c r="D370" t="inlineStr">
         <is>
@@ -10075,7 +10075,7 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>4.118067016355094</v>
+        <v>1.415383882478786</v>
       </c>
       <c r="D371" t="inlineStr">
         <is>
@@ -10101,7 +10101,7 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>3.699102079670697</v>
+        <v>1.308090109028257</v>
       </c>
       <c r="D372" t="inlineStr">
         <is>
@@ -10127,7 +10127,7 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>3.591480943567036</v>
+        <v>1.278564636537029</v>
       </c>
       <c r="D373" t="inlineStr">
         <is>
@@ -10153,7 +10153,7 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>2.681421688483532</v>
+        <v>0.9863471346450161</v>
       </c>
       <c r="D374" t="inlineStr">
         <is>
@@ -10179,7 +10179,7 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>3.647309737840444</v>
+        <v>1.29398983770761</v>
       </c>
       <c r="D375" t="inlineStr">
         <is>
@@ -10205,7 +10205,7 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>3.484893938637397</v>
+        <v>1.248437610072873</v>
       </c>
       <c r="D376" t="inlineStr">
         <is>
@@ -10231,7 +10231,7 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>4.150523446997902</v>
+        <v>1.423234458095383</v>
       </c>
       <c r="D377" t="inlineStr">
         <is>
@@ -10257,7 +10257,7 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>3.609709899112628</v>
+        <v>1.28362740875911</v>
       </c>
       <c r="D378" t="inlineStr">
         <is>
@@ -10283,7 +10283,7 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>2.51932896833973</v>
+        <v>0.9239925836590082</v>
       </c>
       <c r="D379" t="inlineStr">
         <is>
@@ -10309,7 +10309,7 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>3.687056469011135</v>
+        <v>1.304828434841568</v>
       </c>
       <c r="D380" t="inlineStr">
         <is>
@@ -10335,7 +10335,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>2.754798200211547</v>
+        <v>1.013344191360019</v>
       </c>
       <c r="D381" t="inlineStr">
         <is>
@@ -10361,7 +10361,7 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>4.207269490689817</v>
+        <v>1.436813860243922</v>
       </c>
       <c r="D382" t="inlineStr">
         <is>
@@ -10387,7 +10387,7 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>3.656186155652314</v>
+        <v>1.296420570143641</v>
       </c>
       <c r="D383" t="inlineStr">
         <is>
@@ -10413,7 +10413,7 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>5.7080402945961</v>
+        <v>1.741875758909242</v>
       </c>
       <c r="D384" t="inlineStr">
         <is>
@@ -10439,7 +10439,7 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>2.642268354349291</v>
+        <v>0.971637773367928</v>
       </c>
       <c r="D385" t="inlineStr">
         <is>
@@ -10465,7 +10465,7 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>2.625921621524737</v>
+        <v>0.9654319283387267</v>
       </c>
       <c r="D386" t="inlineStr">
         <is>
@@ -10491,7 +10491,7 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>2.612348389659889</v>
+        <v>0.9602495829408978</v>
       </c>
       <c r="D387" t="inlineStr">
         <is>
@@ -10517,7 +10517,7 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>3.064426739748488</v>
+        <v>1.119860517555263</v>
       </c>
       <c r="D388" t="inlineStr">
         <is>
@@ -10543,7 +10543,7 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>5.496239384526737</v>
+        <v>1.704064110108104</v>
       </c>
       <c r="D389" t="inlineStr">
         <is>
@@ -10569,7 +10569,7 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>3.782213212681263</v>
+        <v>1.33030934429007</v>
       </c>
       <c r="D390" t="inlineStr">
         <is>
@@ -10595,7 +10595,7 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>1.959464718904604</v>
+        <v>0.6726713333434279</v>
       </c>
       <c r="D391" t="inlineStr">
         <is>
@@ -10621,7 +10621,7 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>3.275787769942471</v>
+        <v>1.186558380602451</v>
       </c>
       <c r="D392" t="inlineStr">
         <is>
@@ -10647,7 +10647,7 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>3.745783097423464</v>
+        <v>1.320630699895796</v>
       </c>
       <c r="D393" t="inlineStr">
         <is>
@@ -10673,7 +10673,7 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>1.489640934318389</v>
+        <v>0.3985351072372018</v>
       </c>
       <c r="D394" t="inlineStr">
         <is>
@@ -10699,7 +10699,7 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>4.217839449628165</v>
+        <v>1.439323018180946</v>
       </c>
       <c r="D395" t="inlineStr">
         <is>
@@ -10725,7 +10725,7 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>5.72418491917407</v>
+        <v>1.744700167107751</v>
       </c>
       <c r="D396" t="inlineStr">
         <is>
@@ -10751,7 +10751,7 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>4.186692748535647</v>
+        <v>1.431911102098314</v>
       </c>
       <c r="D397" t="inlineStr">
         <is>
@@ -10777,7 +10777,7 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>4.976395698067938</v>
+        <v>1.60470587359113</v>
       </c>
       <c r="D398" t="inlineStr">
         <is>
@@ -10803,7 +10803,7 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>3.191621482712807</v>
+        <v>1.160529089446007</v>
       </c>
       <c r="D399" t="inlineStr">
         <is>
@@ -10829,7 +10829,7 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>4.033826463265554</v>
+        <v>1.394715420080557</v>
       </c>
       <c r="D400" t="inlineStr">
         <is>
@@ -10855,7 +10855,7 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>3.587098175457623</v>
+        <v>1.277343567971424</v>
       </c>
       <c r="D401" t="inlineStr">
         <is>
@@ -10881,7 +10881,7 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>3.691574849072623</v>
+        <v>1.30605315537075</v>
       </c>
       <c r="D402" t="inlineStr">
         <is>
@@ -10907,7 +10907,7 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>2.957114670953328</v>
+        <v>1.084214019608908</v>
       </c>
       <c r="D403" t="inlineStr">
         <is>
@@ -10933,7 +10933,7 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>2.61920792214071</v>
+        <v>0.962871952271542</v>
       </c>
       <c r="D404" t="inlineStr">
         <is>
@@ -10959,7 +10959,7 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>3.040868532010132</v>
+        <v>1.112143175932403</v>
       </c>
       <c r="D405" t="inlineStr">
         <is>
@@ -10985,7 +10985,7 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>4.01113190648849</v>
+        <v>1.389073472432291</v>
       </c>
       <c r="D406" t="inlineStr">
         <is>
@@ -11011,7 +11011,7 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>5.449116443412637</v>
+        <v>1.695453475057463</v>
       </c>
       <c r="D407" t="inlineStr">
         <is>
@@ -11037,7 +11037,7 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>4.760722134328216</v>
+        <v>1.560399365629181</v>
       </c>
       <c r="D408" t="inlineStr">
         <is>
@@ -11063,7 +11063,7 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>4.278357092242738</v>
+        <v>1.453569078949135</v>
       </c>
       <c r="D409" t="inlineStr">
         <is>
@@ -11089,7 +11089,7 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>3.714366498943337</v>
+        <v>1.312208138445161</v>
       </c>
       <c r="D410" t="inlineStr">
         <is>
@@ -11115,7 +11115,7 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>3.986543157596581</v>
+        <v>1.382924478838495</v>
       </c>
       <c r="D411" t="inlineStr">
         <is>
@@ -11141,7 +11141,7 @@
         </is>
       </c>
       <c r="C412" t="n">
-        <v>5.816702929535777</v>
+        <v>1.760733594265038</v>
       </c>
       <c r="D412" t="inlineStr">
         <is>
@@ -11167,7 +11167,7 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>4.15250956092703</v>
+        <v>1.423712864953482</v>
       </c>
       <c r="D413" t="inlineStr">
         <is>
@@ -11193,7 +11193,7 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>2.588253339336453</v>
+        <v>0.9509832618540974</v>
       </c>
       <c r="D414" t="inlineStr">
         <is>
@@ -11219,7 +11219,7 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>4.90829423878745</v>
+        <v>1.590926475904873</v>
       </c>
       <c r="D415" t="inlineStr">
         <is>
@@ -11245,7 +11245,7 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>3.315925813760587</v>
+        <v>1.198736864815485</v>
       </c>
       <c r="D416" t="inlineStr">
         <is>
@@ -11271,7 +11271,7 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>3.418523380873872</v>
+        <v>1.229208697860937</v>
       </c>
       <c r="D417" t="inlineStr">
         <is>
@@ -11297,7 +11297,7 @@
         </is>
       </c>
       <c r="C418" t="n">
-        <v>4.478650439101072</v>
+        <v>1.499321759772545</v>
       </c>
       <c r="D418" t="inlineStr">
         <is>
@@ -11323,7 +11323,7 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>4.428815689971398</v>
+        <v>1.488132209708801</v>
       </c>
       <c r="D419" t="inlineStr">
         <is>
@@ -11349,7 +11349,7 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>5.461462846884182</v>
+        <v>1.697716674547238</v>
       </c>
       <c r="D420" t="inlineStr">
         <is>
@@ -11375,7 +11375,7 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>2.988458590657185</v>
+        <v>1.094757732956354</v>
       </c>
       <c r="D421" t="inlineStr">
         <is>
@@ -11401,7 +11401,7 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>3.419440696634741</v>
+        <v>1.229476998704864</v>
       </c>
       <c r="D422" t="inlineStr">
         <is>
@@ -11427,7 +11427,7 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>3.706878977886729</v>
+        <v>1.310190276720844</v>
       </c>
       <c r="D423" t="inlineStr">
         <is>
@@ -11453,7 +11453,7 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>3.65132773309605</v>
+        <v>1.295090863940934</v>
       </c>
       <c r="D424" t="inlineStr">
         <is>
@@ -11479,7 +11479,7 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>3.28008194653524</v>
+        <v>1.187868405783733</v>
       </c>
       <c r="D425" t="inlineStr">
         <is>
@@ -11505,7 +11505,7 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>4.1878690715375</v>
+        <v>1.43219202975396</v>
       </c>
       <c r="D426" t="inlineStr">
         <is>
@@ -11531,7 +11531,7 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>3.615033277145613</v>
+        <v>1.285101060864518</v>
       </c>
       <c r="D427" t="inlineStr">
         <is>
@@ -11557,7 +11557,7 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>3.793652524305171</v>
+        <v>1.333329281737471</v>
       </c>
       <c r="D428" t="inlineStr">
         <is>
@@ -11583,7 +11583,7 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>2.906009270826026</v>
+        <v>1.066780755379075</v>
       </c>
       <c r="D429" t="inlineStr">
         <is>
@@ -11609,7 +11609,7 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>2.898662233460566</v>
+        <v>1.0642493317547</v>
       </c>
       <c r="D430" t="inlineStr">
         <is>
@@ -11635,7 +11635,7 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>2.898662233460566</v>
+        <v>1.0642493317547</v>
       </c>
       <c r="D431" t="inlineStr">
         <is>
@@ -11661,7 +11661,7 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>3.745783097423464</v>
+        <v>1.320630699895796</v>
       </c>
       <c r="D432" t="inlineStr">
         <is>
@@ -11687,7 +11687,7 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>3.984730516998706</v>
+        <v>1.382469685613945</v>
       </c>
       <c r="D433" t="inlineStr">
         <is>
@@ -11713,7 +11713,7 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>3.28694791666735</v>
+        <v>1.189959449307792</v>
       </c>
       <c r="D434" t="inlineStr">
         <is>
@@ -11739,7 +11739,7 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>3.10017503036091</v>
+        <v>1.131458571303961</v>
       </c>
       <c r="D435" t="inlineStr">
         <is>
@@ -11765,7 +11765,7 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>3.782523654973498</v>
+        <v>1.330391420454209</v>
       </c>
       <c r="D436" t="inlineStr">
         <is>
@@ -11791,7 +11791,7 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>3.320232107623856</v>
+        <v>1.200034692419568</v>
       </c>
       <c r="D437" t="inlineStr">
         <is>
@@ -11817,7 +11817,7 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>4.907112878241309</v>
+        <v>1.590685760356805</v>
       </c>
       <c r="D438" t="inlineStr">
         <is>
@@ -11843,7 +11843,7 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>3.692408688167432</v>
+        <v>1.306279006117613</v>
       </c>
       <c r="D439" t="inlineStr">
         <is>
@@ -11869,7 +11869,7 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>3.315248647305011</v>
+        <v>1.198532627553472</v>
       </c>
       <c r="D440" t="inlineStr">
         <is>
@@ -11895,7 +11895,7 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>3.417815575381814</v>
+        <v>1.229001626356988</v>
       </c>
       <c r="D441" t="inlineStr">
         <is>
@@ -11921,7 +11921,7 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>3.568478059376749</v>
+        <v>1.272139190993872</v>
       </c>
       <c r="D442" t="inlineStr">
         <is>
@@ -11947,7 +11947,7 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>3.209114412476056</v>
+        <v>1.165995015115098</v>
       </c>
       <c r="D443" t="inlineStr">
         <is>
@@ -11973,7 +11973,7 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>4.915412845808926</v>
+        <v>1.592375747184271</v>
       </c>
       <c r="D444" t="inlineStr">
         <is>
@@ -11999,7 +11999,7 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>3.422788037429468</v>
+        <v>1.23045543458939</v>
       </c>
       <c r="D445" t="inlineStr">
         <is>
@@ -12025,7 +12025,7 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>3.355555361901345</v>
+        <v>1.210617289333083</v>
       </c>
       <c r="D446" t="inlineStr">
         <is>
@@ -12051,7 +12051,7 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>4.178562289578681</v>
+        <v>1.429967237510785</v>
       </c>
       <c r="D447" t="inlineStr">
         <is>
@@ -12077,7 +12077,7 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>5.664214632750511</v>
+        <v>1.734168249873754</v>
       </c>
       <c r="D448" t="inlineStr">
         <is>
@@ -12103,7 +12103,7 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>3.497055246625211</v>
+        <v>1.2519212562479</v>
       </c>
       <c r="D449" t="inlineStr">
         <is>
@@ -12129,7 +12129,7 @@
         </is>
       </c>
       <c r="C450" t="n">
-        <v>2.660134845113467</v>
+        <v>0.9783768151604073</v>
       </c>
       <c r="D450" t="inlineStr">
         <is>
@@ -12155,7 +12155,7 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>3.319025238978161</v>
+        <v>1.19967113710126</v>
       </c>
       <c r="D451" t="inlineStr">
         <is>
@@ -12181,7 +12181,7 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>3.059198700107313</v>
+        <v>1.118153018962235</v>
       </c>
       <c r="D452" t="inlineStr">
         <is>
@@ -12207,7 +12207,7 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>3.667253000538098</v>
+        <v>1.299442880583805</v>
       </c>
       <c r="D453" t="inlineStr">
         <is>
@@ -12233,7 +12233,7 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>3.094624939022055</v>
+        <v>1.129666715924843</v>
       </c>
       <c r="D454" t="inlineStr">
         <is>
@@ -12259,7 +12259,7 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>2.937340330078739</v>
+        <v>1.077504522275076</v>
       </c>
       <c r="D455" t="inlineStr">
         <is>
@@ -12285,7 +12285,7 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D456" t="inlineStr">
         <is>
@@ -12311,7 +12311,7 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>5.495384366225682</v>
+        <v>1.703908533767034</v>
       </c>
       <c r="D457" t="inlineStr">
         <is>
@@ -12337,7 +12337,7 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>3.762643495828875</v>
+        <v>1.325121767774022</v>
       </c>
       <c r="D458" t="inlineStr">
         <is>
@@ -12363,7 +12363,7 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>3.585295489166757</v>
+        <v>1.27684089441135</v>
       </c>
       <c r="D459" t="inlineStr">
         <is>
@@ -12389,7 +12389,7 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>2.592843349327829</v>
+        <v>0.9527550918229281</v>
       </c>
       <c r="D460" t="inlineStr">
         <is>
@@ -12415,7 +12415,7 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>3.530453384461424</v>
+        <v>1.261426300222295</v>
       </c>
       <c r="D461" t="inlineStr">
         <is>
@@ -12441,7 +12441,7 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>2.634616977465053</v>
+        <v>0.9687378118317904</v>
       </c>
       <c r="D462" t="inlineStr">
         <is>
@@ -12467,7 +12467,7 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>4.303014010611655</v>
+        <v>1.459315709861307</v>
       </c>
       <c r="D463" t="inlineStr">
         <is>
@@ -12493,7 +12493,7 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>5.413751931676683</v>
+        <v>1.688942370355998</v>
       </c>
       <c r="D464" t="inlineStr">
         <is>
@@ -12519,7 +12519,7 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>3.143104182736366</v>
+        <v>1.145210904811836</v>
       </c>
       <c r="D465" t="inlineStr">
         <is>
@@ -12545,7 +12545,7 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>3.489780640629311</v>
+        <v>1.249838880551083</v>
       </c>
       <c r="D466" t="inlineStr">
         <is>
@@ -12571,7 +12571,7 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>4.531534744602277</v>
+        <v>1.511060677834575</v>
       </c>
       <c r="D467" t="inlineStr">
         <is>
@@ -12597,7 +12597,7 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>3.040659224824976</v>
+        <v>1.112074342180883</v>
       </c>
       <c r="D468" t="inlineStr">
         <is>
@@ -12623,7 +12623,7 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>2.787005971448859</v>
+        <v>1.024967891105646</v>
       </c>
       <c r="D469" t="inlineStr">
         <is>
@@ -12649,7 +12649,7 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>2.597611730791097</v>
+        <v>0.9545924578076573</v>
       </c>
       <c r="D470" t="inlineStr">
         <is>
@@ -12675,7 +12675,7 @@
         </is>
       </c>
       <c r="C471" t="n">
-        <v>3.127901702338698</v>
+        <v>1.14036239710575</v>
       </c>
       <c r="D471" t="inlineStr">
         <is>
@@ -12701,7 +12701,7 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>2.658885305344494</v>
+        <v>0.9779069768230394</v>
       </c>
       <c r="D472" t="inlineStr">
         <is>
@@ -12727,7 +12727,7 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>1.513141978705477</v>
+        <v>0.4141882696008717</v>
       </c>
       <c r="D473" t="inlineStr">
         <is>
@@ -12753,7 +12753,7 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>3.547770459333335</v>
+        <v>1.266319366563414</v>
       </c>
       <c r="D474" t="inlineStr">
         <is>
@@ -12779,7 +12779,7 @@
         </is>
       </c>
       <c r="C475" t="n">
-        <v>3.585750336215074</v>
+        <v>1.276967750956407</v>
       </c>
       <c r="D475" t="inlineStr">
         <is>
@@ -12805,7 +12805,7 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>3.023014906931659</v>
+        <v>1.106254646956734</v>
       </c>
       <c r="D476" t="inlineStr">
         <is>
@@ -12831,7 +12831,7 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>5.427244427383135</v>
+        <v>1.691431533201574</v>
       </c>
       <c r="D477" t="inlineStr">
         <is>
@@ -12857,7 +12857,7 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>4.742570660268941</v>
+        <v>1.556579322087454</v>
       </c>
       <c r="D478" t="inlineStr">
         <is>
@@ -12883,7 +12883,7 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>3.657267801888358</v>
+        <v>1.296716366425455</v>
       </c>
       <c r="D479" t="inlineStr">
         <is>
@@ -12909,7 +12909,7 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>5.981015164616304</v>
+        <v>1.788590313524229</v>
       </c>
       <c r="D480" t="inlineStr">
         <is>
@@ -12935,7 +12935,7 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>5.174168382440834</v>
+        <v>1.643678627192708</v>
       </c>
       <c r="D481" t="inlineStr">
         <is>

</xml_diff>